<commit_message>
só ajeitei detalhe de visualização
</commit_message>
<xml_diff>
--- a/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
+++ b/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\UFES\Outros\IC\Github\Instel-I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\GitHub\Instel-I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1EEE08-9B79-48C2-B21E-C183FF7350B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E666C4F6-4E9E-47A0-86A4-B4AE047936A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -821,11 +821,200 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -955,6 +1144,39 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -967,50 +1189,31 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1061,30 +1264,73 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1318,14 +1564,14 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="62"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1348,14 +1594,14 @@
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1406,16 +1652,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="64" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="55"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1438,17 +1684,17 @@
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="55"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="55"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1474,17 +1720,17 @@
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="55"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="55"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="30" t="s">
         <v>61</v>
       </c>
@@ -1510,17 +1756,17 @@
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="55"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="30" t="s">
         <v>62</v>
       </c>
@@ -1546,15 +1792,15 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4"/>
@@ -1578,15 +1824,15 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="48"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="4"/>
@@ -1610,15 +1856,15 @@
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="52" t="s">
+      <c r="C10" s="50"/>
+      <c r="D10" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="48"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="4"/>
@@ -1642,11 +1888,11 @@
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="4"/>
@@ -1670,11 +1916,11 @@
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1698,11 +1944,11 @@
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
       <c r="G13" s="32"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1726,11 +1972,11 @@
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="59"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="33"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1810,14 +2056,14 @@
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1840,14 +2086,14 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1870,14 +2116,14 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1900,14 +2146,14 @@
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1930,14 +2176,14 @@
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -29428,6 +29674,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -29440,23 +29703,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -29467,8 +29713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:L31"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -29510,19 +29756,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="49"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -29540,17 +29786,17 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="51"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="65"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -29568,27 +29814,27 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="91" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="92" t="s">
+      <c r="F4" s="59"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="92" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="55"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -29606,7 +29852,7 @@
     </row>
     <row r="5" spans="1:26" ht="39.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
@@ -29754,35 +30000,35 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="86">
+      <c r="C8" s="92">
         <v>17.579999999999998</v>
       </c>
-      <c r="D8" s="86">
+      <c r="D8" s="92">
         <v>23.9</v>
       </c>
-      <c r="E8" s="82">
+      <c r="E8" s="88">
         <v>3</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="88">
         <v>100</v>
       </c>
-      <c r="G8" s="84">
+      <c r="G8" s="90">
         <v>300</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="83">
         <v>4</v>
       </c>
-      <c r="I8" s="79" t="s">
+      <c r="I8" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="81">
+      <c r="J8" s="87">
         <v>1400</v>
       </c>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -29800,17 +30046,17 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -30419,9 +30665,9 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -30467,11 +30713,11 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -30501,11 +30747,11 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="J25" s="70" t="s">
+      <c r="J25" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="70"/>
-      <c r="L25" s="70"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -30531,11 +30777,11 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="68" t="s">
+      <c r="J26" s="94" t="s">
         <v>75</v>
       </c>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -30561,11 +30807,11 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="68" t="s">
+      <c r="J27" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -30591,11 +30837,11 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="69" t="s">
+      <c r="J28" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="95"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -30621,11 +30867,11 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="69" t="s">
+      <c r="J29" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="95"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -30651,11 +30897,11 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="67" t="s">
+      <c r="J30" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="K30" s="67"/>
-      <c r="L30" s="67"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="93"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -30681,11 +30927,11 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="67" t="s">
+      <c r="J31" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -30711,11 +30957,11 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="94" t="s">
+      <c r="J32" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="K32" s="94"/>
-      <c r="L32" s="94"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -30741,9 +30987,9 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -30769,9 +31015,9 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="94"/>
-      <c r="L34" s="94"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="69"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -57725,6 +57971,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="J32:L34"/>
     <mergeCell ref="B2:L3"/>
     <mergeCell ref="B4:B5"/>
@@ -57741,17 +57998,6 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J29:L29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -57763,7 +58009,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -57775,26 +58021,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1"/>
-    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1"/>
+    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="102" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93" t="s">
+      <c r="D3" s="103"/>
+      <c r="E3" s="102" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="93"/>
-      <c r="G3" s="27" t="s">
+      <c r="F3" s="103"/>
+      <c r="G3" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="100" t="s">
         <v>72</v>
       </c>
       <c r="I3" s="27" t="s">
@@ -57805,24 +58051,24 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="27" t="s">
+      <c r="A4" s="96"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="100" t="s">
         <v>66</v>
       </c>
       <c r="I4" s="27" t="s">
@@ -57836,26 +58082,26 @@
       <c r="A5" s="44">
         <v>1</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="106">
         <v>8</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="107">
         <v>4</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44">
+      <c r="E5" s="106"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="101">
         <f t="shared" ref="H5:H10" si="0">(C5*100+D5*200)+(E5*100+F5*600)+G5</f>
         <v>1600</v>
       </c>
       <c r="I5" s="44">
         <v>127</v>
       </c>
-      <c r="J5" s="95">
+      <c r="J5" s="45">
         <f t="shared" ref="J5:J13" si="1">H5/I5</f>
         <v>12.598425196850394</v>
       </c>
@@ -57864,24 +58110,24 @@
       <c r="A6" s="44">
         <v>2</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="106">
         <v>13</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44">
+      <c r="D6" s="107"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="101">
         <f t="shared" si="0"/>
         <v>1300</v>
       </c>
       <c r="I6" s="44">
         <v>127</v>
       </c>
-      <c r="J6" s="95">
+      <c r="J6" s="45">
         <f t="shared" si="1"/>
         <v>10.236220472440944</v>
       </c>
@@ -57890,26 +58136,26 @@
       <c r="A7" s="44">
         <v>3</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44">
+      <c r="C7" s="106"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="106">
         <v>3</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="107">
         <v>3</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44">
+      <c r="G7" s="112"/>
+      <c r="H7" s="101">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
       <c r="I7" s="44">
         <v>127</v>
       </c>
-      <c r="J7" s="95">
+      <c r="J7" s="45">
         <f t="shared" si="1"/>
         <v>16.535433070866141</v>
       </c>
@@ -57918,26 +58164,26 @@
       <c r="A8" s="44">
         <v>4</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44">
+      <c r="C8" s="106"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="106">
         <v>1</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="107">
         <v>3</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44">
+      <c r="G8" s="112"/>
+      <c r="H8" s="101">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
       <c r="I8" s="44">
         <v>127</v>
       </c>
-      <c r="J8" s="95">
+      <c r="J8" s="45">
         <f t="shared" si="1"/>
         <v>14.960629921259843</v>
       </c>
@@ -57946,26 +58192,26 @@
       <c r="A9" s="44">
         <v>5</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44">
+      <c r="C9" s="106"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="106">
         <v>2</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="107">
         <v>3</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44">
+      <c r="G9" s="112"/>
+      <c r="H9" s="101">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="I9" s="44">
         <v>127</v>
       </c>
-      <c r="J9" s="95">
+      <c r="J9" s="45">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
@@ -57974,26 +58220,26 @@
       <c r="A10" s="44">
         <v>6</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44">
+      <c r="C10" s="106"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="106">
         <v>1</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="107">
         <v>4</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44">
+      <c r="G10" s="112"/>
+      <c r="H10" s="101">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="I10" s="44">
         <v>127</v>
       </c>
-      <c r="J10" s="95">
+      <c r="J10" s="45">
         <f t="shared" si="1"/>
         <v>19.685039370078741</v>
       </c>
@@ -58002,26 +58248,26 @@
       <c r="A11" s="44">
         <v>7</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44">
+      <c r="C11" s="106"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="106">
         <v>2</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="107">
         <v>3</v>
       </c>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44">
+      <c r="G11" s="112"/>
+      <c r="H11" s="101">
         <f>(C11*100+D11*200)+(E11*100+F11*600)+G11</f>
         <v>2000</v>
       </c>
       <c r="I11" s="44">
         <v>127</v>
       </c>
-      <c r="J11" s="95">
+      <c r="J11" s="45">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
@@ -58030,26 +58276,26 @@
       <c r="A12" s="44">
         <v>8</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44">
+      <c r="C12" s="106"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="106">
         <v>2</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="107">
         <v>3</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44">
+      <c r="G12" s="112"/>
+      <c r="H12" s="101">
         <f>(C12*100+D12*200)+(E12*100+F12*600)+G12</f>
         <v>2000</v>
       </c>
       <c r="I12" s="44">
         <v>127</v>
       </c>
-      <c r="J12" s="95">
+      <c r="J12" s="45">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
@@ -58058,26 +58304,26 @@
       <c r="A13" s="44">
         <v>9</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44">
+      <c r="C13" s="106"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="106">
         <v>2</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="107">
         <v>3</v>
       </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44">
+      <c r="G13" s="112"/>
+      <c r="H13" s="101">
         <f>(C13*100+D13*200)+(E13*100+F13*600)+G13</f>
         <v>2000</v>
       </c>
       <c r="I13" s="44">
         <v>127</v>
       </c>
-      <c r="J13" s="95">
+      <c r="J13" s="45">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
@@ -58086,24 +58332,24 @@
       <c r="A14" s="44">
         <v>10</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44">
+      <c r="C14" s="106"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="112">
         <v>5400</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="101">
         <f>(C14*100+D14*200)+(E14*100+F14*600)+G14</f>
         <v>5400</v>
       </c>
       <c r="I14" s="44">
         <v>220</v>
       </c>
-      <c r="J14" s="95">
+      <c r="J14" s="45">
         <f>H14/I14</f>
         <v>24.545454545454547</v>
       </c>
@@ -58112,24 +58358,24 @@
       <c r="A15" s="44">
         <v>11</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44">
+      <c r="C15" s="106"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="112">
         <v>5400</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="101">
         <f t="shared" ref="H15:H20" si="2">(C15*100+D15*200)+(E15*100+F15*600)+G15</f>
         <v>5400</v>
       </c>
       <c r="I15" s="44">
         <v>220</v>
       </c>
-      <c r="J15" s="95">
+      <c r="J15" s="45">
         <f>H15/I15</f>
         <v>24.545454545454547</v>
       </c>
@@ -58138,24 +58384,24 @@
       <c r="A16" s="44">
         <v>12</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44">
+      <c r="C16" s="106"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="112">
         <v>2625</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="101">
         <f t="shared" si="2"/>
         <v>2625</v>
       </c>
       <c r="I16" s="44">
         <v>220</v>
       </c>
-      <c r="J16" s="95">
+      <c r="J16" s="45">
         <f>H16/I16</f>
         <v>11.931818181818182</v>
       </c>
@@ -58164,24 +58410,24 @@
       <c r="A17" s="44">
         <v>13</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44">
+      <c r="C17" s="106"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="112">
         <v>1650</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="101">
         <f t="shared" si="2"/>
         <v>1650</v>
       </c>
       <c r="I17" s="44">
         <v>220</v>
       </c>
-      <c r="J17" s="95">
+      <c r="J17" s="45">
         <f t="shared" ref="J17:J20" si="3">H17/I17</f>
         <v>7.5</v>
       </c>
@@ -58190,24 +58436,24 @@
       <c r="A18" s="44">
         <v>14</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44">
+      <c r="C18" s="106"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="107"/>
+      <c r="G18" s="112">
         <v>1650</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="101">
         <f t="shared" si="2"/>
         <v>1650</v>
       </c>
       <c r="I18" s="44">
         <v>220</v>
       </c>
-      <c r="J18" s="95">
+      <c r="J18" s="45">
         <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
@@ -58216,24 +58462,24 @@
       <c r="A19" s="44">
         <v>15</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="14">
+      <c r="C19" s="106"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="113">
         <v>246</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="101">
         <f t="shared" si="2"/>
         <v>246</v>
       </c>
       <c r="I19" s="44">
         <v>127</v>
       </c>
-      <c r="J19" s="95">
+      <c r="J19" s="45">
         <f t="shared" si="3"/>
         <v>1.9370078740157479</v>
       </c>
@@ -58242,54 +58488,54 @@
       <c r="A20" s="44">
         <v>16</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="19">
+      <c r="C20" s="106"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="114">
         <v>1760</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="101">
         <f t="shared" si="2"/>
         <v>1760</v>
       </c>
       <c r="I20" s="44">
         <v>220</v>
       </c>
-      <c r="J20" s="95">
+      <c r="J20" s="45">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27">
+      <c r="B21" s="98"/>
+      <c r="C21" s="108">
         <f t="shared" ref="C21:J21" si="4">SUM(C5:C20)</f>
         <v>21</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="109">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="108">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="109">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="115">
         <f t="shared" si="4"/>
         <v>18731</v>
       </c>
-      <c r="H21" s="27">
+      <c r="H21" s="100">
         <f t="shared" si="4"/>
         <v>36131</v>
       </c>
@@ -58297,7 +58543,7 @@
         <f t="shared" si="4"/>
         <v>2590</v>
       </c>
-      <c r="J21" s="96">
+      <c r="J21" s="46">
         <f t="shared" si="4"/>
         <v>222.96760916249107</v>
       </c>

</xml_diff>

<commit_message>
identificado área de lazer
- identificado que área de lazer será tampada.

- falta por lâmpadas na área de lazer e tomadas.

- e diminuir o tamanho das lâmpadas.
</commit_message>
<xml_diff>
--- a/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
+++ b/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\GitHub\Instel I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29ADA5D-3FAA-43F4-86E0-A59559F32964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CEAE79-E1B4-451E-9548-FF590755C88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação_Informações" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>Alunos: Gabriel Schettino Lucas e Ramon Rodrigues Morello</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Suíte</t>
   </si>
   <si>
-    <t>DESTACADO DE VERMELHO = DÚVIDA! TÁ CERTO?</t>
-  </si>
-  <si>
     <t>3:600 e 3:100</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>2:600 e 2:100</t>
   </si>
   <si>
     <t>Potência (VA)*</t>
@@ -301,27 +295,6 @@
     <t>CORRENTE</t>
   </si>
   <si>
-    <t>acho que ta certo, pela norma, a gnt vai ter: https://neoipsum.com.br/previsao-de-cargas-de-iluminacao-de-acordo-com-a-nbr-5410/</t>
-  </si>
-  <si>
-    <t>(6m2 = 100VA )+ (11,58m2 / 4) = 2,895 arredondado pra 3 x 60VA = 280 VA no total, arredondado pra 3 pontos com 100VA cada</t>
-  </si>
-  <si>
-    <t>Seguindo o mesmo caso da de cima, temos:</t>
-  </si>
-  <si>
-    <t>30,23m2 - 6m2 = 24,23m2, dividido por 4 = 6 aproximadamente, então no final: (100 + (6 x 60)) = 460 (será q da pra arredondar pra 500??)</t>
-  </si>
-  <si>
-    <t>Esse aqui eu acho q deveriam ser 5, tirando daqui: https://neoipsum.com.br/numero-minimo-de-tomadas-nbr-5410-projetos-eletricos-residenciais/</t>
-  </si>
-  <si>
-    <t>no caso o perimetro é 23,9, dividido por 5 = 4,78 e arredondando pra cima, 5 tomadas</t>
-  </si>
-  <si>
-    <t>Pelo que eu vi a norma define apenas 1 TUG(mínimo) para garagem, varanda, hall e corredor</t>
-  </si>
-  <si>
     <t>DESCRIÇÃO</t>
   </si>
   <si>
@@ -391,12 +364,6 @@
     </r>
   </si>
   <si>
-    <t>✔</t>
-  </si>
-  <si>
-    <t>arredondar é instrução do professor</t>
-  </si>
-  <si>
     <t>Os valores de potência total foram arredondados para o próximo valor multiplo de 100.</t>
   </si>
   <si>
@@ -424,6 +391,9 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Área de lazer e corredor frontal, será considerado com área tampada.</t>
   </si>
 </sst>
 </file>
@@ -548,7 +518,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,37 +545,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1196,10 +1136,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1223,46 +1163,31 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1271,16 +1196,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1292,36 +1217,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1334,36 +1269,44 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1379,9 +1322,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1394,87 +1334,67 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1707,14 +1627,14 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="72"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1737,14 +1657,14 @@
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1795,16 +1715,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="77" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="68"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1827,17 +1747,17 @@
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="68"/>
+      <c r="F5" s="64"/>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1863,19 +1783,19 @@
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="79" t="s">
-        <v>56</v>
+      <c r="E6" s="63" t="s">
+        <v>54</v>
       </c>
-      <c r="F6" s="68"/>
+      <c r="F6" s="64"/>
       <c r="G6" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="4"/>
@@ -1899,19 +1819,19 @@
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="79" t="s">
-        <v>49</v>
+      <c r="B7" s="63" t="s">
+        <v>47</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="64"/>
       <c r="D7" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
-      <c r="E7" s="79" t="s">
-        <v>57</v>
+      <c r="E7" s="63" t="s">
+        <v>55</v>
       </c>
-      <c r="F7" s="68"/>
+      <c r="F7" s="64"/>
       <c r="G7" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="4"/>
@@ -1935,15 +1855,15 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="79" t="s">
-        <v>50</v>
+      <c r="B8" s="63" t="s">
+        <v>48</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="68"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="64"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4"/>
@@ -1967,15 +1887,15 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="68"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="4"/>
@@ -1999,15 +1919,15 @@
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="65" t="s">
-        <v>46</v>
+      <c r="C10" s="66"/>
+      <c r="D10" s="82" t="s">
+        <v>44</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="64"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="4"/>
@@ -2031,11 +1951,11 @@
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="64"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="4"/>
@@ -2059,11 +1979,11 @@
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="64"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="68"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2087,11 +2007,11 @@
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="62"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
       <c r="G13" s="32"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2115,11 +2035,11 @@
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="72"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="72"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
       <c r="G14" s="33"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2199,14 +2119,14 @@
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="111" t="s">
-        <v>51</v>
+      <c r="B17" s="84" t="s">
+        <v>49</v>
       </c>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="113"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2229,14 +2149,14 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="114" t="s">
-        <v>48</v>
+      <c r="B18" s="87" t="s">
+        <v>46</v>
       </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="115"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="89"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2259,14 +2179,14 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="116" t="s">
-        <v>47</v>
+      <c r="B19" s="57" t="s">
+        <v>45</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="117"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2289,14 +2209,14 @@
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="116" t="s">
-        <v>58</v>
+      <c r="B20" s="57" t="s">
+        <v>56</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="117"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="59"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2319,14 +2239,14 @@
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="118" t="s">
-        <v>59</v>
+      <c r="B21" s="76" t="s">
+        <v>57</v>
       </c>
-      <c r="C21" s="119"/>
-      <c r="D21" s="119"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="120"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="78"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2349,14 +2269,14 @@
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="116" t="s">
-        <v>98</v>
+      <c r="B22" s="57" t="s">
+        <v>89</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="117"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="59"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2379,12 +2299,12 @@
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="117"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="59"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2407,16 +2327,16 @@
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="121" t="s">
-        <v>99</v>
+      <c r="B24" s="60" t="s">
+        <v>90</v>
       </c>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122"/>
-      <c r="E24" s="122"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="123"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="62"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="110"/>
+      <c r="I24" s="55"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -29821,6 +29741,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
@@ -29836,23 +29772,7 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29863,8 +29783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32:L34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29906,19 +29826,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="62"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -29936,17 +29856,17 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="81"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -29964,27 +29884,27 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="94" t="s">
+      <c r="D4" s="64"/>
+      <c r="E4" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="95" t="s">
+      <c r="F4" s="75"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="95" t="s">
+      <c r="I4" s="75"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="68"/>
+      <c r="L4" s="64"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -30002,7 +29922,7 @@
     </row>
     <row r="5" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="66"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
@@ -30031,7 +29951,7 @@
         <v>22</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -30078,7 +29998,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L6" s="14">
         <v>246</v>
@@ -30128,7 +30048,7 @@
         <v>1800</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L7" s="13">
         <v>2625</v>
@@ -30151,30 +30071,30 @@
     <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="100" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
-      <c r="C8" s="87">
+      <c r="C8" s="102">
         <v>17.579999999999998</v>
       </c>
-      <c r="D8" s="87">
+      <c r="D8" s="102">
         <v>23.9</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="107">
         <v>3</v>
       </c>
-      <c r="F8" s="83">
+      <c r="F8" s="107">
         <v>100</v>
       </c>
-      <c r="G8" s="85">
+      <c r="G8" s="108">
         <v>300</v>
       </c>
-      <c r="H8" s="101">
+      <c r="H8" s="108">
         <v>4</v>
       </c>
-      <c r="I8" s="103" t="s">
-        <v>37</v>
+      <c r="I8" s="109" t="s">
+        <v>36</v>
       </c>
-      <c r="J8" s="105">
+      <c r="J8" s="107">
         <v>200</v>
       </c>
       <c r="K8" s="98"/>
@@ -30196,15 +30116,15 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
       <c r="K9" s="99"/>
       <c r="L9" s="99"/>
       <c r="M9" s="1"/>
@@ -30225,7 +30145,7 @@
     <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="15">
         <v>21.83</v>
@@ -30484,13 +30404,13 @@
         <v>6</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J15" s="19">
         <v>2100</v>
       </c>
       <c r="K15" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L15" s="19">
         <v>1760</v>
@@ -30530,14 +30450,14 @@
       <c r="G16" s="13">
         <v>400</v>
       </c>
-      <c r="H16" s="38">
-        <v>4</v>
+      <c r="H16" s="112">
+        <v>1</v>
       </c>
-      <c r="I16" s="39" t="s">
-        <v>42</v>
+      <c r="I16" s="113">
+        <v>600</v>
       </c>
-      <c r="J16" s="40">
-        <v>1400</v>
+      <c r="J16" s="114">
+        <v>600</v>
       </c>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
@@ -30626,13 +30546,13 @@
         <v>3</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" s="19">
         <v>1900</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L18" s="19">
         <v>1650</v>
@@ -30663,26 +30583,26 @@
       <c r="D19" s="18">
         <v>25.3</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="114">
         <v>5</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="114">
         <v>100</v>
       </c>
-      <c r="G19" s="37">
+      <c r="G19" s="112">
         <v>500</v>
       </c>
       <c r="H19" s="13">
         <v>5</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J19" s="19">
         <v>2000</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L19" s="19">
         <v>1650</v>
@@ -30726,7 +30646,7 @@
         <v>5</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J20" s="13">
         <v>2000</v>
@@ -30751,7 +30671,7 @@
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="28">
         <f t="shared" ref="C21:J21" si="0">SUM(C6:C20)</f>
@@ -30775,15 +30695,15 @@
       </c>
       <c r="H21" s="28">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I21" s="28">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>4200</v>
       </c>
       <c r="J21" s="28">
         <f t="shared" si="0"/>
-        <v>14400</v>
+        <v>13600</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="28">
@@ -30835,13 +30755,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="127" t="s">
-        <v>103</v>
+      <c r="B23" s="90" t="s">
+        <v>92</v>
       </c>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -30864,19 +30784,21 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="128" t="s">
-        <v>102</v>
+      <c r="B24" s="56" t="s">
+        <v>91</v>
       </c>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="J24" s="115"/>
+      <c r="K24" s="115"/>
+      <c r="L24" s="116"/>
+      <c r="M24" s="116"/>
+      <c r="N24" s="116"/>
+      <c r="O24" s="116"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -30891,23 +30813,21 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="128" t="s">
-        <v>44</v>
+      <c r="B25" s="56" t="s">
+        <v>42</v>
       </c>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="J25" s="96" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="96"/>
-      <c r="L25" s="96"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+      <c r="J25" s="117"/>
+      <c r="K25" s="117"/>
+      <c r="L25" s="117"/>
+      <c r="M25" s="116"/>
+      <c r="N25" s="116"/>
+      <c r="O25" s="116"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -30922,24 +30842,22 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="B26" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="K26" s="81"/>
-      <c r="L26" s="81"/>
-      <c r="M26" s="124" t="s">
-        <v>100</v>
-      </c>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="118"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="116"/>
+      <c r="O26" s="116"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -30962,14 +30880,12 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="81" t="s">
-        <v>75</v>
-      </c>
-      <c r="K27" s="81"/>
-      <c r="L27" s="81"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="120"/>
+      <c r="N27" s="116"/>
+      <c r="O27" s="116"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -30992,16 +30908,12 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="82" t="s">
-        <v>76</v>
-      </c>
-      <c r="K28" s="82"/>
-      <c r="L28" s="82"/>
-      <c r="M28" s="126" t="s">
-        <v>101</v>
-      </c>
-      <c r="N28" s="126"/>
-      <c r="O28" s="126"/>
+      <c r="J28" s="118"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="118"/>
+      <c r="M28" s="121"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="121"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -31024,14 +30936,12 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="K29" s="82"/>
-      <c r="L29" s="82"/>
-      <c r="M29" s="126"/>
-      <c r="N29" s="126"/>
-      <c r="O29" s="126"/>
+      <c r="J29" s="118"/>
+      <c r="K29" s="118"/>
+      <c r="L29" s="118"/>
+      <c r="M29" s="121"/>
+      <c r="N29" s="121"/>
+      <c r="O29" s="121"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -31054,16 +30964,12 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" s="80"/>
-      <c r="L30" s="80"/>
-      <c r="M30" s="124" t="s">
-        <v>100</v>
-      </c>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="118"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="116"/>
+      <c r="O30" s="116"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
@@ -31086,14 +30992,12 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="K31" s="80"/>
-      <c r="L31" s="80"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
+      <c r="J31" s="118"/>
+      <c r="K31" s="118"/>
+      <c r="L31" s="118"/>
+      <c r="M31" s="120"/>
+      <c r="N31" s="116"/>
+      <c r="O31" s="116"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -31116,14 +31020,12 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="89" t="s">
-        <v>80</v>
-      </c>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
+      <c r="J32" s="122"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="122"/>
+      <c r="M32" s="116"/>
+      <c r="N32" s="116"/>
+      <c r="O32" s="116"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -31146,12 +31048,12 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="89"/>
-      <c r="K33" s="89"/>
-      <c r="L33" s="89"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="116"/>
+      <c r="N33" s="116"/>
+      <c r="O33" s="116"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -31174,12 +31076,12 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="89"/>
-      <c r="K34" s="89"/>
-      <c r="L34" s="89"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="J34" s="122"/>
+      <c r="K34" s="122"/>
+      <c r="L34" s="122"/>
+      <c r="M34" s="116"/>
+      <c r="N34" s="116"/>
+      <c r="O34" s="116"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -58129,19 +58031,7 @@
       <c r="Z996" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="M28:O29"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="J32:L34"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="J25:L25"/>
+  <mergeCells count="31">
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="L8:L9"/>
@@ -58154,12 +58044,25 @@
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="M28:O29"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="J32:L34"/>
+    <mergeCell ref="J25:L25"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="J26:L26"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="J28:L28"/>
     <mergeCell ref="J29:L29"/>
+    <mergeCell ref="B26:F26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -58170,7 +58073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398C07AF-3B06-4C71-BE66-D657F989F064}">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -58186,519 +58089,519 @@
     <row r="1" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="103" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="106"/>
+      <c r="F3" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="107" t="s">
-        <v>81</v>
+      <c r="G3" s="106"/>
+      <c r="H3" s="49" t="s">
+        <v>16</v>
       </c>
-      <c r="D3" s="108" t="s">
+      <c r="I3" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="108" t="s">
+      <c r="J3" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="109"/>
-      <c r="H3" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="46" t="s">
+      <c r="K3" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="27" t="s">
-        <v>72</v>
+    </row>
+    <row r="4" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="43" t="s">
+        <v>60</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="E4" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="36">
+        <v>1</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="106"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41">
-        <v>1</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="50">
+      <c r="D5" s="45">
         <v>8</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="46">
         <v>4</v>
       </c>
-      <c r="F5" s="50"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="47">
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="42">
         <f t="shared" ref="I5:I10" si="0">(D5*100+E5*200)+(F5*100+G5*600)+H5</f>
         <v>1600</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="36">
         <v>127</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="37">
         <f t="shared" ref="K5:K13" si="1">I5/J5</f>
         <v>12.598425196850394</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41">
+      <c r="B6" s="36">
         <v>2</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>83</v>
+      <c r="C6" s="40" t="s">
+        <v>74</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D6" s="45">
         <v>13</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="47">
+      <c r="E6" s="46"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="42">
         <f t="shared" si="0"/>
         <v>1300</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="36">
         <v>127</v>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="37">
         <f t="shared" si="1"/>
         <v>10.236220472440944</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41">
+      <c r="B7" s="36">
         <v>3</v>
       </c>
-      <c r="C7" s="45" t="s">
-        <v>91</v>
+      <c r="C7" s="40" t="s">
+        <v>82</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="50">
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="45">
         <v>3</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="46">
         <v>3</v>
       </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="47">
+      <c r="H7" s="51"/>
+      <c r="I7" s="42">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="36">
         <v>127</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="37">
         <f t="shared" si="1"/>
         <v>16.535433070866141</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41">
+      <c r="B8" s="36">
         <v>4</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>97</v>
+      <c r="C8" s="40" t="s">
+        <v>88</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="50">
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="45">
         <v>1</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="46">
         <v>3</v>
       </c>
-      <c r="H8" s="56"/>
-      <c r="I8" s="47">
+      <c r="H8" s="51"/>
+      <c r="I8" s="42">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="36">
         <v>127</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="37">
         <f t="shared" si="1"/>
         <v>14.960629921259843</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41">
+      <c r="B9" s="36">
         <v>5</v>
       </c>
-      <c r="C9" s="45" t="s">
-        <v>92</v>
+      <c r="C9" s="40" t="s">
+        <v>83</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="50">
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="45">
         <v>2</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="46">
         <v>3</v>
       </c>
-      <c r="H9" s="56"/>
-      <c r="I9" s="47">
+      <c r="H9" s="51"/>
+      <c r="I9" s="42">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="36">
         <v>127</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="37">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41">
+      <c r="B10" s="36">
         <v>6</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>95</v>
+      <c r="C10" s="40" t="s">
+        <v>86</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="50">
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="45">
         <v>1</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="46">
         <v>4</v>
       </c>
-      <c r="H10" s="56"/>
-      <c r="I10" s="47">
+      <c r="H10" s="51"/>
+      <c r="I10" s="42">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="36">
         <v>127</v>
       </c>
-      <c r="K10" s="42">
+      <c r="K10" s="37">
         <f t="shared" si="1"/>
         <v>19.685039370078741</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41">
+      <c r="B11" s="36">
         <v>7</v>
       </c>
-      <c r="C11" s="45" t="s">
-        <v>93</v>
+      <c r="C11" s="40" t="s">
+        <v>84</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="50">
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="45">
         <v>2</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="46">
         <v>3</v>
       </c>
-      <c r="H11" s="56"/>
-      <c r="I11" s="47">
+      <c r="H11" s="51"/>
+      <c r="I11" s="42">
         <f>(D11*100+E11*200)+(F11*100+G11*600)+H11</f>
         <v>2000</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="36">
         <v>127</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="37">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41">
+      <c r="B12" s="36">
         <v>8</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>94</v>
+      <c r="C12" s="40" t="s">
+        <v>85</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="50">
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="45">
         <v>2</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="46">
         <v>3</v>
       </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="47">
+      <c r="H12" s="51"/>
+      <c r="I12" s="42">
         <f>(D12*100+E12*200)+(F12*100+G12*600)+H12</f>
         <v>2000</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="36">
         <v>127</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="37">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41">
+      <c r="B13" s="36">
         <v>9</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>96</v>
+      <c r="C13" s="40" t="s">
+        <v>87</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="50">
+      <c r="D13" s="45"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="45">
         <v>2</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="46">
         <v>3</v>
       </c>
-      <c r="H13" s="56"/>
-      <c r="I13" s="47">
+      <c r="H13" s="51"/>
+      <c r="I13" s="42">
         <f>(D13*100+E13*200)+(F13*100+G13*600)+H13</f>
         <v>2000</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J13" s="36">
         <v>127</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="37">
         <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="41">
+      <c r="B14" s="36">
         <v>10</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>84</v>
+      <c r="C14" s="40" t="s">
+        <v>75</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="56">
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="51">
         <v>5400</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="42">
         <f>(D14*100+E14*200)+(F14*100+G14*600)+H14</f>
         <v>5400</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="36">
         <v>220</v>
       </c>
-      <c r="K14" s="42">
+      <c r="K14" s="37">
         <f>I14/J14</f>
         <v>24.545454545454547</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="41">
+      <c r="B15" s="36">
         <v>11</v>
       </c>
-      <c r="C15" s="45" t="s">
-        <v>85</v>
+      <c r="C15" s="40" t="s">
+        <v>76</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="56">
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="51">
         <v>5400</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="42">
         <f t="shared" ref="I15:I20" si="2">(D15*100+E15*200)+(F15*100+G15*600)+H15</f>
         <v>5400</v>
       </c>
-      <c r="J15" s="41">
+      <c r="J15" s="36">
         <v>220</v>
       </c>
-      <c r="K15" s="42">
+      <c r="K15" s="37">
         <f>I15/J15</f>
         <v>24.545454545454547</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41">
+      <c r="B16" s="36">
         <v>12</v>
       </c>
-      <c r="C16" s="45" t="s">
-        <v>86</v>
+      <c r="C16" s="40" t="s">
+        <v>77</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="56">
+      <c r="D16" s="45"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="51">
         <v>2625</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="42">
         <f t="shared" si="2"/>
         <v>2625</v>
       </c>
-      <c r="J16" s="41">
+      <c r="J16" s="36">
         <v>220</v>
       </c>
-      <c r="K16" s="42">
+      <c r="K16" s="37">
         <f>I16/J16</f>
         <v>11.931818181818182</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="41">
+      <c r="B17" s="36">
         <v>13</v>
       </c>
-      <c r="C17" s="45" t="s">
-        <v>87</v>
+      <c r="C17" s="40" t="s">
+        <v>78</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="56">
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="51">
         <v>1650</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="42">
         <f t="shared" si="2"/>
         <v>1650</v>
       </c>
-      <c r="J17" s="41">
+      <c r="J17" s="36">
         <v>220</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="37">
         <f t="shared" ref="K17:K20" si="3">I17/J17</f>
         <v>7.5</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41">
+      <c r="B18" s="36">
         <v>14</v>
       </c>
-      <c r="C18" s="45" t="s">
-        <v>88</v>
+      <c r="C18" s="40" t="s">
+        <v>79</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="56">
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="51">
         <v>1650</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="42">
         <f t="shared" si="2"/>
         <v>1650</v>
       </c>
-      <c r="J18" s="41">
+      <c r="J18" s="36">
         <v>220</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="37">
         <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="41">
+      <c r="B19" s="36">
         <v>15</v>
       </c>
-      <c r="C19" s="45" t="s">
-        <v>89</v>
+      <c r="C19" s="40" t="s">
+        <v>80</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="57">
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="52">
         <v>246</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="42">
         <f t="shared" si="2"/>
         <v>246</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="36">
         <v>127</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="37">
         <f t="shared" si="3"/>
         <v>1.9370078740157479</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="41">
+      <c r="B20" s="36">
         <v>16</v>
       </c>
-      <c r="C20" s="45" t="s">
-        <v>90</v>
+      <c r="C20" s="40" t="s">
+        <v>81</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="58">
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="53">
         <v>1760</v>
       </c>
-      <c r="I20" s="47">
+      <c r="I20" s="42">
         <f t="shared" si="2"/>
         <v>1760</v>
       </c>
-      <c r="J20" s="41">
+      <c r="J20" s="36">
         <v>220</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="37">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="52">
+      <c r="C21" s="39"/>
+      <c r="D21" s="47">
         <f t="shared" ref="D21:K21" si="4">SUM(D5:D20)</f>
         <v>21</v>
       </c>
-      <c r="E21" s="53">
+      <c r="E21" s="48">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="47">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="48">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="H21" s="59">
+      <c r="H21" s="54">
         <f t="shared" si="4"/>
         <v>18731</v>
       </c>
-      <c r="I21" s="46">
+      <c r="I21" s="41">
         <f t="shared" si="4"/>
         <v>36131</v>
       </c>
@@ -58706,7 +58609,7 @@
         <f t="shared" si="4"/>
         <v>2590</v>
       </c>
-      <c r="K21" s="43">
+      <c r="K21" s="38">
         <f t="shared" si="4"/>
         <v>222.96760916249107</v>
       </c>

</xml_diff>

<commit_message>
Capacidade de corrente calculada
Necessário remover cores CLARAS do nosso projeto (Branco/Amarelo/Azul Claro), porque a impressão A3 será feito em papel A3 branco.

Exemplo de como fica a impressão com as cores atuais está na pasta 3ª Entrega.
</commit_message>
<xml_diff>
--- a/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
+++ b/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\GitHub\Instel-I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66BB6E6-A082-4092-8FA7-ABD1266037CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD629833-662B-48D6-BD96-1F4358C3A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação_Informações" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Quadro_de_cargas" sheetId="3" r:id="rId3"/>
     <sheet name="Secção Mínima" sheetId="4" r:id="rId4"/>
     <sheet name="Capacidade de Corrente" sheetId="5" r:id="rId5"/>
+    <sheet name="Limite de Queda de Tensão" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
   <si>
     <t>Alunos: Gabriel Schettino Lucas e Ramon Rodrigues Morello</t>
   </si>
@@ -482,14 +483,61 @@
     <t xml:space="preserve">Como usar o FCA no nosso caso? R: considerar o condutor por onde o circuito mais tem contato com outros cabos. </t>
   </si>
   <si>
-    <t>Ex.: em um trecho o circuito 1, está junto de outros 4 circuitos, logo o FCA desse trecho é o que vale</t>
+    <t>Ex.: em um trecho o circuito 1, está junto de outros 4 circuitos, logo o FCA desse trecho é o que vale para todos</t>
+  </si>
+  <si>
+    <t>Para os circuitos reservas foi suposto que eles vão se agrupar nos eletrodutos que já possuem 5 cabos, passando no máximo para 6 cabos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">considerando a suposição acima, eu deveria considerar um circuito a mais em todos os eletrodutos, visando que um dia pode ser colocado um circuito extra? </t>
+  </si>
+  <si>
+    <t>opinião: gasto desnecessário, se em ocasião futura for adicionado um dos circuitos reservas, deverá quebrar a parede e trocar todos os cabos por cabos maiores. Outra, duvido que ele tenha tempo para verificar 1 por 1.</t>
+  </si>
+  <si>
+    <t>ALIMENTADOR</t>
+  </si>
+  <si>
+    <t>CAPACIDADE DE CORRENTE [IC]</t>
+  </si>
+  <si>
+    <t>REFERÊNCIAS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1]: Tabela de capacidade de condução de corrente em ampéres (Referência B1/3 condutores carregados) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>[Inserir as tabela como imagem nessa planilha]</t>
+    </r>
+  </si>
+  <si>
+    <t>[mm²]</t>
+  </si>
+  <si>
+    <t>CAPACIDADE DE CORRENTE TABELADA [IC']*[1]</t>
+  </si>
+  <si>
+    <t>RESULTADO DO CRITÉRIO DA CAP. CORRENTE</t>
+  </si>
+  <si>
+    <t>WHAT?</t>
+  </si>
+  <si>
+    <t>[IC']:  Capacidade de corrente que será usada para dimensionar eletrodutos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,21 +642,51 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
-      <sz val="22"/>
+      <sz val="28"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="36"/>
+      <sz val="28"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,8 +711,20 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -1155,11 +1245,137 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1307,20 +1523,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1333,45 +1588,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1386,22 +1630,18 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,48 +1655,120 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="20" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1675,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1689,14 +2001,14 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="76"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1719,14 +2031,14 @@
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="76"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1777,16 +2089,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="79"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="58"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="60"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1809,17 +2121,17 @@
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="58"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1845,17 +2157,17 @@
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="58"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1881,17 +2193,17 @@
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1917,15 +2229,15 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4"/>
@@ -1949,15 +2261,15 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="4"/>
@@ -1981,15 +2293,15 @@
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="55" t="s">
+      <c r="C10" s="71"/>
+      <c r="D10" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="4"/>
@@ -2013,11 +2325,11 @@
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="58"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="4"/>
@@ -2041,11 +2353,11 @@
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2069,11 +2381,11 @@
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="68"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="7"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2097,11 +2409,11 @@
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="58"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2181,14 +2493,14 @@
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="52"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2211,14 +2523,14 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="63"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2241,14 +2553,14 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="67"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2271,14 +2583,14 @@
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="67"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="63"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2301,14 +2613,14 @@
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="63"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2331,14 +2643,14 @@
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="67"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="63"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2361,12 +2673,12 @@
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="67"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="63"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2389,14 +2701,14 @@
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="54"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="66"/>
       <c r="H24" s="1"/>
       <c r="I24" s="8"/>
       <c r="J24" s="1"/>
@@ -8795,6 +9107,24 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
@@ -8809,24 +9139,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -8880,19 +9192,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="52"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -8910,17 +9222,17 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="54"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="66"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -8938,27 +9250,27 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="86" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="87" t="s">
+      <c r="F4" s="79"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="87" t="s">
+      <c r="I4" s="79"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="58"/>
+      <c r="L4" s="60"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -8976,7 +9288,7 @@
     </row>
     <row r="5" spans="1:26" ht="39.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="56"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
@@ -9124,35 +9436,35 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="101">
         <v>17.579999999999998</v>
       </c>
-      <c r="D8" s="83">
+      <c r="D8" s="101">
         <v>23.9</v>
       </c>
-      <c r="E8" s="79">
+      <c r="E8" s="87">
         <v>3</v>
       </c>
-      <c r="F8" s="79">
+      <c r="F8" s="87">
         <v>100</v>
       </c>
-      <c r="G8" s="77">
+      <c r="G8" s="97">
         <v>300</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="97">
         <v>4</v>
       </c>
-      <c r="I8" s="79" t="s">
+      <c r="I8" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="79">
+      <c r="J8" s="87">
         <v>200</v>
       </c>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -9170,17 +9482,17 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -9793,9 +10105,9 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -9813,13 +10125,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -9878,9 +10190,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="66"/>
-      <c r="L25" s="66"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -9898,20 +10210,20 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="88"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="84"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -9936,10 +10248,10 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="66"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -9964,12 +10276,12 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="66"/>
-      <c r="M28" s="93"/>
-      <c r="N28" s="66"/>
-      <c r="O28" s="66"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -9992,12 +10304,12 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="66"/>
-      <c r="N29" s="66"/>
-      <c r="O29" s="66"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -10020,10 +10332,10 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="88"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="84"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -10048,10 +10360,10 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="66"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="62"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -10076,9 +10388,9 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="90"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="66"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -10104,9 +10416,9 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="66"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -10132,9 +10444,9 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="66"/>
-      <c r="L34" s="66"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -16302,6 +16614,23 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="J32:L34"/>
@@ -16316,23 +16645,6 @@
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="M30:M31"/>
     <mergeCell ref="J31:L31"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B23:F23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16343,8 +16655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" topLeftCell="F10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16414,20 +16726,20 @@
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="97" t="s">
+      <c r="E3" s="106"/>
+      <c r="F3" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="98"/>
+      <c r="G3" s="106"/>
       <c r="H3" s="30" t="s">
         <v>30</v>
       </c>
@@ -16458,8 +16770,8 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="96"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="32" t="s">
         <v>72</v>
       </c>
@@ -44878,263 +45190,263 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6759B52-4959-44EC-8CDD-E150AEF41805}">
   <dimension ref="B4:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="99"/>
-    <col min="2" max="2" width="15.7109375" style="99" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="99" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="99" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="99"/>
+    <col min="1" max="1" width="9.140625" style="51"/>
+    <col min="2" max="2" width="15.7109375" style="51" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="51" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="51" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="51"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="109" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="104"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="110"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="102">
+      <c r="B6" s="53">
         <v>1</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="105">
+      <c r="D6" s="54">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="102">
+      <c r="B7" s="53">
         <v>2</v>
       </c>
-      <c r="C7" s="102" t="s">
+      <c r="C7" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="105">
+      <c r="D7" s="54">
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="102">
+      <c r="B8" s="53">
         <v>3</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="105">
+      <c r="D8" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="102">
+      <c r="B9" s="53">
         <v>4</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="105">
+      <c r="D9" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="102">
+      <c r="B10" s="53">
         <v>5</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="105">
+      <c r="D10" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="102">
+      <c r="B11" s="53">
         <v>6</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="105">
+      <c r="D11" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="102">
+      <c r="B12" s="53">
         <v>7</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="105">
+      <c r="D12" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="102">
+      <c r="B13" s="53">
         <v>8</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="105">
+      <c r="D13" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="102">
+      <c r="B14" s="53">
         <v>9</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="105">
+      <c r="D14" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="102">
+      <c r="B15" s="53">
         <v>10</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="105">
+      <c r="D15" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="102">
+      <c r="B16" s="53">
         <v>11</v>
       </c>
-      <c r="C16" s="105" t="s">
+      <c r="C16" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="105">
+      <c r="D16" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="102">
+      <c r="B17" s="53">
         <v>12</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="105">
+      <c r="D17" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="102">
+      <c r="B18" s="53">
         <v>13</v>
       </c>
-      <c r="C18" s="105" t="s">
+      <c r="C18" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="105">
+      <c r="D18" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="102">
+      <c r="B19" s="53">
         <v>14</v>
       </c>
-      <c r="C19" s="105" t="s">
+      <c r="C19" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="105">
+      <c r="D19" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="102">
+      <c r="B20" s="53">
         <v>15</v>
       </c>
-      <c r="C20" s="105" t="s">
+      <c r="C20" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="105">
+      <c r="D20" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="102">
+      <c r="B21" s="53">
         <v>16</v>
       </c>
-      <c r="C21" s="105" t="s">
+      <c r="C21" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="105">
+      <c r="D21" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="102">
+      <c r="B22" s="53">
         <v>17</v>
       </c>
-      <c r="C22" s="105" t="s">
+      <c r="C22" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="105">
+      <c r="D22" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="102">
+      <c r="B23" s="53">
         <v>18</v>
       </c>
-      <c r="C23" s="102" t="s">
+      <c r="C23" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="105">
+      <c r="D23" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="102">
+      <c r="B24" s="53">
         <v>19</v>
       </c>
-      <c r="C24" s="102" t="s">
+      <c r="C24" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="105">
+      <c r="D24" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="102">
+      <c r="B25" s="53">
         <v>20</v>
       </c>
-      <c r="C25" s="102" t="s">
+      <c r="C25" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="105">
+      <c r="D25" s="54">
         <v>2.5</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="102">
+      <c r="B26" s="53">
         <v>21</v>
       </c>
-      <c r="C26" s="102" t="s">
+      <c r="C26" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="105">
+      <c r="D26" s="54">
         <v>2.5</v>
       </c>
     </row>
@@ -45151,1043 +45463,1748 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36D55B-3867-4EF4-9271-23288EED3B45}">
-  <dimension ref="B1:N40"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="107"/>
-    <col min="2" max="2" width="15.7109375" style="107" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" style="107" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" style="107" customWidth="1"/>
-    <col min="6" max="14" width="15.7109375" style="107" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="107"/>
+    <col min="1" max="1" width="9.140625" style="55"/>
+    <col min="2" max="2" width="15.7109375" style="55" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" style="55" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" style="55" customWidth="1"/>
+    <col min="6" max="14" width="15.7109375" style="55" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="55" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" style="55" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" style="55" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="55" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
-      <c r="B1" s="100" t="s">
+    <row r="1" spans="2:17">
+      <c r="B1" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100" t="s">
+      <c r="E1" s="133"/>
+      <c r="F1" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100" t="s">
+      <c r="G1" s="133"/>
+      <c r="H1" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="K1" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="L1" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="M1" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="N1" s="109" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="2:14">
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-    </row>
-    <row r="3" spans="2:14">
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="108" t="s">
+      <c r="O1" s="109" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" s="109" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" s="109" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+    </row>
+    <row r="3" spans="2:17" ht="31.5" customHeight="1">
+      <c r="B3" s="107"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="108" t="s">
+      <c r="F4" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="108" t="s">
+      <c r="G4" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="108" t="s">
+      <c r="H4" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="108" t="s">
+      <c r="J4" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="108" t="s">
+      <c r="K4" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="111" t="s">
+      <c r="L4" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="M4" s="111" t="s">
+      <c r="M4" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="111" t="s">
+      <c r="N4" s="58" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
-      <c r="B5" s="102">
+      <c r="O4" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q4" s="58" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="53">
         <v>1</v>
       </c>
-      <c r="C5" s="102" t="s">
+      <c r="C5" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="102">
+      <c r="D5" s="53">
         <v>8</v>
       </c>
-      <c r="E5" s="102">
+      <c r="E5" s="53">
         <v>2</v>
       </c>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102">
-        <f t="shared" ref="I5:I21" si="0">(D5*100+E5*200)+(F5*100+G5*600)+H5</f>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53">
+        <f>(D5*100+E5*200)+(F5*100+G5*600)+H5</f>
         <v>1200</v>
       </c>
-      <c r="J5" s="102">
+      <c r="J5" s="53">
         <v>127</v>
       </c>
-      <c r="K5" s="109">
-        <f t="shared" ref="K5:L25" si="1">I5/J5</f>
+      <c r="K5" s="56">
+        <f t="shared" ref="K5:K25" si="0">I5/J5</f>
         <v>9.4488188976377945</v>
       </c>
-      <c r="L5" s="109"/>
-      <c r="M5" s="109">
+      <c r="L5" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M5" s="56">
         <v>1</v>
       </c>
-      <c r="N5" s="109">
+      <c r="N5" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:14">
-      <c r="B6" s="102">
+      <c r="O5" s="56">
+        <f>K5/L5*M5*N5</f>
+        <v>15.748031496062991</v>
+      </c>
+      <c r="P5" s="56">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="56">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="53">
         <v>2</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="102">
+      <c r="D6" s="53">
         <v>13</v>
       </c>
-      <c r="E6" s="102">
+      <c r="E6" s="53">
         <v>2</v>
       </c>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102">
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53">
+        <f>(D6*100+E6*200)+(F6*100+G6*600)+H6</f>
+        <v>1700</v>
+      </c>
+      <c r="J6" s="53">
+        <v>127</v>
+      </c>
+      <c r="K6" s="56">
         <f t="shared" si="0"/>
-        <v>1700</v>
-      </c>
-      <c r="J6" s="102">
+        <v>13.385826771653543</v>
+      </c>
+      <c r="L6" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M6" s="56">
+        <v>1</v>
+      </c>
+      <c r="N6" s="56">
+        <v>1</v>
+      </c>
+      <c r="O6" s="56">
+        <f>K6/L6*M6*N6</f>
+        <v>22.309711286089239</v>
+      </c>
+      <c r="P6" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="53">
+        <v>3</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53">
+        <v>3</v>
+      </c>
+      <c r="G7" s="53">
+        <v>3</v>
+      </c>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53">
+        <f>(D7*100+E7*200)+(F7*100+G7*600)+H7</f>
+        <v>2100</v>
+      </c>
+      <c r="J7" s="53">
         <v>127</v>
       </c>
-      <c r="K6" s="109">
+      <c r="K7" s="56">
+        <f t="shared" si="0"/>
+        <v>16.535433070866141</v>
+      </c>
+      <c r="L7" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M7" s="56">
+        <v>1</v>
+      </c>
+      <c r="N7" s="56">
+        <v>1</v>
+      </c>
+      <c r="O7" s="56">
+        <f t="shared" ref="O7:O25" si="1">K7/L7*M7*N7</f>
+        <v>27.559055118110237</v>
+      </c>
+      <c r="P7" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="53">
+        <v>4</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53">
+        <v>1</v>
+      </c>
+      <c r="G8" s="53">
+        <v>3</v>
+      </c>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53">
+        <f>(D8*100+E8*200)+(F8*100+G8*600)+H8</f>
+        <v>1900</v>
+      </c>
+      <c r="J8" s="53">
+        <v>127</v>
+      </c>
+      <c r="K8" s="56">
+        <f t="shared" si="0"/>
+        <v>14.960629921259843</v>
+      </c>
+      <c r="L8" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M8" s="56">
+        <v>1</v>
+      </c>
+      <c r="N8" s="56">
+        <v>1</v>
+      </c>
+      <c r="O8" s="56">
         <f t="shared" si="1"/>
-        <v>13.385826771653543</v>
-      </c>
-      <c r="L6" s="109">
+        <v>24.934383202099738</v>
+      </c>
+      <c r="P8" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="53">
+        <v>5</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53">
+        <v>1</v>
+      </c>
+      <c r="G9" s="53">
+        <v>3</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53">
+        <f>(D9*100+E9*200)+(F9*100+G9*600)+H9</f>
+        <v>1900</v>
+      </c>
+      <c r="J9" s="53">
+        <v>127</v>
+      </c>
+      <c r="K9" s="56">
+        <f t="shared" si="0"/>
+        <v>14.960629921259843</v>
+      </c>
+      <c r="L9" s="56">
         <v>0.6</v>
       </c>
-      <c r="M6" s="109">
+      <c r="M9" s="56">
         <v>1</v>
       </c>
-      <c r="N6" s="109">
+      <c r="N9" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:14">
-      <c r="B7" s="102">
+      <c r="O9" s="56">
+        <f t="shared" si="1"/>
+        <v>24.934383202099738</v>
+      </c>
+      <c r="P9" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="53">
+        <v>6</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53">
+        <v>1</v>
+      </c>
+      <c r="G10" s="53">
+        <v>4</v>
+      </c>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53">
+        <f>(D10*100+E10*200)+(F10*100+G10*600)+H10</f>
+        <v>2500</v>
+      </c>
+      <c r="J10" s="53">
+        <v>127</v>
+      </c>
+      <c r="K10" s="56">
+        <f t="shared" si="0"/>
+        <v>19.685039370078741</v>
+      </c>
+      <c r="L10" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M10" s="56">
+        <v>1</v>
+      </c>
+      <c r="N10" s="56">
+        <v>1</v>
+      </c>
+      <c r="O10" s="56">
+        <f t="shared" si="1"/>
+        <v>32.808398950131235</v>
+      </c>
+      <c r="P10" s="56">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="53">
+        <v>7</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53">
+        <v>2</v>
+      </c>
+      <c r="G11" s="53">
         <v>3</v>
       </c>
-      <c r="C7" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102">
+      <c r="H11" s="53"/>
+      <c r="I11" s="53">
+        <f>(D11*100+E11*200)+(F11*100+G11*600)+H11</f>
+        <v>2000</v>
+      </c>
+      <c r="J11" s="53">
+        <v>127</v>
+      </c>
+      <c r="K11" s="56">
+        <f t="shared" si="0"/>
+        <v>15.748031496062993</v>
+      </c>
+      <c r="L11" s="56">
+        <v>0.65</v>
+      </c>
+      <c r="M11" s="56">
+        <v>1</v>
+      </c>
+      <c r="N11" s="56">
+        <v>1</v>
+      </c>
+      <c r="O11" s="56">
+        <f t="shared" si="1"/>
+        <v>24.227740763173834</v>
+      </c>
+      <c r="P11" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" s="53">
+        <v>8</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53">
+        <v>2</v>
+      </c>
+      <c r="G12" s="53">
         <v>3</v>
       </c>
-      <c r="G7" s="102">
+      <c r="H12" s="53"/>
+      <c r="I12" s="53">
+        <f>(D12*100+E12*200)+(F12*100+G12*600)+H12</f>
+        <v>2000</v>
+      </c>
+      <c r="J12" s="53">
+        <v>127</v>
+      </c>
+      <c r="K12" s="56">
+        <f t="shared" si="0"/>
+        <v>15.748031496062993</v>
+      </c>
+      <c r="L12" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M12" s="56">
+        <v>1</v>
+      </c>
+      <c r="N12" s="56">
+        <v>1</v>
+      </c>
+      <c r="O12" s="56">
+        <f t="shared" si="1"/>
+        <v>26.246719160104988</v>
+      </c>
+      <c r="P12" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" s="53">
+        <v>9</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53">
+        <v>2</v>
+      </c>
+      <c r="G13" s="53">
         <v>3</v>
       </c>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102">
+      <c r="H13" s="53"/>
+      <c r="I13" s="53">
+        <f>(D13*100+E13*200)+(F13*100+G13*600)+H13</f>
+        <v>2000</v>
+      </c>
+      <c r="J13" s="53">
+        <v>127</v>
+      </c>
+      <c r="K13" s="56">
         <f t="shared" si="0"/>
-        <v>2100</v>
-      </c>
-      <c r="J7" s="102">
+        <v>15.748031496062993</v>
+      </c>
+      <c r="L13" s="56">
+        <v>0.65</v>
+      </c>
+      <c r="M13" s="56">
+        <v>1</v>
+      </c>
+      <c r="N13" s="56">
+        <v>1</v>
+      </c>
+      <c r="O13" s="56">
+        <f t="shared" si="1"/>
+        <v>24.227740763173834</v>
+      </c>
+      <c r="P13" s="56">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="B14" s="53">
+        <v>10</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53">
+        <v>5400</v>
+      </c>
+      <c r="I14" s="53">
+        <f>(D14*100+E14*200)+(F14*100+G14*600)+H14</f>
+        <v>5400</v>
+      </c>
+      <c r="J14" s="53">
+        <v>220</v>
+      </c>
+      <c r="K14" s="56">
+        <f t="shared" si="0"/>
+        <v>24.545454545454547</v>
+      </c>
+      <c r="L14" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M14" s="56">
+        <v>1</v>
+      </c>
+      <c r="N14" s="56">
+        <v>1</v>
+      </c>
+      <c r="O14" s="56">
+        <f t="shared" si="1"/>
+        <v>40.909090909090914</v>
+      </c>
+      <c r="P14" s="56">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="B15" s="53">
+        <v>11</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53">
+        <v>5400</v>
+      </c>
+      <c r="I15" s="53">
+        <f>(D15*100+E15*200)+(F15*100+G15*600)+H15</f>
+        <v>5400</v>
+      </c>
+      <c r="J15" s="53">
+        <v>220</v>
+      </c>
+      <c r="K15" s="56">
+        <f t="shared" si="0"/>
+        <v>24.545454545454547</v>
+      </c>
+      <c r="L15" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M15" s="56">
+        <v>1</v>
+      </c>
+      <c r="N15" s="56">
+        <v>1</v>
+      </c>
+      <c r="O15" s="56">
+        <f t="shared" si="1"/>
+        <v>40.909090909090914</v>
+      </c>
+      <c r="P15" s="56">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="B16" s="53">
+        <v>12</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53">
+        <v>2625</v>
+      </c>
+      <c r="I16" s="53">
+        <f>(D16*100+E16*200)+(F16*100+G16*600)+H16</f>
+        <v>2625</v>
+      </c>
+      <c r="J16" s="53">
+        <v>220</v>
+      </c>
+      <c r="K16" s="56">
+        <f t="shared" si="0"/>
+        <v>11.931818181818182</v>
+      </c>
+      <c r="L16" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M16" s="56">
+        <v>1</v>
+      </c>
+      <c r="N16" s="56">
+        <v>1</v>
+      </c>
+      <c r="O16" s="56">
+        <f t="shared" si="1"/>
+        <v>19.886363636363637</v>
+      </c>
+      <c r="P16" s="56">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="56">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="53">
+        <v>13</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53">
+        <v>1650</v>
+      </c>
+      <c r="I17" s="53">
+        <f>(D17*100+E17*200)+(F17*100+G17*600)+H17</f>
+        <v>1650</v>
+      </c>
+      <c r="J17" s="53">
+        <v>220</v>
+      </c>
+      <c r="K17" s="56">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="L17" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M17" s="56">
+        <v>1</v>
+      </c>
+      <c r="N17" s="56">
+        <v>1</v>
+      </c>
+      <c r="O17" s="56">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="P17" s="56">
+        <v>15.5</v>
+      </c>
+      <c r="Q17" s="126">
+        <v>1.5</v>
+      </c>
+      <c r="R17" s="127" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="53">
+        <v>14</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53">
+        <v>1650</v>
+      </c>
+      <c r="I18" s="53">
+        <f>(D18*100+E18*200)+(F18*100+G18*600)+H18</f>
+        <v>1650</v>
+      </c>
+      <c r="J18" s="53">
+        <v>220</v>
+      </c>
+      <c r="K18" s="56">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="L18" s="56">
+        <v>0.65</v>
+      </c>
+      <c r="M18" s="56">
+        <v>1</v>
+      </c>
+      <c r="N18" s="56">
+        <v>1</v>
+      </c>
+      <c r="O18" s="56">
+        <f t="shared" si="1"/>
+        <v>11.538461538461538</v>
+      </c>
+      <c r="P18" s="56">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="53">
+        <v>15</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53">
+        <v>400</v>
+      </c>
+      <c r="I19" s="53">
+        <f>(D19*100+E19*200)+(F19*100+G19*600)+H19</f>
+        <v>400</v>
+      </c>
+      <c r="J19" s="53">
         <v>127</v>
       </c>
-      <c r="K7" s="109">
+      <c r="K19" s="56">
+        <f t="shared" si="0"/>
+        <v>3.1496062992125986</v>
+      </c>
+      <c r="L19" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M19" s="56">
+        <v>1</v>
+      </c>
+      <c r="N19" s="56">
+        <v>1</v>
+      </c>
+      <c r="O19" s="56">
         <f t="shared" si="1"/>
-        <v>16.535433070866141</v>
-      </c>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109">
+        <v>5.2493438320209975</v>
+      </c>
+      <c r="P19" s="56">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="128">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="53">
+        <v>16</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="57">
+        <v>1760</v>
+      </c>
+      <c r="I20" s="53">
+        <f>(D20*100+E20*200)+(F20*100+G20*600)+H20</f>
+        <v>1760</v>
+      </c>
+      <c r="J20" s="53">
+        <v>220</v>
+      </c>
+      <c r="K20" s="56">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L20" s="56">
+        <v>0.6</v>
+      </c>
+      <c r="M20" s="56">
         <v>1</v>
       </c>
-      <c r="N7" s="109">
+      <c r="N20" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="102">
-        <v>4</v>
-      </c>
-      <c r="C8" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102">
+      <c r="O20" s="56">
+        <f t="shared" si="1"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="P20" s="56">
+        <v>15.5</v>
+      </c>
+      <c r="Q20" s="128">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18">
+      <c r="B21" s="53">
+        <v>17</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="57">
+        <v>300</v>
+      </c>
+      <c r="I21" s="53">
+        <f>(D21*100+E21*200)+(F21*100+G21*600)+H21</f>
+        <v>300</v>
+      </c>
+      <c r="J21" s="53">
+        <v>220</v>
+      </c>
+      <c r="K21" s="56">
+        <f t="shared" si="0"/>
+        <v>1.3636363636363635</v>
+      </c>
+      <c r="L21" s="56">
+        <v>0.65</v>
+      </c>
+      <c r="M21" s="56">
         <v>1</v>
       </c>
-      <c r="G8" s="102">
-        <v>3</v>
-      </c>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102">
+      <c r="N21" s="56">
+        <v>1</v>
+      </c>
+      <c r="O21" s="56">
+        <f t="shared" si="1"/>
+        <v>2.0979020979020975</v>
+      </c>
+      <c r="P21" s="56">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="128">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18">
+      <c r="B22" s="53">
+        <v>18</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53">
+        <v>1</v>
+      </c>
+      <c r="H22" s="57"/>
+      <c r="I22" s="53">
+        <v>600</v>
+      </c>
+      <c r="J22" s="53">
+        <v>127</v>
+      </c>
+      <c r="K22" s="56">
         <f t="shared" si="0"/>
-        <v>1900</v>
-      </c>
-      <c r="J8" s="102">
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="L22" s="56">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M22" s="56">
+        <v>1</v>
+      </c>
+      <c r="N22" s="56">
+        <v>1</v>
+      </c>
+      <c r="O22" s="56">
+        <f t="shared" si="1"/>
+        <v>8.2884376295068378</v>
+      </c>
+      <c r="P22" s="56">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="56">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="B23" s="53">
+        <v>19</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53">
+        <v>1</v>
+      </c>
+      <c r="H23" s="57"/>
+      <c r="I23" s="53">
+        <v>600</v>
+      </c>
+      <c r="J23" s="53">
         <v>127</v>
       </c>
-      <c r="K8" s="109">
+      <c r="K23" s="56">
+        <f t="shared" si="0"/>
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="L23" s="56">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M23" s="56">
+        <v>1</v>
+      </c>
+      <c r="N23" s="56">
+        <v>1</v>
+      </c>
+      <c r="O23" s="56">
         <f t="shared" si="1"/>
-        <v>14.960629921259843</v>
-      </c>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109">
+        <v>8.2884376295068378</v>
+      </c>
+      <c r="P23" s="56">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="56">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18">
+      <c r="B24" s="53">
+        <v>20</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53">
         <v>1</v>
       </c>
-      <c r="N8" s="109">
+      <c r="H24" s="57"/>
+      <c r="I24" s="53">
+        <v>600</v>
+      </c>
+      <c r="J24" s="53">
+        <v>127</v>
+      </c>
+      <c r="K24" s="56">
+        <f t="shared" si="0"/>
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="L24" s="56">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M24" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="102">
-        <v>5</v>
-      </c>
-      <c r="C9" s="102" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102">
+      <c r="N24" s="56">
         <v>1</v>
       </c>
-      <c r="G9" s="102">
-        <v>3</v>
-      </c>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102">
+      <c r="O24" s="56">
+        <f t="shared" si="1"/>
+        <v>8.2884376295068378</v>
+      </c>
+      <c r="P24" s="56">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="56">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="53">
+        <v>21</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53">
+        <v>1</v>
+      </c>
+      <c r="H25" s="57"/>
+      <c r="I25" s="53">
+        <v>600</v>
+      </c>
+      <c r="J25" s="53">
+        <v>127</v>
+      </c>
+      <c r="K25" s="56">
         <f t="shared" si="0"/>
-        <v>1900</v>
-      </c>
-      <c r="J9" s="102">
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="L25" s="56">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M25" s="56">
+        <v>1</v>
+      </c>
+      <c r="N25" s="56">
+        <v>1</v>
+      </c>
+      <c r="O25" s="56">
+        <f t="shared" si="1"/>
+        <v>8.2884376295068378</v>
+      </c>
+      <c r="P25" s="56">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="56">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18">
+      <c r="B26" s="122">
+        <v>22</v>
+      </c>
+      <c r="C26" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="123"/>
+      <c r="I26" s="122">
+        <f>SUM(I5:I25)</f>
+        <v>38885</v>
+      </c>
+      <c r="J26" s="122"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="124"/>
+      <c r="Q26" s="124"/>
+    </row>
+    <row r="28" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B28" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="K9" s="109">
-        <f t="shared" si="1"/>
-        <v>14.960629921259843</v>
-      </c>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109">
-        <v>1</v>
-      </c>
-      <c r="N9" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" s="102">
-        <v>6</v>
-      </c>
-      <c r="C10" s="102" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102">
-        <v>1</v>
-      </c>
-      <c r="G10" s="102">
-        <v>4</v>
-      </c>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102">
-        <f t="shared" si="0"/>
-        <v>2500</v>
-      </c>
-      <c r="J10" s="102">
-        <v>127</v>
-      </c>
-      <c r="K10" s="109">
-        <f t="shared" si="1"/>
-        <v>19.685039370078741</v>
-      </c>
-      <c r="L10" s="109"/>
-      <c r="M10" s="109">
-        <v>1</v>
-      </c>
-      <c r="N10" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="102">
-        <v>7</v>
-      </c>
-      <c r="C11" s="102" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102">
-        <v>2</v>
-      </c>
-      <c r="G11" s="102">
-        <v>3</v>
-      </c>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="J11" s="102">
-        <v>127</v>
-      </c>
-      <c r="K11" s="109">
-        <f t="shared" si="1"/>
-        <v>15.748031496062993</v>
-      </c>
-      <c r="L11" s="109"/>
-      <c r="M11" s="109">
-        <v>1</v>
-      </c>
-      <c r="N11" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="102">
-        <v>8</v>
-      </c>
-      <c r="C12" s="102" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102">
-        <v>2</v>
-      </c>
-      <c r="G12" s="102">
-        <v>3</v>
-      </c>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="J12" s="102">
-        <v>127</v>
-      </c>
-      <c r="K12" s="109">
-        <f t="shared" si="1"/>
-        <v>15.748031496062993</v>
-      </c>
-      <c r="L12" s="109"/>
-      <c r="M12" s="109">
-        <v>1</v>
-      </c>
-      <c r="N12" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="102">
-        <v>9</v>
-      </c>
-      <c r="C13" s="102" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102">
-        <v>2</v>
-      </c>
-      <c r="G13" s="102">
-        <v>3</v>
-      </c>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="J13" s="102">
-        <v>127</v>
-      </c>
-      <c r="K13" s="109">
-        <f t="shared" si="1"/>
-        <v>15.748031496062993</v>
-      </c>
-      <c r="L13" s="109"/>
-      <c r="M13" s="109">
-        <v>1</v>
-      </c>
-      <c r="N13" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="102">
-        <v>10</v>
-      </c>
-      <c r="C14" s="102" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102">
-        <v>5400</v>
-      </c>
-      <c r="I14" s="102">
-        <f t="shared" si="0"/>
-        <v>5400</v>
-      </c>
-      <c r="J14" s="102">
-        <v>220</v>
-      </c>
-      <c r="K14" s="109">
-        <f t="shared" si="1"/>
-        <v>24.545454545454547</v>
-      </c>
-      <c r="L14" s="109"/>
-      <c r="M14" s="109">
-        <v>1</v>
-      </c>
-      <c r="N14" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="102">
-        <v>11</v>
-      </c>
-      <c r="C15" s="102" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="102">
-        <v>5400</v>
-      </c>
-      <c r="I15" s="102">
-        <f t="shared" si="0"/>
-        <v>5400</v>
-      </c>
-      <c r="J15" s="102">
-        <v>220</v>
-      </c>
-      <c r="K15" s="109">
-        <f t="shared" si="1"/>
-        <v>24.545454545454547</v>
-      </c>
-      <c r="L15" s="109"/>
-      <c r="M15" s="109">
-        <v>1</v>
-      </c>
-      <c r="N15" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="102">
-        <v>12</v>
-      </c>
-      <c r="C16" s="102" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="102">
-        <v>2625</v>
-      </c>
-      <c r="I16" s="102">
-        <f t="shared" si="0"/>
-        <v>2625</v>
-      </c>
-      <c r="J16" s="102">
-        <v>220</v>
-      </c>
-      <c r="K16" s="109">
-        <f t="shared" si="1"/>
-        <v>11.931818181818182</v>
-      </c>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109">
-        <v>1</v>
-      </c>
-      <c r="N16" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="102">
-        <v>13</v>
-      </c>
-      <c r="C17" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102">
-        <v>1650</v>
-      </c>
-      <c r="I17" s="102">
-        <f t="shared" si="0"/>
-        <v>1650</v>
-      </c>
-      <c r="J17" s="102">
-        <v>220</v>
-      </c>
-      <c r="K17" s="109">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="L17" s="109"/>
-      <c r="M17" s="109">
-        <v>1</v>
-      </c>
-      <c r="N17" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="B18" s="102">
-        <v>14</v>
-      </c>
-      <c r="C18" s="102" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="102">
-        <v>1650</v>
-      </c>
-      <c r="I18" s="102">
-        <f t="shared" si="0"/>
-        <v>1650</v>
-      </c>
-      <c r="J18" s="102">
-        <v>220</v>
-      </c>
-      <c r="K18" s="109">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="L18" s="109"/>
-      <c r="M18" s="109">
-        <v>1</v>
-      </c>
-      <c r="N18" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="102">
-        <v>15</v>
-      </c>
-      <c r="C19" s="102" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="102">
-        <v>400</v>
-      </c>
-      <c r="I19" s="102">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="J19" s="102">
-        <v>127</v>
-      </c>
-      <c r="K19" s="109">
-        <f t="shared" si="1"/>
-        <v>3.1496062992125986</v>
-      </c>
-      <c r="L19" s="109"/>
-      <c r="M19" s="109">
-        <v>1</v>
-      </c>
-      <c r="N19" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20" s="102">
-        <v>16</v>
-      </c>
-      <c r="C20" s="102" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="110">
-        <v>1760</v>
-      </c>
-      <c r="I20" s="102">
-        <f t="shared" si="0"/>
-        <v>1760</v>
-      </c>
-      <c r="J20" s="102">
-        <v>220</v>
-      </c>
-      <c r="K20" s="109">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109">
-        <v>1</v>
-      </c>
-      <c r="N20" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="B21" s="102">
-        <v>17</v>
-      </c>
-      <c r="C21" s="102" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="110">
-        <v>300</v>
-      </c>
-      <c r="I21" s="102">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="J21" s="102">
-        <v>220</v>
-      </c>
-      <c r="K21" s="109">
-        <f t="shared" si="1"/>
-        <v>1.3636363636363635</v>
-      </c>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109">
-        <v>1</v>
-      </c>
-      <c r="N21" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14">
-      <c r="B22" s="102">
-        <v>18</v>
-      </c>
-      <c r="C22" s="102" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102">
-        <v>1</v>
-      </c>
-      <c r="H22" s="110"/>
-      <c r="I22" s="102">
-        <v>600</v>
-      </c>
-      <c r="J22" s="102">
-        <v>127</v>
-      </c>
-      <c r="K22" s="109">
-        <f t="shared" si="1"/>
-        <v>4.7244094488188972</v>
-      </c>
-      <c r="L22" s="109"/>
-      <c r="M22" s="109">
-        <v>1</v>
-      </c>
-      <c r="N22" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14">
-      <c r="B23" s="102">
-        <v>19</v>
-      </c>
-      <c r="C23" s="102" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="102"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="102">
-        <v>1</v>
-      </c>
-      <c r="H23" s="110"/>
-      <c r="I23" s="102">
-        <v>600</v>
-      </c>
-      <c r="J23" s="102">
-        <v>127</v>
-      </c>
-      <c r="K23" s="109">
-        <f t="shared" si="1"/>
-        <v>4.7244094488188972</v>
-      </c>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109">
-        <v>1</v>
-      </c>
-      <c r="N23" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="102">
-        <v>20</v>
-      </c>
-      <c r="C24" s="102" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102">
-        <v>1</v>
-      </c>
-      <c r="H24" s="110"/>
-      <c r="I24" s="102">
-        <v>600</v>
-      </c>
-      <c r="J24" s="102">
-        <v>127</v>
-      </c>
-      <c r="K24" s="109">
-        <f t="shared" si="1"/>
-        <v>4.7244094488188972</v>
-      </c>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109">
-        <v>1</v>
-      </c>
-      <c r="N24" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="102">
-        <v>21</v>
-      </c>
-      <c r="C25" s="102" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102">
-        <v>1</v>
-      </c>
-      <c r="H25" s="110"/>
-      <c r="I25" s="102">
-        <v>600</v>
-      </c>
-      <c r="J25" s="102">
-        <v>127</v>
-      </c>
-      <c r="K25" s="109">
-        <f t="shared" si="1"/>
-        <v>4.7244094488188972</v>
-      </c>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109">
-        <v>1</v>
-      </c>
-      <c r="N25" s="109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="47.25" customHeight="1">
-      <c r="B28" s="112" t="s">
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="139"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="139"/>
+      <c r="K28" s="139"/>
+      <c r="L28" s="139"/>
+      <c r="M28" s="139"/>
+      <c r="N28" s="139"/>
+      <c r="O28" s="140"/>
+    </row>
+    <row r="29" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B29" s="141" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="114"/>
+      <c r="G29" s="114"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="114"/>
+      <c r="K29" s="114"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="114"/>
+      <c r="N29" s="114"/>
+      <c r="O29" s="142"/>
+    </row>
+    <row r="30" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B30" s="141" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="114"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="114"/>
+      <c r="H30" s="114"/>
+      <c r="I30" s="114"/>
+      <c r="J30" s="114"/>
+      <c r="K30" s="114"/>
+      <c r="L30" s="114"/>
+      <c r="M30" s="114"/>
+      <c r="N30" s="114"/>
+      <c r="O30" s="142"/>
+    </row>
+    <row r="31" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B31" s="141"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="114"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="114"/>
+      <c r="J31" s="114"/>
+      <c r="K31" s="114"/>
+      <c r="L31" s="114"/>
+      <c r="M31" s="114"/>
+      <c r="N31" s="114"/>
+      <c r="O31" s="142"/>
+    </row>
+    <row r="32" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B32" s="141"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="114"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="114"/>
+      <c r="J32" s="114"/>
+      <c r="K32" s="114"/>
+      <c r="L32" s="114"/>
+      <c r="M32" s="114"/>
+      <c r="N32" s="114"/>
+      <c r="O32" s="142"/>
+    </row>
+    <row r="33" spans="1:16" s="115" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B33" s="143"/>
+      <c r="C33" s="144"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="144"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
+      <c r="J33" s="144"/>
+      <c r="K33" s="144"/>
+      <c r="L33" s="144"/>
+      <c r="M33" s="144"/>
+      <c r="N33" s="144"/>
+      <c r="O33" s="145"/>
+    </row>
+    <row r="34" spans="1:16" s="115" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B34" s="125"/>
+      <c r="C34" s="125"/>
+      <c r="D34" s="125"/>
+      <c r="E34" s="125"/>
+      <c r="F34" s="125"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="125"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="125"/>
+      <c r="L34" s="125"/>
+      <c r="M34" s="125"/>
+      <c r="N34" s="125"/>
+      <c r="O34" s="125"/>
+    </row>
+    <row r="35" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A35" s="120"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="120"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="120"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="120"/>
+      <c r="L35" s="120"/>
+      <c r="M35" s="120"/>
+      <c r="N35" s="120"/>
+      <c r="O35" s="120"/>
+    </row>
+    <row r="36" spans="1:16" ht="47.25" customHeight="1">
+      <c r="A36" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="112"/>
-      <c r="D28" s="113" t="s">
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="119" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="2:14">
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="106"/>
-      <c r="I29" s="106"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="106"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="106"/>
-      <c r="N29" s="106"/>
-    </row>
-    <row r="30" spans="2:14">
-      <c r="B30" s="106" t="s">
+      <c r="E36" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="119"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="B37" s="111"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="111"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="111"/>
+      <c r="K37" s="111"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="111"/>
+      <c r="N37" s="111"/>
+    </row>
+    <row r="38" spans="1:16" ht="26.25" customHeight="1">
+      <c r="A38" s="117" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="106"/>
-      <c r="H30" s="106"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="106"/>
-      <c r="N30" s="106"/>
-    </row>
-    <row r="31" spans="2:14">
-      <c r="B31" s="106" t="s">
+      <c r="B38" s="117"/>
+      <c r="C38" s="117"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="117"/>
+      <c r="F38" s="117"/>
+      <c r="G38" s="117"/>
+      <c r="H38" s="117"/>
+      <c r="I38" s="117"/>
+      <c r="J38" s="117"/>
+      <c r="K38" s="117"/>
+      <c r="L38" s="117"/>
+      <c r="M38" s="117"/>
+      <c r="N38" s="117"/>
+    </row>
+    <row r="39" spans="1:16" ht="26.25" customHeight="1">
+      <c r="A39" s="117" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
-      <c r="H31" s="106"/>
-      <c r="I31" s="106"/>
-      <c r="J31" s="106"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="106"/>
-      <c r="M31" s="106"/>
-      <c r="N31" s="106"/>
-    </row>
-    <row r="32" spans="2:14">
-      <c r="B32" s="106"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
-      <c r="K32" s="106"/>
-      <c r="L32" s="106"/>
-      <c r="M32" s="106"/>
-      <c r="N32" s="106"/>
-    </row>
-    <row r="33" spans="2:14">
-      <c r="B33" s="106"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="106"/>
-      <c r="H33" s="106"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="106"/>
-      <c r="N33" s="106"/>
-    </row>
-    <row r="34" spans="2:14">
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="106"/>
-      <c r="H34" s="106"/>
-      <c r="I34" s="106"/>
-      <c r="J34" s="106"/>
-      <c r="K34" s="106"/>
-      <c r="L34" s="106"/>
-      <c r="M34" s="106"/>
-      <c r="N34" s="106"/>
-    </row>
-    <row r="35" spans="2:14">
-      <c r="B35" s="106"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="106"/>
-      <c r="E35" s="106"/>
-      <c r="F35" s="106"/>
-      <c r="G35" s="106"/>
-      <c r="H35" s="106"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="106"/>
-      <c r="K35" s="106"/>
-      <c r="L35" s="106"/>
-      <c r="M35" s="106"/>
-      <c r="N35" s="106"/>
-    </row>
-    <row r="36" spans="2:14">
-      <c r="B36" s="106"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="106"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="106"/>
-      <c r="G36" s="106"/>
-      <c r="H36" s="106"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="106"/>
-      <c r="K36" s="106"/>
-      <c r="L36" s="106"/>
-      <c r="M36" s="106"/>
-      <c r="N36" s="106"/>
-    </row>
-    <row r="37" spans="2:14">
-      <c r="B37" s="106"/>
-      <c r="C37" s="106"/>
-      <c r="D37" s="106"/>
-      <c r="E37" s="106"/>
-      <c r="F37" s="106"/>
-      <c r="G37" s="106"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="106"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="106"/>
-      <c r="N37" s="106"/>
-    </row>
-    <row r="38" spans="2:14">
-      <c r="B38" s="106"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="106"/>
-    </row>
-    <row r="39" spans="2:14">
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="106"/>
-    </row>
-    <row r="40" spans="2:14">
-      <c r="B40" s="106"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="106"/>
-      <c r="E40" s="106"/>
-      <c r="F40" s="106"/>
-      <c r="G40" s="106"/>
-      <c r="H40" s="106"/>
-      <c r="I40" s="106"/>
-      <c r="J40" s="106"/>
-      <c r="K40" s="106"/>
-      <c r="L40" s="106"/>
-      <c r="M40" s="106"/>
-      <c r="N40" s="106"/>
+      <c r="B39" s="117"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="117"/>
+      <c r="H39" s="117"/>
+      <c r="I39" s="117"/>
+      <c r="J39" s="117"/>
+      <c r="K39" s="117"/>
+      <c r="L39" s="117"/>
+      <c r="M39" s="117"/>
+      <c r="N39" s="117"/>
+    </row>
+    <row r="40" spans="1:16" ht="26.25">
+      <c r="B40" s="113"/>
+      <c r="C40" s="113"/>
+      <c r="D40" s="113"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113"/>
+      <c r="G40" s="113"/>
+      <c r="H40" s="113"/>
+      <c r="I40" s="113"/>
+      <c r="J40" s="113"/>
+      <c r="K40" s="113"/>
+      <c r="L40" s="113"/>
+      <c r="M40" s="113"/>
+      <c r="N40" s="113"/>
+    </row>
+    <row r="41" spans="1:16" ht="38.25" customHeight="1">
+      <c r="A41" s="116" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="116"/>
+      <c r="C41" s="116"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="116"/>
+      <c r="G41" s="116"/>
+      <c r="H41" s="116"/>
+      <c r="I41" s="116"/>
+      <c r="J41" s="116"/>
+      <c r="K41" s="116"/>
+      <c r="L41" s="116"/>
+      <c r="M41" s="116"/>
+      <c r="N41" s="121"/>
+    </row>
+    <row r="42" spans="1:16" ht="39.75" customHeight="1">
+      <c r="A42" s="116" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="116"/>
+      <c r="C42" s="116"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="116"/>
+      <c r="G42" s="116"/>
+      <c r="H42" s="116"/>
+      <c r="I42" s="116"/>
+      <c r="J42" s="116"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="112"/>
+      <c r="P42" s="112"/>
+    </row>
+    <row r="43" spans="1:16" ht="60.75" customHeight="1">
+      <c r="A43" s="116" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="116"/>
+      <c r="C43" s="116"/>
+      <c r="D43" s="116"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="116"/>
+      <c r="I43" s="116"/>
+      <c r="J43" s="116"/>
+      <c r="K43" s="116"/>
+      <c r="L43" s="116"/>
+      <c r="M43" s="116"/>
+      <c r="N43" s="116"/>
+      <c r="O43" s="112"/>
+      <c r="P43" s="112"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="111"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="111"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="111"/>
+      <c r="G44" s="111"/>
+      <c r="H44" s="111"/>
+      <c r="I44" s="111"/>
+      <c r="J44" s="111"/>
+      <c r="K44" s="111"/>
+      <c r="L44" s="111"/>
+      <c r="M44" s="111"/>
+      <c r="N44" s="111"/>
+      <c r="O44" s="112"/>
+      <c r="P44" s="112"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="111"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="111"/>
+      <c r="D45" s="111"/>
+      <c r="E45" s="111"/>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="111"/>
+      <c r="J45" s="111"/>
+      <c r="K45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="111"/>
+      <c r="N45" s="111"/>
+      <c r="O45" s="112"/>
+      <c r="P45" s="112"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="111"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="111"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="111"/>
+      <c r="F46" s="111"/>
+      <c r="G46" s="111"/>
+      <c r="H46" s="111"/>
+      <c r="I46" s="111"/>
+      <c r="J46" s="111"/>
+      <c r="K46" s="111"/>
+      <c r="L46" s="111"/>
+      <c r="M46" s="111"/>
+      <c r="N46" s="111"/>
+      <c r="O46" s="112"/>
+      <c r="P46" s="112"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="111"/>
+      <c r="B47" s="111"/>
+      <c r="C47" s="111"/>
+      <c r="D47" s="111"/>
+      <c r="E47" s="111"/>
+      <c r="F47" s="111"/>
+      <c r="G47" s="111"/>
+      <c r="H47" s="111"/>
+      <c r="I47" s="111"/>
+      <c r="J47" s="111"/>
+      <c r="K47" s="111"/>
+      <c r="L47" s="111"/>
+      <c r="M47" s="111"/>
+      <c r="N47" s="111"/>
+      <c r="O47" s="112"/>
+      <c r="P47" s="112"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="111"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="111"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="111"/>
+      <c r="G48" s="111"/>
+      <c r="H48" s="111"/>
+      <c r="I48" s="111"/>
+      <c r="J48" s="111"/>
+      <c r="K48" s="111"/>
+      <c r="L48" s="111"/>
+      <c r="M48" s="111"/>
+      <c r="N48" s="111"/>
+      <c r="O48" s="112"/>
+      <c r="P48" s="112"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="111"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="111"/>
+      <c r="F49" s="111"/>
+      <c r="G49" s="111"/>
+      <c r="H49" s="111"/>
+      <c r="I49" s="111"/>
+      <c r="J49" s="111"/>
+      <c r="K49" s="111"/>
+      <c r="L49" s="111"/>
+      <c r="M49" s="111"/>
+      <c r="N49" s="111"/>
+      <c r="O49" s="112"/>
+      <c r="P49" s="112"/>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="111"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
+      <c r="K50" s="111"/>
+      <c r="L50" s="111"/>
+      <c r="M50" s="111"/>
+      <c r="N50" s="111"/>
+      <c r="O50" s="112"/>
+      <c r="P50" s="112"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="111"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="111"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="111"/>
+      <c r="F51" s="111"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="111"/>
+      <c r="K51" s="111"/>
+      <c r="L51" s="111"/>
+      <c r="M51" s="111"/>
+      <c r="N51" s="111"/>
+      <c r="O51" s="112"/>
+      <c r="P51" s="112"/>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="111"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="111"/>
+      <c r="D52" s="111"/>
+      <c r="E52" s="111"/>
+      <c r="F52" s="111"/>
+      <c r="G52" s="111"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="111"/>
+      <c r="J52" s="111"/>
+      <c r="K52" s="111"/>
+      <c r="L52" s="111"/>
+      <c r="M52" s="111"/>
+      <c r="N52" s="111"/>
+      <c r="O52" s="112"/>
+      <c r="P52" s="112"/>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="111"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="111"/>
+      <c r="D53" s="111"/>
+      <c r="E53" s="111"/>
+      <c r="F53" s="111"/>
+      <c r="G53" s="111"/>
+      <c r="H53" s="111"/>
+      <c r="I53" s="111"/>
+      <c r="J53" s="111"/>
+      <c r="K53" s="111"/>
+      <c r="L53" s="111"/>
+      <c r="M53" s="111"/>
+      <c r="N53" s="111"/>
+      <c r="O53" s="112"/>
+      <c r="P53" s="112"/>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" s="111"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="111"/>
+      <c r="D54" s="111"/>
+      <c r="E54" s="111"/>
+      <c r="F54" s="111"/>
+      <c r="G54" s="111"/>
+      <c r="H54" s="111"/>
+      <c r="I54" s="111"/>
+      <c r="J54" s="111"/>
+      <c r="K54" s="111"/>
+      <c r="L54" s="111"/>
+      <c r="M54" s="111"/>
+      <c r="N54" s="111"/>
+      <c r="O54" s="112"/>
+      <c r="P54" s="112"/>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="111"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="111"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="111"/>
+      <c r="F55" s="111"/>
+      <c r="G55" s="111"/>
+      <c r="H55" s="111"/>
+      <c r="I55" s="111"/>
+      <c r="J55" s="111"/>
+      <c r="K55" s="111"/>
+      <c r="L55" s="111"/>
+      <c r="M55" s="111"/>
+      <c r="N55" s="111"/>
+      <c r="O55" s="112"/>
+      <c r="P55" s="112"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="111"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="111"/>
+      <c r="D56" s="111"/>
+      <c r="E56" s="111"/>
+      <c r="F56" s="111"/>
+      <c r="G56" s="111"/>
+      <c r="H56" s="111"/>
+      <c r="I56" s="111"/>
+      <c r="J56" s="111"/>
+      <c r="K56" s="111"/>
+      <c r="L56" s="111"/>
+      <c r="M56" s="111"/>
+      <c r="N56" s="111"/>
+      <c r="O56" s="112"/>
+      <c r="P56" s="112"/>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" s="111"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="111"/>
+      <c r="D57" s="111"/>
+      <c r="E57" s="111"/>
+      <c r="F57" s="111"/>
+      <c r="G57" s="111"/>
+      <c r="H57" s="111"/>
+      <c r="I57" s="111"/>
+      <c r="J57" s="111"/>
+      <c r="K57" s="111"/>
+      <c r="L57" s="111"/>
+      <c r="M57" s="111"/>
+      <c r="N57" s="111"/>
+      <c r="O57" s="112"/>
+      <c r="P57" s="112"/>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" s="111"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="111"/>
+      <c r="D58" s="111"/>
+      <c r="E58" s="111"/>
+      <c r="F58" s="111"/>
+      <c r="G58" s="111"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="111"/>
+      <c r="K58" s="111"/>
+      <c r="L58" s="111"/>
+      <c r="M58" s="111"/>
+      <c r="N58" s="111"/>
+      <c r="O58" s="112"/>
+      <c r="P58" s="112"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="111"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="111"/>
+      <c r="D59" s="111"/>
+      <c r="E59" s="111"/>
+      <c r="F59" s="111"/>
+      <c r="G59" s="111"/>
+      <c r="H59" s="111"/>
+      <c r="I59" s="111"/>
+      <c r="J59" s="111"/>
+      <c r="K59" s="111"/>
+      <c r="L59" s="111"/>
+      <c r="M59" s="111"/>
+      <c r="N59" s="111"/>
+      <c r="O59" s="112"/>
+      <c r="P59" s="112"/>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" s="112"/>
+      <c r="B60" s="112"/>
+      <c r="C60" s="112"/>
+      <c r="D60" s="112"/>
+      <c r="E60" s="112"/>
+      <c r="F60" s="112"/>
+      <c r="G60" s="112"/>
+      <c r="H60" s="112"/>
+      <c r="I60" s="112"/>
+      <c r="J60" s="112"/>
+      <c r="K60" s="112"/>
+      <c r="L60" s="112"/>
+      <c r="M60" s="112"/>
+      <c r="N60" s="112"/>
+      <c r="O60" s="112"/>
+      <c r="P60" s="112"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B40:N40"/>
-    <mergeCell ref="B34:N34"/>
-    <mergeCell ref="B35:N35"/>
-    <mergeCell ref="B36:N36"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="B38:N38"/>
-    <mergeCell ref="B39:N39"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B30:N30"/>
-    <mergeCell ref="B31:N31"/>
-    <mergeCell ref="B32:N32"/>
-    <mergeCell ref="B33:N33"/>
+  <mergeCells count="43">
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B31:O31"/>
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="B33:O33"/>
+    <mergeCell ref="B28:O28"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="A41:M41"/>
+    <mergeCell ref="A38:N38"/>
+    <mergeCell ref="A39:N39"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="A55:N55"/>
+    <mergeCell ref="A56:N56"/>
+    <mergeCell ref="A57:N57"/>
+    <mergeCell ref="A58:N58"/>
+    <mergeCell ref="A59:N59"/>
+    <mergeCell ref="A50:N50"/>
+    <mergeCell ref="A51:N51"/>
+    <mergeCell ref="A52:N52"/>
+    <mergeCell ref="A53:N53"/>
+    <mergeCell ref="A54:N54"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="B1:B4"/>
@@ -46199,7 +47216,34 @@
     <mergeCell ref="D1:E3"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:H3"/>
+    <mergeCell ref="A42:N42"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="A43:N43"/>
+    <mergeCell ref="A44:N44"/>
+    <mergeCell ref="A45:N45"/>
+    <mergeCell ref="A46:N46"/>
+    <mergeCell ref="A47:N47"/>
+    <mergeCell ref="A48:N48"/>
+    <mergeCell ref="A49:N49"/>
   </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE09EFEF-EC0B-4984-B180-595A6EF1BBAD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="20.7109375" style="51"/>
+  </cols>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
leia os commits anteriores
</commit_message>
<xml_diff>
--- a/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
+++ b/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\GitHub\Instel-I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\UFES\GitHub\Instel-I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD629833-662B-48D6-BD96-1F4358C3A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9D2E8A-B620-42EC-BC7D-0F2127962940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação_Informações" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="137">
   <si>
     <t>Alunos: Gabriel Schettino Lucas e Ramon Rodrigues Morello</t>
   </si>
@@ -532,12 +532,21 @@
   <si>
     <t>[IC']:  Capacidade de corrente que será usada para dimensionar eletrodutos</t>
   </si>
+  <si>
+    <t>OBSERVAÇÕES</t>
+  </si>
+  <si>
+    <t>1) O cálculo do método "limte de queda de tensão" utilizará a corrente de projeto já calculada na planinha "Capacidade de Corrente", as colunas estão relacionadas!</t>
+  </si>
+  <si>
+    <t>2) No projeto um circuito pode estar passando por mais de um caminho, logo nesse cálculo será considerado o pior dos caminhos que o circuito está fazendo.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,6 +691,14 @@
     <font>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1375,7 +1392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1547,35 +1564,59 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1588,34 +1629,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1630,18 +1682,22 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1665,19 +1721,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1689,44 +1757,8 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1746,28 +1778,28 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2001,14 +2033,14 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="76"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2031,14 +2063,14 @@
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2089,16 +2121,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="78" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="60"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="79"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2121,17 +2153,17 @@
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="60"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2157,17 +2189,17 @@
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="60"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="60"/>
+      <c r="F6" s="79"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2193,17 +2225,17 @@
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="60"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="60"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
@@ -2229,15 +2261,15 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="79"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4"/>
@@ -2261,15 +2293,15 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="59"/>
-      <c r="F9" s="60"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="79"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="4"/>
@@ -2293,15 +2325,15 @@
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="82" t="s">
+      <c r="C10" s="73"/>
+      <c r="D10" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="4"/>
@@ -2325,11 +2357,11 @@
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="79"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="4"/>
@@ -2353,11 +2385,11 @@
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2381,11 +2413,11 @@
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="68"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92"/>
       <c r="G13" s="7"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2409,11 +2441,11 @@
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="79"/>
       <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2493,14 +2525,14 @@
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="73"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2523,14 +2555,14 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="63"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="88"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2553,14 +2585,14 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="63"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="88"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2583,14 +2615,14 @@
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="63"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="88"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2613,14 +2645,14 @@
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="63"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="88"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2643,14 +2675,14 @@
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="63"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="88"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2673,12 +2705,12 @@
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="63"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="88"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2701,14 +2733,14 @@
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="75"/>
       <c r="H24" s="1"/>
       <c r="I24" s="8"/>
       <c r="J24" s="1"/>
@@ -9107,24 +9139,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
@@ -9139,6 +9153,24 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -9192,19 +9224,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="71"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="73"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -9222,17 +9254,17 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="66"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="75"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -9250,27 +9282,27 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="94" t="s">
+      <c r="D4" s="79"/>
+      <c r="E4" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="95" t="s">
+      <c r="F4" s="85"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="79"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="95" t="s">
+      <c r="I4" s="85"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="60"/>
+      <c r="L4" s="79"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -9288,7 +9320,7 @@
     </row>
     <row r="5" spans="1:26" ht="39.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="83"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
@@ -9436,35 +9468,35 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="101">
+      <c r="C8" s="104">
         <v>17.579999999999998</v>
       </c>
-      <c r="D8" s="101">
+      <c r="D8" s="104">
         <v>23.9</v>
       </c>
-      <c r="E8" s="87">
+      <c r="E8" s="100">
         <v>3</v>
       </c>
-      <c r="F8" s="87">
+      <c r="F8" s="100">
         <v>100</v>
       </c>
-      <c r="G8" s="97">
+      <c r="G8" s="98">
         <v>300</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="98">
         <v>4</v>
       </c>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="87">
+      <c r="J8" s="100">
         <v>200</v>
       </c>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -9482,17 +9514,17 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="100"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -10105,9 +10137,9 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="89"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -10125,13 +10157,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -10190,9 +10222,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -10210,20 +10242,20 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="96" t="s">
+      <c r="B26" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="85"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="84"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="109"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -10248,10 +10280,10 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -10276,12 +10308,12 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="91"/>
-      <c r="N28" s="62"/>
-      <c r="O28" s="62"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="114"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -10304,12 +10336,12 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="85"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="62"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -10332,10 +10364,10 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="85"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="84"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="109"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -10360,10 +10392,10 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="85"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="87"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -10388,9 +10420,9 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="62"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -10416,9 +10448,9 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
+      <c r="J33" s="87"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="87"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -10444,9 +10476,9 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -16614,23 +16646,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:L4"/>
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="J32:L34"/>
@@ -16645,6 +16660,23 @@
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="M30:M31"/>
     <mergeCell ref="J31:L31"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B23:F23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16726,20 +16758,20 @@
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="106"/>
-      <c r="F3" s="105" t="s">
+      <c r="E3" s="119"/>
+      <c r="F3" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="106"/>
+      <c r="G3" s="119"/>
       <c r="H3" s="30" t="s">
         <v>30</v>
       </c>
@@ -16770,8 +16802,8 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="104"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="32" t="s">
         <v>72</v>
       </c>
@@ -45204,20 +45236,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="109" t="s">
+      <c r="D4" s="122" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="110"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="123"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="53">
@@ -45465,8 +45497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36D55B-3867-4EF4-9271-23288EED3B45}">
   <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -45484,90 +45516,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="132" t="s">
+      <c r="D1" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="133"/>
-      <c r="F1" s="132" t="s">
+      <c r="E1" s="138"/>
+      <c r="F1" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="133"/>
-      <c r="H1" s="129" t="s">
+      <c r="G1" s="138"/>
+      <c r="H1" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="107" t="s">
+      <c r="I1" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="107" t="s">
+      <c r="J1" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="109" t="s">
+      <c r="K1" s="122" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="109" t="s">
+      <c r="L1" s="122" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="109" t="s">
+      <c r="M1" s="122" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="109" t="s">
+      <c r="N1" s="122" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="109" t="s">
+      <c r="O1" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="P1" s="109" t="s">
+      <c r="P1" s="122" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" s="109" t="s">
+      <c r="Q1" s="122" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" spans="2:17">
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
     </row>
     <row r="3" spans="2:17" ht="31.5" customHeight="1">
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="122"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="107"/>
-      <c r="C4" s="107"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="52" t="s">
         <v>72</v>
       </c>
@@ -45628,14 +45660,14 @@
       <c r="G5" s="53"/>
       <c r="H5" s="53"/>
       <c r="I5" s="53">
-        <f>(D5*100+E5*200)+(F5*100+G5*600)+H5</f>
+        <f t="shared" ref="I5:I21" si="0">(D5*100+E5*200)+(F5*100+G5*600)+H5</f>
         <v>1200</v>
       </c>
       <c r="J5" s="53">
         <v>127</v>
       </c>
       <c r="K5" s="56">
-        <f t="shared" ref="K5:K25" si="0">I5/J5</f>
+        <f t="shared" ref="K5:K25" si="1">I5/J5</f>
         <v>9.4488188976377945</v>
       </c>
       <c r="L5" s="56">
@@ -45675,14 +45707,14 @@
       <c r="G6" s="53"/>
       <c r="H6" s="53"/>
       <c r="I6" s="53">
-        <f>(D6*100+E6*200)+(F6*100+G6*600)+H6</f>
+        <f t="shared" si="0"/>
         <v>1700</v>
       </c>
       <c r="J6" s="53">
         <v>127</v>
       </c>
       <c r="K6" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.385826771653543</v>
       </c>
       <c r="L6" s="56">
@@ -45722,14 +45754,14 @@
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53">
-        <f>(D7*100+E7*200)+(F7*100+G7*600)+H7</f>
+        <f t="shared" si="0"/>
         <v>2100</v>
       </c>
       <c r="J7" s="53">
         <v>127</v>
       </c>
       <c r="K7" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.535433070866141</v>
       </c>
       <c r="L7" s="56">
@@ -45742,7 +45774,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="56">
-        <f t="shared" ref="O7:O25" si="1">K7/L7*M7*N7</f>
+        <f t="shared" ref="O7:O25" si="2">K7/L7*M7*N7</f>
         <v>27.559055118110237</v>
       </c>
       <c r="P7" s="56">
@@ -45769,14 +45801,14 @@
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53">
-        <f>(D8*100+E8*200)+(F8*100+G8*600)+H8</f>
+        <f t="shared" si="0"/>
         <v>1900</v>
       </c>
       <c r="J8" s="53">
         <v>127</v>
       </c>
       <c r="K8" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.960629921259843</v>
       </c>
       <c r="L8" s="56">
@@ -45789,7 +45821,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.934383202099738</v>
       </c>
       <c r="P8" s="56">
@@ -45816,14 +45848,14 @@
       </c>
       <c r="H9" s="53"/>
       <c r="I9" s="53">
-        <f>(D9*100+E9*200)+(F9*100+G9*600)+H9</f>
+        <f t="shared" si="0"/>
         <v>1900</v>
       </c>
       <c r="J9" s="53">
         <v>127</v>
       </c>
       <c r="K9" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.960629921259843</v>
       </c>
       <c r="L9" s="56">
@@ -45836,7 +45868,7 @@
         <v>1</v>
       </c>
       <c r="O9" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.934383202099738</v>
       </c>
       <c r="P9" s="56">
@@ -45863,14 +45895,14 @@
       </c>
       <c r="H10" s="53"/>
       <c r="I10" s="53">
-        <f>(D10*100+E10*200)+(F10*100+G10*600)+H10</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="J10" s="53">
         <v>127</v>
       </c>
       <c r="K10" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.685039370078741</v>
       </c>
       <c r="L10" s="56">
@@ -45883,7 +45915,7 @@
         <v>1</v>
       </c>
       <c r="O10" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.808398950131235</v>
       </c>
       <c r="P10" s="56">
@@ -45910,14 +45942,14 @@
       </c>
       <c r="H11" s="53"/>
       <c r="I11" s="53">
-        <f>(D11*100+E11*200)+(F11*100+G11*600)+H11</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="J11" s="53">
         <v>127</v>
       </c>
       <c r="K11" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
       <c r="L11" s="56">
@@ -45930,7 +45962,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.227740763173834</v>
       </c>
       <c r="P11" s="56">
@@ -45957,14 +45989,14 @@
       </c>
       <c r="H12" s="53"/>
       <c r="I12" s="53">
-        <f>(D12*100+E12*200)+(F12*100+G12*600)+H12</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="J12" s="53">
         <v>127</v>
       </c>
       <c r="K12" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
       <c r="L12" s="56">
@@ -45977,7 +46009,7 @@
         <v>1</v>
       </c>
       <c r="O12" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26.246719160104988</v>
       </c>
       <c r="P12" s="56">
@@ -46004,14 +46036,14 @@
       </c>
       <c r="H13" s="53"/>
       <c r="I13" s="53">
-        <f>(D13*100+E13*200)+(F13*100+G13*600)+H13</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="J13" s="53">
         <v>127</v>
       </c>
       <c r="K13" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.748031496062993</v>
       </c>
       <c r="L13" s="56">
@@ -46024,7 +46056,7 @@
         <v>1</v>
       </c>
       <c r="O13" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.227740763173834</v>
       </c>
       <c r="P13" s="56">
@@ -46049,14 +46081,14 @@
         <v>5400</v>
       </c>
       <c r="I14" s="53">
-        <f>(D14*100+E14*200)+(F14*100+G14*600)+H14</f>
+        <f t="shared" si="0"/>
         <v>5400</v>
       </c>
       <c r="J14" s="53">
         <v>220</v>
       </c>
       <c r="K14" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.545454545454547</v>
       </c>
       <c r="L14" s="56">
@@ -46069,7 +46101,7 @@
         <v>1</v>
       </c>
       <c r="O14" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.909090909090914</v>
       </c>
       <c r="P14" s="56">
@@ -46094,14 +46126,14 @@
         <v>5400</v>
       </c>
       <c r="I15" s="53">
-        <f>(D15*100+E15*200)+(F15*100+G15*600)+H15</f>
+        <f t="shared" si="0"/>
         <v>5400</v>
       </c>
       <c r="J15" s="53">
         <v>220</v>
       </c>
       <c r="K15" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.545454545454547</v>
       </c>
       <c r="L15" s="56">
@@ -46114,7 +46146,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.909090909090914</v>
       </c>
       <c r="P15" s="56">
@@ -46139,14 +46171,14 @@
         <v>2625</v>
       </c>
       <c r="I16" s="53">
-        <f>(D16*100+E16*200)+(F16*100+G16*600)+H16</f>
+        <f t="shared" si="0"/>
         <v>2625</v>
       </c>
       <c r="J16" s="53">
         <v>220</v>
       </c>
       <c r="K16" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.931818181818182</v>
       </c>
       <c r="L16" s="56">
@@ -46159,7 +46191,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.886363636363637</v>
       </c>
       <c r="P16" s="56">
@@ -46184,14 +46216,14 @@
         <v>1650</v>
       </c>
       <c r="I17" s="53">
-        <f>(D17*100+E17*200)+(F17*100+G17*600)+H17</f>
+        <f t="shared" si="0"/>
         <v>1650</v>
       </c>
       <c r="J17" s="53">
         <v>220</v>
       </c>
       <c r="K17" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="L17" s="56">
@@ -46204,16 +46236,16 @@
         <v>1</v>
       </c>
       <c r="O17" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="P17" s="56">
         <v>15.5</v>
       </c>
-      <c r="Q17" s="126">
+      <c r="Q17" s="69">
         <v>1.5</v>
       </c>
-      <c r="R17" s="127" t="s">
+      <c r="R17" s="70" t="s">
         <v>132</v>
       </c>
     </row>
@@ -46232,14 +46264,14 @@
         <v>1650</v>
       </c>
       <c r="I18" s="53">
-        <f>(D18*100+E18*200)+(F18*100+G18*600)+H18</f>
+        <f t="shared" si="0"/>
         <v>1650</v>
       </c>
       <c r="J18" s="53">
         <v>220</v>
       </c>
       <c r="K18" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="L18" s="56">
@@ -46252,13 +46284,13 @@
         <v>1</v>
       </c>
       <c r="O18" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.538461538461538</v>
       </c>
       <c r="P18" s="56">
         <v>12</v>
       </c>
-      <c r="Q18" s="128">
+      <c r="Q18" s="71">
         <v>1</v>
       </c>
     </row>
@@ -46277,14 +46309,14 @@
         <v>400</v>
       </c>
       <c r="I19" s="53">
-        <f>(D19*100+E19*200)+(F19*100+G19*600)+H19</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="J19" s="53">
         <v>127</v>
       </c>
       <c r="K19" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1496062992125986</v>
       </c>
       <c r="L19" s="56">
@@ -46297,13 +46329,13 @@
         <v>1</v>
       </c>
       <c r="O19" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2493438320209975</v>
       </c>
       <c r="P19" s="56">
         <v>8</v>
       </c>
-      <c r="Q19" s="128">
+      <c r="Q19" s="71">
         <v>0.5</v>
       </c>
     </row>
@@ -46322,14 +46354,14 @@
         <v>1760</v>
       </c>
       <c r="I20" s="53">
-        <f>(D20*100+E20*200)+(F20*100+G20*600)+H20</f>
+        <f t="shared" si="0"/>
         <v>1760</v>
       </c>
       <c r="J20" s="53">
         <v>220</v>
       </c>
       <c r="K20" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L20" s="56">
@@ -46342,13 +46374,13 @@
         <v>1</v>
       </c>
       <c r="O20" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
       <c r="P20" s="56">
         <v>15.5</v>
       </c>
-      <c r="Q20" s="128">
+      <c r="Q20" s="71">
         <v>1.5</v>
       </c>
     </row>
@@ -46367,14 +46399,14 @@
         <v>300</v>
       </c>
       <c r="I21" s="53">
-        <f>(D21*100+E21*200)+(F21*100+G21*600)+H21</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="J21" s="53">
         <v>220</v>
       </c>
       <c r="K21" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3636363636363635</v>
       </c>
       <c r="L21" s="56">
@@ -46387,13 +46419,13 @@
         <v>1</v>
       </c>
       <c r="O21" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0979020979020975</v>
       </c>
       <c r="P21" s="56">
         <v>8</v>
       </c>
-      <c r="Q21" s="128">
+      <c r="Q21" s="71">
         <v>0.5</v>
       </c>
     </row>
@@ -46418,7 +46450,7 @@
         <v>127</v>
       </c>
       <c r="K22" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7244094488188972</v>
       </c>
       <c r="L22" s="56">
@@ -46431,7 +46463,7 @@
         <v>1</v>
       </c>
       <c r="O22" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2884376295068378</v>
       </c>
       <c r="P22" s="56">
@@ -46462,7 +46494,7 @@
         <v>127</v>
       </c>
       <c r="K23" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7244094488188972</v>
       </c>
       <c r="L23" s="56">
@@ -46475,7 +46507,7 @@
         <v>1</v>
       </c>
       <c r="O23" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2884376295068378</v>
       </c>
       <c r="P23" s="56">
@@ -46506,7 +46538,7 @@
         <v>127</v>
       </c>
       <c r="K24" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7244094488188972</v>
       </c>
       <c r="L24" s="56">
@@ -46519,7 +46551,7 @@
         <v>1</v>
       </c>
       <c r="O24" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2884376295068378</v>
       </c>
       <c r="P24" s="56">
@@ -46550,7 +46582,7 @@
         <v>127</v>
       </c>
       <c r="K25" s="56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7244094488188972</v>
       </c>
       <c r="L25" s="56">
@@ -46563,7 +46595,7 @@
         <v>1</v>
       </c>
       <c r="O25" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2884376295068378</v>
       </c>
       <c r="P25" s="56">
@@ -46574,637 +46606,638 @@
       </c>
     </row>
     <row r="26" spans="2:18">
-      <c r="B26" s="122">
+      <c r="B26" s="65">
         <v>22</v>
       </c>
-      <c r="C26" s="122" t="s">
+      <c r="C26" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="122"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="123"/>
-      <c r="I26" s="122">
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="65">
         <f>SUM(I5:I25)</f>
         <v>38885</v>
       </c>
-      <c r="J26" s="122"/>
-      <c r="K26" s="124"/>
-      <c r="L26" s="124"/>
-      <c r="M26" s="124"/>
-      <c r="N26" s="124"/>
-      <c r="O26" s="124"/>
-      <c r="P26" s="124"/>
-      <c r="Q26" s="124"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
+      <c r="P26" s="67"/>
+      <c r="Q26" s="67"/>
     </row>
     <row r="28" spans="2:18" ht="31.5" customHeight="1">
-      <c r="B28" s="138" t="s">
+      <c r="B28" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="139"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="139"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="139"/>
-      <c r="H28" s="139"/>
-      <c r="I28" s="139"/>
-      <c r="J28" s="139"/>
-      <c r="K28" s="139"/>
-      <c r="L28" s="139"/>
-      <c r="M28" s="139"/>
-      <c r="N28" s="139"/>
-      <c r="O28" s="140"/>
-    </row>
-    <row r="29" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B29" s="141" t="s">
+      <c r="C28" s="131"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="131"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="131"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="131"/>
+      <c r="N28" s="131"/>
+      <c r="O28" s="132"/>
+    </row>
+    <row r="29" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B29" s="124" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="114"/>
-      <c r="D29" s="114"/>
-      <c r="E29" s="114"/>
-      <c r="F29" s="114"/>
-      <c r="G29" s="114"/>
-      <c r="H29" s="114"/>
-      <c r="I29" s="114"/>
-      <c r="J29" s="114"/>
-      <c r="K29" s="114"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="114"/>
-      <c r="N29" s="114"/>
-      <c r="O29" s="142"/>
-    </row>
-    <row r="30" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B30" s="141" t="s">
+      <c r="C29" s="125"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="125"/>
+      <c r="F29" s="125"/>
+      <c r="G29" s="125"/>
+      <c r="H29" s="125"/>
+      <c r="I29" s="125"/>
+      <c r="J29" s="125"/>
+      <c r="K29" s="125"/>
+      <c r="L29" s="125"/>
+      <c r="M29" s="125"/>
+      <c r="N29" s="125"/>
+      <c r="O29" s="126"/>
+    </row>
+    <row r="30" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B30" s="124" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="114"/>
-      <c r="L30" s="114"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="114"/>
-      <c r="O30" s="142"/>
-    </row>
-    <row r="31" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B31" s="141"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114"/>
-      <c r="L31" s="114"/>
-      <c r="M31" s="114"/>
-      <c r="N31" s="114"/>
-      <c r="O31" s="142"/>
-    </row>
-    <row r="32" spans="2:18" s="115" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B32" s="141"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-      <c r="G32" s="114"/>
-      <c r="H32" s="114"/>
-      <c r="I32" s="114"/>
-      <c r="J32" s="114"/>
-      <c r="K32" s="114"/>
-      <c r="L32" s="114"/>
-      <c r="M32" s="114"/>
-      <c r="N32" s="114"/>
-      <c r="O32" s="142"/>
-    </row>
-    <row r="33" spans="1:16" s="115" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B33" s="143"/>
-      <c r="C33" s="144"/>
-      <c r="D33" s="144"/>
-      <c r="E33" s="144"/>
-      <c r="F33" s="144"/>
-      <c r="G33" s="144"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
-      <c r="J33" s="144"/>
-      <c r="K33" s="144"/>
-      <c r="L33" s="144"/>
-      <c r="M33" s="144"/>
-      <c r="N33" s="144"/>
-      <c r="O33" s="145"/>
-    </row>
-    <row r="34" spans="1:16" s="115" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B34" s="125"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="125"/>
-      <c r="I34" s="125"/>
-      <c r="J34" s="125"/>
-      <c r="K34" s="125"/>
-      <c r="L34" s="125"/>
-      <c r="M34" s="125"/>
-      <c r="N34" s="125"/>
-      <c r="O34" s="125"/>
+      <c r="C30" s="125"/>
+      <c r="D30" s="125"/>
+      <c r="E30" s="125"/>
+      <c r="F30" s="125"/>
+      <c r="G30" s="125"/>
+      <c r="H30" s="125"/>
+      <c r="I30" s="125"/>
+      <c r="J30" s="125"/>
+      <c r="K30" s="125"/>
+      <c r="L30" s="125"/>
+      <c r="M30" s="125"/>
+      <c r="N30" s="125"/>
+      <c r="O30" s="126"/>
+    </row>
+    <row r="31" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B31" s="124"/>
+      <c r="C31" s="125"/>
+      <c r="D31" s="125"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="125"/>
+      <c r="G31" s="125"/>
+      <c r="H31" s="125"/>
+      <c r="I31" s="125"/>
+      <c r="J31" s="125"/>
+      <c r="K31" s="125"/>
+      <c r="L31" s="125"/>
+      <c r="M31" s="125"/>
+      <c r="N31" s="125"/>
+      <c r="O31" s="126"/>
+    </row>
+    <row r="32" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B32" s="124"/>
+      <c r="C32" s="125"/>
+      <c r="D32" s="125"/>
+      <c r="E32" s="125"/>
+      <c r="F32" s="125"/>
+      <c r="G32" s="125"/>
+      <c r="H32" s="125"/>
+      <c r="I32" s="125"/>
+      <c r="J32" s="125"/>
+      <c r="K32" s="125"/>
+      <c r="L32" s="125"/>
+      <c r="M32" s="125"/>
+      <c r="N32" s="125"/>
+      <c r="O32" s="126"/>
+    </row>
+    <row r="33" spans="1:16" s="61" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B33" s="127"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="128"/>
+      <c r="K33" s="128"/>
+      <c r="L33" s="128"/>
+      <c r="M33" s="128"/>
+      <c r="N33" s="128"/>
+      <c r="O33" s="129"/>
+    </row>
+    <row r="34" spans="1:16" s="61" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="68"/>
+      <c r="O34" s="68"/>
     </row>
     <row r="35" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A35" s="120"/>
-      <c r="B35" s="120"/>
-      <c r="C35" s="120"/>
-      <c r="D35" s="120"/>
-      <c r="E35" s="120"/>
-      <c r="F35" s="120"/>
-      <c r="G35" s="120"/>
-      <c r="H35" s="120"/>
-      <c r="I35" s="120"/>
-      <c r="J35" s="120"/>
-      <c r="K35" s="120"/>
-      <c r="L35" s="120"/>
-      <c r="M35" s="120"/>
-      <c r="N35" s="120"/>
-      <c r="O35" s="120"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="64"/>
     </row>
     <row r="36" spans="1:16" ht="47.25" customHeight="1">
-      <c r="A36" s="118" t="s">
+      <c r="A36" s="135" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="118"/>
-      <c r="C36" s="118"/>
-      <c r="D36" s="119" t="s">
+      <c r="B36" s="135"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="119" t="s">
+      <c r="E36" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="F36" s="119" t="s">
+      <c r="F36" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="G36" s="119"/>
+      <c r="G36" s="63"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-      <c r="L37" s="111"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="111"/>
+      <c r="B37" s="136"/>
+      <c r="C37" s="136"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="136"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="136"/>
+      <c r="H37" s="136"/>
+      <c r="I37" s="136"/>
+      <c r="J37" s="136"/>
+      <c r="K37" s="136"/>
+      <c r="L37" s="136"/>
+      <c r="M37" s="136"/>
+      <c r="N37" s="136"/>
     </row>
     <row r="38" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A38" s="117" t="s">
+      <c r="A38" s="134" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="117"/>
-      <c r="C38" s="117"/>
-      <c r="D38" s="117"/>
-      <c r="E38" s="117"/>
-      <c r="F38" s="117"/>
-      <c r="G38" s="117"/>
-      <c r="H38" s="117"/>
-      <c r="I38" s="117"/>
-      <c r="J38" s="117"/>
-      <c r="K38" s="117"/>
-      <c r="L38" s="117"/>
-      <c r="M38" s="117"/>
-      <c r="N38" s="117"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="134"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="134"/>
+      <c r="G38" s="134"/>
+      <c r="H38" s="134"/>
+      <c r="I38" s="134"/>
+      <c r="J38" s="134"/>
+      <c r="K38" s="134"/>
+      <c r="L38" s="134"/>
+      <c r="M38" s="134"/>
+      <c r="N38" s="134"/>
     </row>
     <row r="39" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A39" s="117" t="s">
+      <c r="A39" s="134" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="117"/>
-      <c r="C39" s="117"/>
-      <c r="D39" s="117"/>
-      <c r="E39" s="117"/>
-      <c r="F39" s="117"/>
-      <c r="G39" s="117"/>
-      <c r="H39" s="117"/>
-      <c r="I39" s="117"/>
-      <c r="J39" s="117"/>
-      <c r="K39" s="117"/>
-      <c r="L39" s="117"/>
-      <c r="M39" s="117"/>
-      <c r="N39" s="117"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="134"/>
+      <c r="G39" s="134"/>
+      <c r="H39" s="134"/>
+      <c r="I39" s="134"/>
+      <c r="J39" s="134"/>
+      <c r="K39" s="134"/>
+      <c r="L39" s="134"/>
+      <c r="M39" s="134"/>
+      <c r="N39" s="134"/>
     </row>
     <row r="40" spans="1:16" ht="26.25">
-      <c r="B40" s="113"/>
-      <c r="C40" s="113"/>
-      <c r="D40" s="113"/>
-      <c r="E40" s="113"/>
-      <c r="F40" s="113"/>
-      <c r="G40" s="113"/>
-      <c r="H40" s="113"/>
-      <c r="I40" s="113"/>
-      <c r="J40" s="113"/>
-      <c r="K40" s="113"/>
-      <c r="L40" s="113"/>
-      <c r="M40" s="113"/>
-      <c r="N40" s="113"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="60"/>
+      <c r="K40" s="60"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
     </row>
     <row r="41" spans="1:16" ht="38.25" customHeight="1">
-      <c r="A41" s="116" t="s">
+      <c r="A41" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="116"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="116"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="116"/>
-      <c r="H41" s="116"/>
-      <c r="I41" s="116"/>
-      <c r="J41" s="116"/>
-      <c r="K41" s="116"/>
-      <c r="L41" s="116"/>
-      <c r="M41" s="116"/>
-      <c r="N41" s="121"/>
+      <c r="B41" s="133"/>
+      <c r="C41" s="133"/>
+      <c r="D41" s="133"/>
+      <c r="E41" s="133"/>
+      <c r="F41" s="133"/>
+      <c r="G41" s="133"/>
+      <c r="H41" s="133"/>
+      <c r="I41" s="133"/>
+      <c r="J41" s="133"/>
+      <c r="K41" s="133"/>
+      <c r="L41" s="133"/>
+      <c r="M41" s="133"/>
+      <c r="N41" s="62"/>
     </row>
     <row r="42" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A42" s="116" t="s">
+      <c r="A42" s="133" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="116"/>
-      <c r="C42" s="116"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="116"/>
-      <c r="G42" s="116"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="116"/>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="112"/>
-      <c r="P42" s="112"/>
+      <c r="B42" s="133"/>
+      <c r="C42" s="133"/>
+      <c r="D42" s="133"/>
+      <c r="E42" s="133"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="133"/>
+      <c r="H42" s="133"/>
+      <c r="I42" s="133"/>
+      <c r="J42" s="133"/>
+      <c r="K42" s="133"/>
+      <c r="L42" s="133"/>
+      <c r="M42" s="133"/>
+      <c r="N42" s="133"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
     </row>
     <row r="43" spans="1:16" ht="60.75" customHeight="1">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="133" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="116"/>
-      <c r="C43" s="116"/>
-      <c r="D43" s="116"/>
-      <c r="E43" s="116"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="116"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="116"/>
-      <c r="L43" s="116"/>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116"/>
-      <c r="O43" s="112"/>
-      <c r="P43" s="112"/>
+      <c r="B43" s="133"/>
+      <c r="C43" s="133"/>
+      <c r="D43" s="133"/>
+      <c r="E43" s="133"/>
+      <c r="F43" s="133"/>
+      <c r="G43" s="133"/>
+      <c r="H43" s="133"/>
+      <c r="I43" s="133"/>
+      <c r="J43" s="133"/>
+      <c r="K43" s="133"/>
+      <c r="L43" s="133"/>
+      <c r="M43" s="133"/>
+      <c r="N43" s="133"/>
+      <c r="O43" s="59"/>
+      <c r="P43" s="59"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="111"/>
-      <c r="B44" s="111"/>
-      <c r="C44" s="111"/>
-      <c r="D44" s="111"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="111"/>
-      <c r="G44" s="111"/>
-      <c r="H44" s="111"/>
-      <c r="I44" s="111"/>
-      <c r="J44" s="111"/>
-      <c r="K44" s="111"/>
-      <c r="L44" s="111"/>
-      <c r="M44" s="111"/>
-      <c r="N44" s="111"/>
-      <c r="O44" s="112"/>
-      <c r="P44" s="112"/>
+      <c r="A44" s="136"/>
+      <c r="B44" s="136"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="136"/>
+      <c r="G44" s="136"/>
+      <c r="H44" s="136"/>
+      <c r="I44" s="136"/>
+      <c r="J44" s="136"/>
+      <c r="K44" s="136"/>
+      <c r="L44" s="136"/>
+      <c r="M44" s="136"/>
+      <c r="N44" s="136"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="59"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="111"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
-      <c r="L45" s="111"/>
-      <c r="M45" s="111"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="112"/>
-      <c r="P45" s="112"/>
+      <c r="A45" s="136"/>
+      <c r="B45" s="136"/>
+      <c r="C45" s="136"/>
+      <c r="D45" s="136"/>
+      <c r="E45" s="136"/>
+      <c r="F45" s="136"/>
+      <c r="G45" s="136"/>
+      <c r="H45" s="136"/>
+      <c r="I45" s="136"/>
+      <c r="J45" s="136"/>
+      <c r="K45" s="136"/>
+      <c r="L45" s="136"/>
+      <c r="M45" s="136"/>
+      <c r="N45" s="136"/>
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="111"/>
-      <c r="B46" s="111"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="111"/>
-      <c r="H46" s="111"/>
-      <c r="I46" s="111"/>
-      <c r="J46" s="111"/>
-      <c r="K46" s="111"/>
-      <c r="L46" s="111"/>
-      <c r="M46" s="111"/>
-      <c r="N46" s="111"/>
-      <c r="O46" s="112"/>
-      <c r="P46" s="112"/>
+      <c r="A46" s="136"/>
+      <c r="B46" s="136"/>
+      <c r="C46" s="136"/>
+      <c r="D46" s="136"/>
+      <c r="E46" s="136"/>
+      <c r="F46" s="136"/>
+      <c r="G46" s="136"/>
+      <c r="H46" s="136"/>
+      <c r="I46" s="136"/>
+      <c r="J46" s="136"/>
+      <c r="K46" s="136"/>
+      <c r="L46" s="136"/>
+      <c r="M46" s="136"/>
+      <c r="N46" s="136"/>
+      <c r="O46" s="59"/>
+      <c r="P46" s="59"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="111"/>
-      <c r="B47" s="111"/>
-      <c r="C47" s="111"/>
-      <c r="D47" s="111"/>
-      <c r="E47" s="111"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="111"/>
-      <c r="H47" s="111"/>
-      <c r="I47" s="111"/>
-      <c r="J47" s="111"/>
-      <c r="K47" s="111"/>
-      <c r="L47" s="111"/>
-      <c r="M47" s="111"/>
-      <c r="N47" s="111"/>
-      <c r="O47" s="112"/>
-      <c r="P47" s="112"/>
+      <c r="A47" s="136"/>
+      <c r="B47" s="136"/>
+      <c r="C47" s="136"/>
+      <c r="D47" s="136"/>
+      <c r="E47" s="136"/>
+      <c r="F47" s="136"/>
+      <c r="G47" s="136"/>
+      <c r="H47" s="136"/>
+      <c r="I47" s="136"/>
+      <c r="J47" s="136"/>
+      <c r="K47" s="136"/>
+      <c r="L47" s="136"/>
+      <c r="M47" s="136"/>
+      <c r="N47" s="136"/>
+      <c r="O47" s="59"/>
+      <c r="P47" s="59"/>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="111"/>
-      <c r="B48" s="111"/>
-      <c r="C48" s="111"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="111"/>
-      <c r="G48" s="111"/>
-      <c r="H48" s="111"/>
-      <c r="I48" s="111"/>
-      <c r="J48" s="111"/>
-      <c r="K48" s="111"/>
-      <c r="L48" s="111"/>
-      <c r="M48" s="111"/>
-      <c r="N48" s="111"/>
-      <c r="O48" s="112"/>
-      <c r="P48" s="112"/>
+      <c r="A48" s="136"/>
+      <c r="B48" s="136"/>
+      <c r="C48" s="136"/>
+      <c r="D48" s="136"/>
+      <c r="E48" s="136"/>
+      <c r="F48" s="136"/>
+      <c r="G48" s="136"/>
+      <c r="H48" s="136"/>
+      <c r="I48" s="136"/>
+      <c r="J48" s="136"/>
+      <c r="K48" s="136"/>
+      <c r="L48" s="136"/>
+      <c r="M48" s="136"/>
+      <c r="N48" s="136"/>
+      <c r="O48" s="59"/>
+      <c r="P48" s="59"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="111"/>
-      <c r="B49" s="111"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="111"/>
-      <c r="I49" s="111"/>
-      <c r="J49" s="111"/>
-      <c r="K49" s="111"/>
-      <c r="L49" s="111"/>
-      <c r="M49" s="111"/>
-      <c r="N49" s="111"/>
-      <c r="O49" s="112"/>
-      <c r="P49" s="112"/>
+      <c r="A49" s="136"/>
+      <c r="B49" s="136"/>
+      <c r="C49" s="136"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="136"/>
+      <c r="H49" s="136"/>
+      <c r="I49" s="136"/>
+      <c r="J49" s="136"/>
+      <c r="K49" s="136"/>
+      <c r="L49" s="136"/>
+      <c r="M49" s="136"/>
+      <c r="N49" s="136"/>
+      <c r="O49" s="59"/>
+      <c r="P49" s="59"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="111"/>
-      <c r="B50" s="111"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
-      <c r="K50" s="111"/>
-      <c r="L50" s="111"/>
-      <c r="M50" s="111"/>
-      <c r="N50" s="111"/>
-      <c r="O50" s="112"/>
-      <c r="P50" s="112"/>
+      <c r="A50" s="136"/>
+      <c r="B50" s="136"/>
+      <c r="C50" s="136"/>
+      <c r="D50" s="136"/>
+      <c r="E50" s="136"/>
+      <c r="F50" s="136"/>
+      <c r="G50" s="136"/>
+      <c r="H50" s="136"/>
+      <c r="I50" s="136"/>
+      <c r="J50" s="136"/>
+      <c r="K50" s="136"/>
+      <c r="L50" s="136"/>
+      <c r="M50" s="136"/>
+      <c r="N50" s="136"/>
+      <c r="O50" s="59"/>
+      <c r="P50" s="59"/>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="111"/>
-      <c r="B51" s="111"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="111"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
-      <c r="K51" s="111"/>
-      <c r="L51" s="111"/>
-      <c r="M51" s="111"/>
-      <c r="N51" s="111"/>
-      <c r="O51" s="112"/>
-      <c r="P51" s="112"/>
+      <c r="A51" s="136"/>
+      <c r="B51" s="136"/>
+      <c r="C51" s="136"/>
+      <c r="D51" s="136"/>
+      <c r="E51" s="136"/>
+      <c r="F51" s="136"/>
+      <c r="G51" s="136"/>
+      <c r="H51" s="136"/>
+      <c r="I51" s="136"/>
+      <c r="J51" s="136"/>
+      <c r="K51" s="136"/>
+      <c r="L51" s="136"/>
+      <c r="M51" s="136"/>
+      <c r="N51" s="136"/>
+      <c r="O51" s="59"/>
+      <c r="P51" s="59"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="111"/>
-      <c r="B52" s="111"/>
-      <c r="C52" s="111"/>
-      <c r="D52" s="111"/>
-      <c r="E52" s="111"/>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="111"/>
-      <c r="I52" s="111"/>
-      <c r="J52" s="111"/>
-      <c r="K52" s="111"/>
-      <c r="L52" s="111"/>
-      <c r="M52" s="111"/>
-      <c r="N52" s="111"/>
-      <c r="O52" s="112"/>
-      <c r="P52" s="112"/>
+      <c r="A52" s="136"/>
+      <c r="B52" s="136"/>
+      <c r="C52" s="136"/>
+      <c r="D52" s="136"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="136"/>
+      <c r="G52" s="136"/>
+      <c r="H52" s="136"/>
+      <c r="I52" s="136"/>
+      <c r="J52" s="136"/>
+      <c r="K52" s="136"/>
+      <c r="L52" s="136"/>
+      <c r="M52" s="136"/>
+      <c r="N52" s="136"/>
+      <c r="O52" s="59"/>
+      <c r="P52" s="59"/>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="111"/>
-      <c r="B53" s="111"/>
-      <c r="C53" s="111"/>
-      <c r="D53" s="111"/>
-      <c r="E53" s="111"/>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="111"/>
-      <c r="I53" s="111"/>
-      <c r="J53" s="111"/>
-      <c r="K53" s="111"/>
-      <c r="L53" s="111"/>
-      <c r="M53" s="111"/>
-      <c r="N53" s="111"/>
-      <c r="O53" s="112"/>
-      <c r="P53" s="112"/>
+      <c r="A53" s="136"/>
+      <c r="B53" s="136"/>
+      <c r="C53" s="136"/>
+      <c r="D53" s="136"/>
+      <c r="E53" s="136"/>
+      <c r="F53" s="136"/>
+      <c r="G53" s="136"/>
+      <c r="H53" s="136"/>
+      <c r="I53" s="136"/>
+      <c r="J53" s="136"/>
+      <c r="K53" s="136"/>
+      <c r="L53" s="136"/>
+      <c r="M53" s="136"/>
+      <c r="N53" s="136"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="111"/>
-      <c r="B54" s="111"/>
-      <c r="C54" s="111"/>
-      <c r="D54" s="111"/>
-      <c r="E54" s="111"/>
-      <c r="F54" s="111"/>
-      <c r="G54" s="111"/>
-      <c r="H54" s="111"/>
-      <c r="I54" s="111"/>
-      <c r="J54" s="111"/>
-      <c r="K54" s="111"/>
-      <c r="L54" s="111"/>
-      <c r="M54" s="111"/>
-      <c r="N54" s="111"/>
-      <c r="O54" s="112"/>
-      <c r="P54" s="112"/>
+      <c r="A54" s="136"/>
+      <c r="B54" s="136"/>
+      <c r="C54" s="136"/>
+      <c r="D54" s="136"/>
+      <c r="E54" s="136"/>
+      <c r="F54" s="136"/>
+      <c r="G54" s="136"/>
+      <c r="H54" s="136"/>
+      <c r="I54" s="136"/>
+      <c r="J54" s="136"/>
+      <c r="K54" s="136"/>
+      <c r="L54" s="136"/>
+      <c r="M54" s="136"/>
+      <c r="N54" s="136"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="111"/>
-      <c r="B55" s="111"/>
-      <c r="C55" s="111"/>
-      <c r="D55" s="111"/>
-      <c r="E55" s="111"/>
-      <c r="F55" s="111"/>
-      <c r="G55" s="111"/>
-      <c r="H55" s="111"/>
-      <c r="I55" s="111"/>
-      <c r="J55" s="111"/>
-      <c r="K55" s="111"/>
-      <c r="L55" s="111"/>
-      <c r="M55" s="111"/>
-      <c r="N55" s="111"/>
-      <c r="O55" s="112"/>
-      <c r="P55" s="112"/>
+      <c r="A55" s="136"/>
+      <c r="B55" s="136"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="136"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="136"/>
+      <c r="H55" s="136"/>
+      <c r="I55" s="136"/>
+      <c r="J55" s="136"/>
+      <c r="K55" s="136"/>
+      <c r="L55" s="136"/>
+      <c r="M55" s="136"/>
+      <c r="N55" s="136"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="111"/>
-      <c r="B56" s="111"/>
-      <c r="C56" s="111"/>
-      <c r="D56" s="111"/>
-      <c r="E56" s="111"/>
-      <c r="F56" s="111"/>
-      <c r="G56" s="111"/>
-      <c r="H56" s="111"/>
-      <c r="I56" s="111"/>
-      <c r="J56" s="111"/>
-      <c r="K56" s="111"/>
-      <c r="L56" s="111"/>
-      <c r="M56" s="111"/>
-      <c r="N56" s="111"/>
-      <c r="O56" s="112"/>
-      <c r="P56" s="112"/>
+      <c r="A56" s="136"/>
+      <c r="B56" s="136"/>
+      <c r="C56" s="136"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="136"/>
+      <c r="I56" s="136"/>
+      <c r="J56" s="136"/>
+      <c r="K56" s="136"/>
+      <c r="L56" s="136"/>
+      <c r="M56" s="136"/>
+      <c r="N56" s="136"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="59"/>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="111"/>
-      <c r="B57" s="111"/>
-      <c r="C57" s="111"/>
-      <c r="D57" s="111"/>
-      <c r="E57" s="111"/>
-      <c r="F57" s="111"/>
-      <c r="G57" s="111"/>
-      <c r="H57" s="111"/>
-      <c r="I57" s="111"/>
-      <c r="J57" s="111"/>
-      <c r="K57" s="111"/>
-      <c r="L57" s="111"/>
-      <c r="M57" s="111"/>
-      <c r="N57" s="111"/>
-      <c r="O57" s="112"/>
-      <c r="P57" s="112"/>
+      <c r="A57" s="136"/>
+      <c r="B57" s="136"/>
+      <c r="C57" s="136"/>
+      <c r="D57" s="136"/>
+      <c r="E57" s="136"/>
+      <c r="F57" s="136"/>
+      <c r="G57" s="136"/>
+      <c r="H57" s="136"/>
+      <c r="I57" s="136"/>
+      <c r="J57" s="136"/>
+      <c r="K57" s="136"/>
+      <c r="L57" s="136"/>
+      <c r="M57" s="136"/>
+      <c r="N57" s="136"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="59"/>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="111"/>
-      <c r="B58" s="111"/>
-      <c r="C58" s="111"/>
-      <c r="D58" s="111"/>
-      <c r="E58" s="111"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="111"/>
-      <c r="K58" s="111"/>
-      <c r="L58" s="111"/>
-      <c r="M58" s="111"/>
-      <c r="N58" s="111"/>
-      <c r="O58" s="112"/>
-      <c r="P58" s="112"/>
+      <c r="A58" s="136"/>
+      <c r="B58" s="136"/>
+      <c r="C58" s="136"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="136"/>
+      <c r="G58" s="136"/>
+      <c r="H58" s="136"/>
+      <c r="I58" s="136"/>
+      <c r="J58" s="136"/>
+      <c r="K58" s="136"/>
+      <c r="L58" s="136"/>
+      <c r="M58" s="136"/>
+      <c r="N58" s="136"/>
+      <c r="O58" s="59"/>
+      <c r="P58" s="59"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="111"/>
-      <c r="B59" s="111"/>
-      <c r="C59" s="111"/>
-      <c r="D59" s="111"/>
-      <c r="E59" s="111"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
-      <c r="H59" s="111"/>
-      <c r="I59" s="111"/>
-      <c r="J59" s="111"/>
-      <c r="K59" s="111"/>
-      <c r="L59" s="111"/>
-      <c r="M59" s="111"/>
-      <c r="N59" s="111"/>
-      <c r="O59" s="112"/>
-      <c r="P59" s="112"/>
+      <c r="A59" s="136"/>
+      <c r="B59" s="136"/>
+      <c r="C59" s="136"/>
+      <c r="D59" s="136"/>
+      <c r="E59" s="136"/>
+      <c r="F59" s="136"/>
+      <c r="G59" s="136"/>
+      <c r="H59" s="136"/>
+      <c r="I59" s="136"/>
+      <c r="J59" s="136"/>
+      <c r="K59" s="136"/>
+      <c r="L59" s="136"/>
+      <c r="M59" s="136"/>
+      <c r="N59" s="136"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="112"/>
-      <c r="B60" s="112"/>
-      <c r="C60" s="112"/>
-      <c r="D60" s="112"/>
-      <c r="E60" s="112"/>
-      <c r="F60" s="112"/>
-      <c r="G60" s="112"/>
-      <c r="H60" s="112"/>
-      <c r="I60" s="112"/>
-      <c r="J60" s="112"/>
-      <c r="K60" s="112"/>
-      <c r="L60" s="112"/>
-      <c r="M60" s="112"/>
-      <c r="N60" s="112"/>
-      <c r="O60" s="112"/>
-      <c r="P60" s="112"/>
+      <c r="A60" s="59"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="59"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="59"/>
+      <c r="N60" s="59"/>
+      <c r="O60" s="59"/>
+      <c r="P60" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="B30:O30"/>
-    <mergeCell ref="B31:O31"/>
-    <mergeCell ref="B32:O32"/>
-    <mergeCell ref="B33:O33"/>
-    <mergeCell ref="B28:O28"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="A46:N46"/>
+    <mergeCell ref="A47:N47"/>
+    <mergeCell ref="A48:N48"/>
+    <mergeCell ref="A49:N49"/>
+    <mergeCell ref="A42:N42"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="A43:N43"/>
+    <mergeCell ref="A44:N44"/>
+    <mergeCell ref="A45:N45"/>
+    <mergeCell ref="A50:N50"/>
+    <mergeCell ref="A51:N51"/>
+    <mergeCell ref="A52:N52"/>
+    <mergeCell ref="A53:N53"/>
+    <mergeCell ref="A54:N54"/>
+    <mergeCell ref="A55:N55"/>
+    <mergeCell ref="A56:N56"/>
+    <mergeCell ref="A57:N57"/>
+    <mergeCell ref="A58:N58"/>
+    <mergeCell ref="A59:N59"/>
     <mergeCell ref="A41:M41"/>
     <mergeCell ref="A38:N38"/>
     <mergeCell ref="A39:N39"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="O1:O3"/>
-    <mergeCell ref="A55:N55"/>
-    <mergeCell ref="A56:N56"/>
-    <mergeCell ref="A57:N57"/>
-    <mergeCell ref="A58:N58"/>
-    <mergeCell ref="A59:N59"/>
-    <mergeCell ref="A50:N50"/>
-    <mergeCell ref="A51:N51"/>
-    <mergeCell ref="A52:N52"/>
-    <mergeCell ref="A53:N53"/>
-    <mergeCell ref="A54:N54"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="B1:B4"/>
@@ -47216,15 +47249,14 @@
     <mergeCell ref="D1:E3"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="A42:N42"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="A43:N43"/>
-    <mergeCell ref="A44:N44"/>
-    <mergeCell ref="A45:N45"/>
-    <mergeCell ref="A46:N46"/>
-    <mergeCell ref="A47:N47"/>
-    <mergeCell ref="A48:N48"/>
-    <mergeCell ref="A49:N49"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B31:O31"/>
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="B33:O33"/>
+    <mergeCell ref="B28:O28"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="B29:O29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -47233,17 +47265,551 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE09EFEF-EC0B-4984-B180-595A6EF1BBAD}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="16384" width="20.7109375" style="51"/>
+    <col min="1" max="1" width="20.7109375" style="51"/>
+    <col min="2" max="2" width="15.7109375" style="51" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" style="51" customWidth="1"/>
+    <col min="4" max="16384" width="20.7109375" style="51"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B1" s="147" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+    </row>
+    <row r="2" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B2" s="148" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+    </row>
+    <row r="3" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B3" s="148"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
+    </row>
+    <row r="4" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B4" s="149" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="149"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="149"/>
+    </row>
+    <row r="5" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B5" s="150"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="150"/>
+      <c r="E5" s="150"/>
+      <c r="F5" s="150"/>
+    </row>
+    <row r="6" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="120" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="120" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="120" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="122" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="122"/>
+    </row>
+    <row r="8" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="122"/>
+    </row>
+    <row r="9" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B9" s="120"/>
+      <c r="C9" s="120"/>
+      <c r="D9" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="53">
+        <v>1</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="54">
+        <f>'Capacidade de Corrente'!I5</f>
+        <v>1200</v>
+      </c>
+      <c r="E10" s="54">
+        <f>'Capacidade de Corrente'!J5</f>
+        <v>127</v>
+      </c>
+      <c r="F10" s="146">
+        <f>'Capacidade de Corrente'!K5</f>
+        <v>9.4488188976377945</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="53">
+        <v>2</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="54">
+        <f>'Capacidade de Corrente'!I6</f>
+        <v>1700</v>
+      </c>
+      <c r="E11" s="54">
+        <f>'Capacidade de Corrente'!J6</f>
+        <v>127</v>
+      </c>
+      <c r="F11" s="146">
+        <f>'Capacidade de Corrente'!K6</f>
+        <v>13.385826771653543</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="53">
+        <v>3</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="54">
+        <f>'Capacidade de Corrente'!I7</f>
+        <v>2100</v>
+      </c>
+      <c r="E12" s="54">
+        <f>'Capacidade de Corrente'!J7</f>
+        <v>127</v>
+      </c>
+      <c r="F12" s="146">
+        <f>'Capacidade de Corrente'!K7</f>
+        <v>16.535433070866141</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="53">
+        <v>4</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="54">
+        <f>'Capacidade de Corrente'!I8</f>
+        <v>1900</v>
+      </c>
+      <c r="E13" s="54">
+        <f>'Capacidade de Corrente'!J8</f>
+        <v>127</v>
+      </c>
+      <c r="F13" s="146">
+        <f>'Capacidade de Corrente'!K8</f>
+        <v>14.960629921259843</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B14" s="53">
+        <v>5</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="54">
+        <f>'Capacidade de Corrente'!I9</f>
+        <v>1900</v>
+      </c>
+      <c r="E14" s="54">
+        <f>'Capacidade de Corrente'!J9</f>
+        <v>127</v>
+      </c>
+      <c r="F14" s="146">
+        <f>'Capacidade de Corrente'!K9</f>
+        <v>14.960629921259843</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B15" s="53">
+        <v>6</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="54">
+        <f>'Capacidade de Corrente'!I10</f>
+        <v>2500</v>
+      </c>
+      <c r="E15" s="54">
+        <f>'Capacidade de Corrente'!J10</f>
+        <v>127</v>
+      </c>
+      <c r="F15" s="146">
+        <f>'Capacidade de Corrente'!K10</f>
+        <v>19.685039370078741</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B16" s="53">
+        <v>7</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="54">
+        <f>'Capacidade de Corrente'!I11</f>
+        <v>2000</v>
+      </c>
+      <c r="E16" s="54">
+        <f>'Capacidade de Corrente'!J11</f>
+        <v>127</v>
+      </c>
+      <c r="F16" s="146">
+        <f>'Capacidade de Corrente'!K11</f>
+        <v>15.748031496062993</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B17" s="53">
+        <v>8</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="54">
+        <f>'Capacidade de Corrente'!I12</f>
+        <v>2000</v>
+      </c>
+      <c r="E17" s="54">
+        <f>'Capacidade de Corrente'!J12</f>
+        <v>127</v>
+      </c>
+      <c r="F17" s="146">
+        <f>'Capacidade de Corrente'!K12</f>
+        <v>15.748031496062993</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B18" s="53">
+        <v>9</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="54">
+        <f>'Capacidade de Corrente'!I13</f>
+        <v>2000</v>
+      </c>
+      <c r="E18" s="54">
+        <f>'Capacidade de Corrente'!J13</f>
+        <v>127</v>
+      </c>
+      <c r="F18" s="146">
+        <f>'Capacidade de Corrente'!K13</f>
+        <v>15.748031496062993</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B19" s="53">
+        <v>10</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="54">
+        <f>'Capacidade de Corrente'!I14</f>
+        <v>5400</v>
+      </c>
+      <c r="E19" s="54">
+        <f>'Capacidade de Corrente'!J14</f>
+        <v>220</v>
+      </c>
+      <c r="F19" s="146">
+        <f>'Capacidade de Corrente'!K14</f>
+        <v>24.545454545454547</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B20" s="53">
+        <v>11</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="54">
+        <f>'Capacidade de Corrente'!I15</f>
+        <v>5400</v>
+      </c>
+      <c r="E20" s="54">
+        <f>'Capacidade de Corrente'!J15</f>
+        <v>220</v>
+      </c>
+      <c r="F20" s="146">
+        <f>'Capacidade de Corrente'!K15</f>
+        <v>24.545454545454547</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B21" s="53">
+        <v>12</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="54">
+        <f>'Capacidade de Corrente'!I16</f>
+        <v>2625</v>
+      </c>
+      <c r="E21" s="54">
+        <f>'Capacidade de Corrente'!J16</f>
+        <v>220</v>
+      </c>
+      <c r="F21" s="146">
+        <f>'Capacidade de Corrente'!K16</f>
+        <v>11.931818181818182</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B22" s="53">
+        <v>13</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="54">
+        <f>'Capacidade de Corrente'!I17</f>
+        <v>1650</v>
+      </c>
+      <c r="E22" s="54">
+        <f>'Capacidade de Corrente'!J17</f>
+        <v>220</v>
+      </c>
+      <c r="F22" s="146">
+        <f>'Capacidade de Corrente'!K17</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B23" s="53">
+        <v>14</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="54">
+        <f>'Capacidade de Corrente'!I18</f>
+        <v>1650</v>
+      </c>
+      <c r="E23" s="54">
+        <f>'Capacidade de Corrente'!J18</f>
+        <v>220</v>
+      </c>
+      <c r="F23" s="146">
+        <f>'Capacidade de Corrente'!K18</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B24" s="53">
+        <v>15</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="54">
+        <f>'Capacidade de Corrente'!I19</f>
+        <v>400</v>
+      </c>
+      <c r="E24" s="54">
+        <f>'Capacidade de Corrente'!J19</f>
+        <v>127</v>
+      </c>
+      <c r="F24" s="146">
+        <f>'Capacidade de Corrente'!K19</f>
+        <v>3.1496062992125986</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B25" s="53">
+        <v>16</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="54">
+        <f>'Capacidade de Corrente'!I20</f>
+        <v>1760</v>
+      </c>
+      <c r="E25" s="54">
+        <f>'Capacidade de Corrente'!J20</f>
+        <v>220</v>
+      </c>
+      <c r="F25" s="146">
+        <f>'Capacidade de Corrente'!K20</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B26" s="53">
+        <v>17</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="54">
+        <f>'Capacidade de Corrente'!I21</f>
+        <v>300</v>
+      </c>
+      <c r="E26" s="54">
+        <f>'Capacidade de Corrente'!J21</f>
+        <v>220</v>
+      </c>
+      <c r="F26" s="146">
+        <f>'Capacidade de Corrente'!K21</f>
+        <v>1.3636363636363635</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B27" s="53">
+        <v>18</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="54">
+        <f>'Capacidade de Corrente'!I22</f>
+        <v>600</v>
+      </c>
+      <c r="E27" s="54">
+        <f>'Capacidade de Corrente'!J22</f>
+        <v>127</v>
+      </c>
+      <c r="F27" s="146">
+        <f>'Capacidade de Corrente'!K22</f>
+        <v>4.7244094488188972</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B28" s="53">
+        <v>19</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="54">
+        <f>'Capacidade de Corrente'!I23</f>
+        <v>600</v>
+      </c>
+      <c r="E28" s="54">
+        <f>'Capacidade de Corrente'!J23</f>
+        <v>127</v>
+      </c>
+      <c r="F28" s="146">
+        <f>'Capacidade de Corrente'!K23</f>
+        <v>4.7244094488188972</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B29" s="53">
+        <v>20</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="54">
+        <f>'Capacidade de Corrente'!I24</f>
+        <v>600</v>
+      </c>
+      <c r="E29" s="54">
+        <f>'Capacidade de Corrente'!J24</f>
+        <v>127</v>
+      </c>
+      <c r="F29" s="146">
+        <f>'Capacidade de Corrente'!K24</f>
+        <v>4.7244094488188972</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B30" s="53">
+        <v>21</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="54">
+        <f>'Capacidade de Corrente'!I25</f>
+        <v>600</v>
+      </c>
+      <c r="E30" s="54">
+        <f>'Capacidade de Corrente'!J25</f>
+        <v>127</v>
+      </c>
+      <c r="F30" s="146">
+        <f>'Capacidade de Corrente'!K25</f>
+        <v>4.7244094488188972</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="20.100000000000001" customHeight="1">
+      <c r="B31" s="65">
+        <v>22</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="54">
+        <f>'Capacidade de Corrente'!I26</f>
+        <v>38885</v>
+      </c>
+      <c r="E31" s="54"/>
+      <c r="F31" s="146"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
leia tudo que há pra tras
queda de tensão para iluminação fez pelo método mais cachorro possível, pq ao contrário iria dar uma trabalheira da poha
</commit_message>
<xml_diff>
--- a/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
+++ b/Memorial_de_calculo_Gabriel.S_&_Ramon.M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\UFES\GitHub\Instel-I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9D2E8A-B620-42EC-BC7D-0F2127962940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A1B253-BAC9-4545-B1B7-E0E780B41ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação_Informações" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="182">
   <si>
     <t>Alunos: Gabriel Schettino Lucas e Ramon Rodrigues Morello</t>
   </si>
@@ -539,14 +539,152 @@
     <t>1) O cálculo do método "limte de queda de tensão" utilizará a corrente de projeto já calculada na planinha "Capacidade de Corrente", as colunas estão relacionadas!</t>
   </si>
   <si>
-    <t>2) No projeto um circuito pode estar passando por mais de um caminho, logo nesse cálculo será considerado o pior dos caminhos que o circuito está fazendo.</t>
+    <t>LEGENDA</t>
+  </si>
+  <si>
+    <t>PL: Ponto de Luz</t>
+  </si>
+  <si>
+    <t>TM: Tomada</t>
+  </si>
+  <si>
+    <t>TRECHO</t>
+  </si>
+  <si>
+    <t>Potência aparente do trecho (VA)</t>
+  </si>
+  <si>
+    <t>Corrente de projeto (A)</t>
+  </si>
+  <si>
+    <t>Comprimento do circuito (m)</t>
+  </si>
+  <si>
+    <t>Comprimento do circuito (km)</t>
+  </si>
+  <si>
+    <t>Δe_trecho (%)</t>
+  </si>
+  <si>
+    <t>Δe_acumulado (%)</t>
+  </si>
+  <si>
+    <t>EXEMPLO</t>
+  </si>
+  <si>
+    <t>QDC até ponto de luz A = QDC - PL(A)</t>
+  </si>
+  <si>
+    <t>Ponto de luz A até tomada 8 = PL(A) - TM(8)</t>
+  </si>
+  <si>
+    <t>QDC - PL(B1)</t>
+  </si>
+  <si>
+    <t>PL(B1) - PL(B2)</t>
+  </si>
+  <si>
+    <t>PL(B2) - PL(B3)</t>
+  </si>
+  <si>
+    <t>PL(B3) - PL(B4)</t>
+  </si>
+  <si>
+    <t>QDC - PL(I)</t>
+  </si>
+  <si>
+    <t>PL(I) - PL(J)</t>
+  </si>
+  <si>
+    <t>ANOTAÇÃO  EXTRA</t>
+  </si>
+  <si>
+    <t>Se houver mais um de um ponto de luz com mesma letra, eles serão numerados conforme proximadade do QDC, onde PL(A1) é o ponto de luz A mais proximo do QDC.</t>
+  </si>
+  <si>
+    <t>PL(I) - PL(K1)</t>
+  </si>
+  <si>
+    <t>PL(K1) - PL(K2)</t>
+  </si>
+  <si>
+    <t>PL(N1) - PL(N2)</t>
+  </si>
+  <si>
+    <t>PL(N2) - PL(N3)</t>
+  </si>
+  <si>
+    <t>Secção sugerida (mm²)</t>
+  </si>
+  <si>
+    <t>PL(N3) - PL(O)</t>
+  </si>
+  <si>
+    <t>QDC - PL(N1)</t>
+  </si>
+  <si>
+    <t>ΔV                (V/A*km) [2]</t>
+  </si>
+  <si>
+    <t>2) Os valores de "ΔV" utlizado nas tabelas a seguir será escolhido baseando-se na secção sugerida pelo método "Capacidade de Corrente" e com FP = 0.8</t>
+  </si>
+  <si>
+    <t>Tensão                    (V)</t>
+  </si>
+  <si>
+    <t>PL(M1) - PL(M2)</t>
+  </si>
+  <si>
+    <t>QDC - PL(M1)</t>
+  </si>
+  <si>
+    <t>QDC - PL(Q1)</t>
+  </si>
+  <si>
+    <t>PL(Q1) - PL(Q2)</t>
+  </si>
+  <si>
+    <t>PL(Q1) - PL(P1)</t>
+  </si>
+  <si>
+    <t>PL(P1) - PL(P2)</t>
+  </si>
+  <si>
+    <t>CIRCUITO 1: ILUMINAÇÃO EXTERNA</t>
+  </si>
+  <si>
+    <t>CIRCUITO 2: ILUMINAÇÃO INTERNA</t>
+  </si>
+  <si>
+    <t>QDC - PL(H)</t>
+  </si>
+  <si>
+    <t>PL(H) - PL(G)</t>
+  </si>
+  <si>
+    <t>PL(G) - PL(F)</t>
+  </si>
+  <si>
+    <t>PL(E) - PL(D)</t>
+  </si>
+  <si>
+    <t>PL(F) - PL(E)</t>
+  </si>
+  <si>
+    <t>PL(E) - PL(C.)</t>
+  </si>
+  <si>
+    <t>PL(B1) - PL(A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,8 +840,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,8 +885,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="56">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -1388,11 +1539,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1603,20 +1791,38 @@
     <xf numFmtId="2" fontId="1" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1629,45 +1835,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1682,22 +1877,18 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1721,32 +1912,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1755,9 +1922,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1787,13 +1951,31 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1801,6 +1983,96 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="16" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2033,14 +2305,14 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="82"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2063,14 +2335,14 @@
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="82"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="90"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2121,16 +2393,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="84" t="s">
+      <c r="C4" s="93"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="79"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="74"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2153,17 +2425,17 @@
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="79"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="79"/>
+      <c r="F5" s="74"/>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2189,17 +2461,17 @@
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="79"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="78" t="s">
+      <c r="E6" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="79"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2225,17 +2497,17 @@
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="79"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="78" t="s">
+      <c r="E7" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="79"/>
+      <c r="F7" s="74"/>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
@@ -2261,15 +2533,15 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4"/>
@@ -2293,15 +2565,15 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="79"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="78"/>
-      <c r="F9" s="79"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="74"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="4"/>
@@ -2325,15 +2597,15 @@
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="76" t="s">
+      <c r="C10" s="85"/>
+      <c r="D10" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="4"/>
@@ -2357,11 +2629,11 @@
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="79"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="4"/>
@@ -2385,11 +2657,11 @@
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2413,11 +2685,11 @@
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="92"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="82"/>
       <c r="G13" s="7"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2441,11 +2713,11 @@
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="79"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="74"/>
       <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2525,14 +2797,14 @@
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="73"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="85"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2555,14 +2827,14 @@
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="95" t="s">
+      <c r="B18" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="88"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="77"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2585,14 +2857,14 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="88"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="77"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2615,14 +2887,14 @@
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="88"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="77"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2645,14 +2917,14 @@
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="88"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2675,14 +2947,14 @@
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="88"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2705,12 +2977,12 @@
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="88"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2733,14 +3005,14 @@
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="75"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="1"/>
       <c r="I24" s="8"/>
       <c r="J24" s="1"/>
@@ -9139,6 +9411,24 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
@@ -9153,24 +9443,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -9181,7 +9453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:F26"/>
     </sheetView>
   </sheetViews>
@@ -9224,19 +9496,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="73"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -9254,17 +9526,17 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="75"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -9282,27 +9554,27 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="107" t="s">
+      <c r="D4" s="74"/>
+      <c r="E4" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="108" t="s">
+      <c r="F4" s="93"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="85"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="108" t="s">
+      <c r="I4" s="93"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="79"/>
+      <c r="L4" s="74"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -9320,7 +9592,7 @@
     </row>
     <row r="5" spans="1:26" ht="39.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="77"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
@@ -9468,35 +9740,35 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="104">
+      <c r="C8" s="115">
         <v>17.579999999999998</v>
       </c>
-      <c r="D8" s="104">
+      <c r="D8" s="115">
         <v>23.9</v>
       </c>
-      <c r="E8" s="100">
+      <c r="E8" s="101">
         <v>3</v>
       </c>
-      <c r="F8" s="100">
+      <c r="F8" s="101">
         <v>100</v>
       </c>
-      <c r="G8" s="98">
+      <c r="G8" s="111">
         <v>300</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="111">
         <v>4</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="100">
+      <c r="J8" s="101">
         <v>200</v>
       </c>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -9514,17 +9786,17 @@
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -10137,9 +10409,9 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="112"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
+      <c r="J22" s="103"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -10157,13 +10429,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -10222,9 +10494,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -10242,20 +10514,20 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="M26" s="109"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="98"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -10280,10 +10552,10 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -10308,12 +10580,12 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="114"/>
-      <c r="N28" s="87"/>
-      <c r="O28" s="87"/>
+      <c r="J28" s="99"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="105"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="76"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -10336,12 +10608,12 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="76"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -10364,10 +10636,10 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="109"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="98"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -10392,10 +10664,10 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="110"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="87"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="76"/>
+      <c r="L31" s="76"/>
+      <c r="M31" s="76"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -10420,9 +10692,9 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="111"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="76"/>
+      <c r="L32" s="76"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -10448,9 +10720,9 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="76"/>
+      <c r="L33" s="76"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -10476,9 +10748,9 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="87"/>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -16646,6 +16918,23 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="J32:L34"/>
@@ -16660,23 +16949,6 @@
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="M30:M31"/>
     <mergeCell ref="J31:L31"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B23:F23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16687,8 +16959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I25"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16758,20 +17030,20 @@
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="119"/>
-      <c r="F3" s="118" t="s">
+      <c r="E3" s="120"/>
+      <c r="F3" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="119"/>
+      <c r="G3" s="120"/>
       <c r="H3" s="30" t="s">
         <v>30</v>
       </c>
@@ -16802,8 +17074,8 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="117"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="32" t="s">
         <v>72</v>
       </c>
@@ -45222,7 +45494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6759B52-4959-44EC-8CDD-E150AEF41805}">
   <dimension ref="B4:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -45236,20 +45508,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="121" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="123" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="123"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="124"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="53">
@@ -45497,8 +45769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36D55B-3867-4EF4-9271-23288EED3B45}">
   <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -45516,90 +45788,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="121" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="137" t="s">
+      <c r="D1" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="138"/>
-      <c r="F1" s="137" t="s">
+      <c r="E1" s="130"/>
+      <c r="F1" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="138"/>
-      <c r="H1" s="143" t="s">
+      <c r="G1" s="130"/>
+      <c r="H1" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="120" t="s">
+      <c r="J1" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="122" t="s">
+      <c r="K1" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="122" t="s">
+      <c r="L1" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="122" t="s">
+      <c r="M1" s="123" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="122" t="s">
+      <c r="N1" s="123" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="122" t="s">
+      <c r="O1" s="123" t="s">
         <v>126</v>
       </c>
-      <c r="P1" s="122" t="s">
+      <c r="P1" s="123" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" s="122" t="s">
+      <c r="Q1" s="123" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" spans="2:17">
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
     </row>
     <row r="3" spans="2:17" ht="31.5" customHeight="1">
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
-      <c r="Q3" s="122"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="123"/>
+      <c r="Q3" s="123"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
       <c r="D4" s="52" t="s">
         <v>72</v>
       </c>
@@ -46631,106 +46903,106 @@
       <c r="Q26" s="67"/>
     </row>
     <row r="28" spans="2:18" ht="31.5" customHeight="1">
-      <c r="B28" s="130" t="s">
+      <c r="B28" s="144" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="131"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="131"/>
-      <c r="F28" s="131"/>
-      <c r="G28" s="131"/>
-      <c r="H28" s="131"/>
-      <c r="I28" s="131"/>
-      <c r="J28" s="131"/>
-      <c r="K28" s="131"/>
-      <c r="L28" s="131"/>
-      <c r="M28" s="131"/>
-      <c r="N28" s="131"/>
-      <c r="O28" s="132"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="145"/>
+      <c r="L28" s="145"/>
+      <c r="M28" s="145"/>
+      <c r="N28" s="145"/>
+      <c r="O28" s="146"/>
     </row>
     <row r="29" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B29" s="124" t="s">
+      <c r="B29" s="138" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
-      <c r="G29" s="125"/>
-      <c r="H29" s="125"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="125"/>
-      <c r="L29" s="125"/>
-      <c r="M29" s="125"/>
-      <c r="N29" s="125"/>
-      <c r="O29" s="126"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="139"/>
+      <c r="L29" s="139"/>
+      <c r="M29" s="139"/>
+      <c r="N29" s="139"/>
+      <c r="O29" s="140"/>
     </row>
     <row r="30" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B30" s="124" t="s">
+      <c r="B30" s="138" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="125"/>
-      <c r="G30" s="125"/>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="125"/>
-      <c r="L30" s="125"/>
-      <c r="M30" s="125"/>
-      <c r="N30" s="125"/>
-      <c r="O30" s="126"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="139"/>
+      <c r="J30" s="139"/>
+      <c r="K30" s="139"/>
+      <c r="L30" s="139"/>
+      <c r="M30" s="139"/>
+      <c r="N30" s="139"/>
+      <c r="O30" s="140"/>
     </row>
     <row r="31" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B31" s="124"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="125"/>
-      <c r="H31" s="125"/>
-      <c r="I31" s="125"/>
-      <c r="J31" s="125"/>
-      <c r="K31" s="125"/>
-      <c r="L31" s="125"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="125"/>
-      <c r="O31" s="126"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="139"/>
+      <c r="H31" s="139"/>
+      <c r="I31" s="139"/>
+      <c r="J31" s="139"/>
+      <c r="K31" s="139"/>
+      <c r="L31" s="139"/>
+      <c r="M31" s="139"/>
+      <c r="N31" s="139"/>
+      <c r="O31" s="140"/>
     </row>
     <row r="32" spans="2:18" s="61" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B32" s="124"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="125"/>
-      <c r="G32" s="125"/>
-      <c r="H32" s="125"/>
-      <c r="I32" s="125"/>
-      <c r="J32" s="125"/>
-      <c r="K32" s="125"/>
-      <c r="L32" s="125"/>
-      <c r="M32" s="125"/>
-      <c r="N32" s="125"/>
-      <c r="O32" s="126"/>
+      <c r="B32" s="138"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="139"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="139"/>
+      <c r="I32" s="139"/>
+      <c r="J32" s="139"/>
+      <c r="K32" s="139"/>
+      <c r="L32" s="139"/>
+      <c r="M32" s="139"/>
+      <c r="N32" s="139"/>
+      <c r="O32" s="140"/>
     </row>
     <row r="33" spans="1:16" s="61" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B33" s="127"/>
-      <c r="C33" s="128"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="128"/>
-      <c r="F33" s="128"/>
-      <c r="G33" s="128"/>
-      <c r="H33" s="128"/>
-      <c r="I33" s="128"/>
-      <c r="J33" s="128"/>
-      <c r="K33" s="128"/>
-      <c r="L33" s="128"/>
-      <c r="M33" s="128"/>
-      <c r="N33" s="128"/>
-      <c r="O33" s="129"/>
+      <c r="B33" s="141"/>
+      <c r="C33" s="142"/>
+      <c r="D33" s="142"/>
+      <c r="E33" s="142"/>
+      <c r="F33" s="142"/>
+      <c r="G33" s="142"/>
+      <c r="H33" s="142"/>
+      <c r="I33" s="142"/>
+      <c r="J33" s="142"/>
+      <c r="K33" s="142"/>
+      <c r="L33" s="142"/>
+      <c r="M33" s="142"/>
+      <c r="N33" s="142"/>
+      <c r="O33" s="143"/>
     </row>
     <row r="34" spans="1:16" s="61" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B34" s="68"/>
@@ -46766,11 +47038,11 @@
       <c r="O35" s="64"/>
     </row>
     <row r="36" spans="1:16" ht="47.25" customHeight="1">
-      <c r="A36" s="135" t="s">
+      <c r="A36" s="128" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="135"/>
-      <c r="C36" s="135"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="128"/>
       <c r="D36" s="63" t="s">
         <v>119</v>
       </c>
@@ -46783,55 +47055,55 @@
       <c r="G36" s="63"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="B37" s="136"/>
-      <c r="C37" s="136"/>
-      <c r="D37" s="136"/>
-      <c r="E37" s="136"/>
-      <c r="F37" s="136"/>
-      <c r="G37" s="136"/>
-      <c r="H37" s="136"/>
-      <c r="I37" s="136"/>
-      <c r="J37" s="136"/>
-      <c r="K37" s="136"/>
-      <c r="L37" s="136"/>
-      <c r="M37" s="136"/>
-      <c r="N37" s="136"/>
+      <c r="B37" s="125"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="125"/>
+      <c r="E37" s="125"/>
+      <c r="F37" s="125"/>
+      <c r="G37" s="125"/>
+      <c r="H37" s="125"/>
+      <c r="I37" s="125"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="125"/>
+      <c r="L37" s="125"/>
+      <c r="M37" s="125"/>
+      <c r="N37" s="125"/>
     </row>
     <row r="38" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A38" s="134" t="s">
+      <c r="A38" s="127" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="134"/>
-      <c r="C38" s="134"/>
-      <c r="D38" s="134"/>
-      <c r="E38" s="134"/>
-      <c r="F38" s="134"/>
-      <c r="G38" s="134"/>
-      <c r="H38" s="134"/>
-      <c r="I38" s="134"/>
-      <c r="J38" s="134"/>
-      <c r="K38" s="134"/>
-      <c r="L38" s="134"/>
-      <c r="M38" s="134"/>
-      <c r="N38" s="134"/>
+      <c r="B38" s="127"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="127"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="127"/>
+      <c r="G38" s="127"/>
+      <c r="H38" s="127"/>
+      <c r="I38" s="127"/>
+      <c r="J38" s="127"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="127"/>
+      <c r="M38" s="127"/>
+      <c r="N38" s="127"/>
     </row>
     <row r="39" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A39" s="134" t="s">
+      <c r="A39" s="127" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="134"/>
-      <c r="C39" s="134"/>
-      <c r="D39" s="134"/>
-      <c r="E39" s="134"/>
-      <c r="F39" s="134"/>
-      <c r="G39" s="134"/>
-      <c r="H39" s="134"/>
-      <c r="I39" s="134"/>
-      <c r="J39" s="134"/>
-      <c r="K39" s="134"/>
-      <c r="L39" s="134"/>
-      <c r="M39" s="134"/>
-      <c r="N39" s="134"/>
+      <c r="B39" s="127"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="127"/>
+      <c r="E39" s="127"/>
+      <c r="F39" s="127"/>
+      <c r="G39" s="127"/>
+      <c r="H39" s="127"/>
+      <c r="I39" s="127"/>
+      <c r="J39" s="127"/>
+      <c r="K39" s="127"/>
+      <c r="L39" s="127"/>
+      <c r="M39" s="127"/>
+      <c r="N39" s="127"/>
     </row>
     <row r="40" spans="1:16" ht="26.25">
       <c r="B40" s="60"/>
@@ -46849,348 +47121,348 @@
       <c r="N40" s="60"/>
     </row>
     <row r="41" spans="1:16" ht="38.25" customHeight="1">
-      <c r="A41" s="133" t="s">
+      <c r="A41" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="133"/>
-      <c r="C41" s="133"/>
-      <c r="D41" s="133"/>
-      <c r="E41" s="133"/>
-      <c r="F41" s="133"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="133"/>
-      <c r="K41" s="133"/>
-      <c r="L41" s="133"/>
-      <c r="M41" s="133"/>
+      <c r="B41" s="126"/>
+      <c r="C41" s="126"/>
+      <c r="D41" s="126"/>
+      <c r="E41" s="126"/>
+      <c r="F41" s="126"/>
+      <c r="G41" s="126"/>
+      <c r="H41" s="126"/>
+      <c r="I41" s="126"/>
+      <c r="J41" s="126"/>
+      <c r="K41" s="126"/>
+      <c r="L41" s="126"/>
+      <c r="M41" s="126"/>
       <c r="N41" s="62"/>
     </row>
     <row r="42" spans="1:16" ht="39.75" customHeight="1">
-      <c r="A42" s="133" t="s">
+      <c r="A42" s="126" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="133"/>
-      <c r="C42" s="133"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="133"/>
-      <c r="F42" s="133"/>
-      <c r="G42" s="133"/>
-      <c r="H42" s="133"/>
-      <c r="I42" s="133"/>
-      <c r="J42" s="133"/>
-      <c r="K42" s="133"/>
-      <c r="L42" s="133"/>
-      <c r="M42" s="133"/>
-      <c r="N42" s="133"/>
+      <c r="B42" s="126"/>
+      <c r="C42" s="126"/>
+      <c r="D42" s="126"/>
+      <c r="E42" s="126"/>
+      <c r="F42" s="126"/>
+      <c r="G42" s="126"/>
+      <c r="H42" s="126"/>
+      <c r="I42" s="126"/>
+      <c r="J42" s="126"/>
+      <c r="K42" s="126"/>
+      <c r="L42" s="126"/>
+      <c r="M42" s="126"/>
+      <c r="N42" s="126"/>
       <c r="O42" s="59"/>
       <c r="P42" s="59"/>
     </row>
     <row r="43" spans="1:16" ht="60.75" customHeight="1">
-      <c r="A43" s="133" t="s">
+      <c r="A43" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="133"/>
-      <c r="C43" s="133"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="133"/>
-      <c r="F43" s="133"/>
-      <c r="G43" s="133"/>
-      <c r="H43" s="133"/>
-      <c r="I43" s="133"/>
-      <c r="J43" s="133"/>
-      <c r="K43" s="133"/>
-      <c r="L43" s="133"/>
-      <c r="M43" s="133"/>
-      <c r="N43" s="133"/>
+      <c r="B43" s="126"/>
+      <c r="C43" s="126"/>
+      <c r="D43" s="126"/>
+      <c r="E43" s="126"/>
+      <c r="F43" s="126"/>
+      <c r="G43" s="126"/>
+      <c r="H43" s="126"/>
+      <c r="I43" s="126"/>
+      <c r="J43" s="126"/>
+      <c r="K43" s="126"/>
+      <c r="L43" s="126"/>
+      <c r="M43" s="126"/>
+      <c r="N43" s="126"/>
       <c r="O43" s="59"/>
       <c r="P43" s="59"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="136"/>
-      <c r="B44" s="136"/>
-      <c r="C44" s="136"/>
-      <c r="D44" s="136"/>
-      <c r="E44" s="136"/>
-      <c r="F44" s="136"/>
-      <c r="G44" s="136"/>
-      <c r="H44" s="136"/>
-      <c r="I44" s="136"/>
-      <c r="J44" s="136"/>
-      <c r="K44" s="136"/>
-      <c r="L44" s="136"/>
-      <c r="M44" s="136"/>
-      <c r="N44" s="136"/>
+      <c r="A44" s="125"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="125"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="125"/>
+      <c r="F44" s="125"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="125"/>
+      <c r="I44" s="125"/>
+      <c r="J44" s="125"/>
+      <c r="K44" s="125"/>
+      <c r="L44" s="125"/>
+      <c r="M44" s="125"/>
+      <c r="N44" s="125"/>
       <c r="O44" s="59"/>
       <c r="P44" s="59"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="136"/>
-      <c r="B45" s="136"/>
-      <c r="C45" s="136"/>
-      <c r="D45" s="136"/>
-      <c r="E45" s="136"/>
-      <c r="F45" s="136"/>
-      <c r="G45" s="136"/>
-      <c r="H45" s="136"/>
-      <c r="I45" s="136"/>
-      <c r="J45" s="136"/>
-      <c r="K45" s="136"/>
-      <c r="L45" s="136"/>
-      <c r="M45" s="136"/>
-      <c r="N45" s="136"/>
+      <c r="A45" s="125"/>
+      <c r="B45" s="125"/>
+      <c r="C45" s="125"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="125"/>
+      <c r="F45" s="125"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="125"/>
+      <c r="I45" s="125"/>
+      <c r="J45" s="125"/>
+      <c r="K45" s="125"/>
+      <c r="L45" s="125"/>
+      <c r="M45" s="125"/>
+      <c r="N45" s="125"/>
       <c r="O45" s="59"/>
       <c r="P45" s="59"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="136"/>
-      <c r="B46" s="136"/>
-      <c r="C46" s="136"/>
-      <c r="D46" s="136"/>
-      <c r="E46" s="136"/>
-      <c r="F46" s="136"/>
-      <c r="G46" s="136"/>
-      <c r="H46" s="136"/>
-      <c r="I46" s="136"/>
-      <c r="J46" s="136"/>
-      <c r="K46" s="136"/>
-      <c r="L46" s="136"/>
-      <c r="M46" s="136"/>
-      <c r="N46" s="136"/>
+      <c r="A46" s="125"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="125"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="125"/>
+      <c r="F46" s="125"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="125"/>
+      <c r="I46" s="125"/>
+      <c r="J46" s="125"/>
+      <c r="K46" s="125"/>
+      <c r="L46" s="125"/>
+      <c r="M46" s="125"/>
+      <c r="N46" s="125"/>
       <c r="O46" s="59"/>
       <c r="P46" s="59"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="136"/>
-      <c r="B47" s="136"/>
-      <c r="C47" s="136"/>
-      <c r="D47" s="136"/>
-      <c r="E47" s="136"/>
-      <c r="F47" s="136"/>
-      <c r="G47" s="136"/>
-      <c r="H47" s="136"/>
-      <c r="I47" s="136"/>
-      <c r="J47" s="136"/>
-      <c r="K47" s="136"/>
-      <c r="L47" s="136"/>
-      <c r="M47" s="136"/>
-      <c r="N47" s="136"/>
+      <c r="A47" s="125"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="125"/>
+      <c r="D47" s="125"/>
+      <c r="E47" s="125"/>
+      <c r="F47" s="125"/>
+      <c r="G47" s="125"/>
+      <c r="H47" s="125"/>
+      <c r="I47" s="125"/>
+      <c r="J47" s="125"/>
+      <c r="K47" s="125"/>
+      <c r="L47" s="125"/>
+      <c r="M47" s="125"/>
+      <c r="N47" s="125"/>
       <c r="O47" s="59"/>
       <c r="P47" s="59"/>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="136"/>
-      <c r="B48" s="136"/>
-      <c r="C48" s="136"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="136"/>
-      <c r="F48" s="136"/>
-      <c r="G48" s="136"/>
-      <c r="H48" s="136"/>
-      <c r="I48" s="136"/>
-      <c r="J48" s="136"/>
-      <c r="K48" s="136"/>
-      <c r="L48" s="136"/>
-      <c r="M48" s="136"/>
-      <c r="N48" s="136"/>
+      <c r="A48" s="125"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="125"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="125"/>
+      <c r="F48" s="125"/>
+      <c r="G48" s="125"/>
+      <c r="H48" s="125"/>
+      <c r="I48" s="125"/>
+      <c r="J48" s="125"/>
+      <c r="K48" s="125"/>
+      <c r="L48" s="125"/>
+      <c r="M48" s="125"/>
+      <c r="N48" s="125"/>
       <c r="O48" s="59"/>
       <c r="P48" s="59"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="136"/>
-      <c r="B49" s="136"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="136"/>
-      <c r="F49" s="136"/>
-      <c r="G49" s="136"/>
-      <c r="H49" s="136"/>
-      <c r="I49" s="136"/>
-      <c r="J49" s="136"/>
-      <c r="K49" s="136"/>
-      <c r="L49" s="136"/>
-      <c r="M49" s="136"/>
-      <c r="N49" s="136"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="125"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="125"/>
+      <c r="F49" s="125"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="125"/>
+      <c r="I49" s="125"/>
+      <c r="J49" s="125"/>
+      <c r="K49" s="125"/>
+      <c r="L49" s="125"/>
+      <c r="M49" s="125"/>
+      <c r="N49" s="125"/>
       <c r="O49" s="59"/>
       <c r="P49" s="59"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="136"/>
-      <c r="B50" s="136"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="136"/>
-      <c r="G50" s="136"/>
-      <c r="H50" s="136"/>
-      <c r="I50" s="136"/>
-      <c r="J50" s="136"/>
-      <c r="K50" s="136"/>
-      <c r="L50" s="136"/>
-      <c r="M50" s="136"/>
-      <c r="N50" s="136"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="125"/>
+      <c r="F50" s="125"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="125"/>
+      <c r="I50" s="125"/>
+      <c r="J50" s="125"/>
+      <c r="K50" s="125"/>
+      <c r="L50" s="125"/>
+      <c r="M50" s="125"/>
+      <c r="N50" s="125"/>
       <c r="O50" s="59"/>
       <c r="P50" s="59"/>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="136"/>
-      <c r="B51" s="136"/>
-      <c r="C51" s="136"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136"/>
-      <c r="F51" s="136"/>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
-      <c r="K51" s="136"/>
-      <c r="L51" s="136"/>
-      <c r="M51" s="136"/>
-      <c r="N51" s="136"/>
+      <c r="A51" s="125"/>
+      <c r="B51" s="125"/>
+      <c r="C51" s="125"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="125"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="125"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="125"/>
+      <c r="K51" s="125"/>
+      <c r="L51" s="125"/>
+      <c r="M51" s="125"/>
+      <c r="N51" s="125"/>
       <c r="O51" s="59"/>
       <c r="P51" s="59"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="136"/>
-      <c r="B52" s="136"/>
-      <c r="C52" s="136"/>
-      <c r="D52" s="136"/>
-      <c r="E52" s="136"/>
-      <c r="F52" s="136"/>
-      <c r="G52" s="136"/>
-      <c r="H52" s="136"/>
-      <c r="I52" s="136"/>
-      <c r="J52" s="136"/>
-      <c r="K52" s="136"/>
-      <c r="L52" s="136"/>
-      <c r="M52" s="136"/>
-      <c r="N52" s="136"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="125"/>
+      <c r="C52" s="125"/>
+      <c r="D52" s="125"/>
+      <c r="E52" s="125"/>
+      <c r="F52" s="125"/>
+      <c r="G52" s="125"/>
+      <c r="H52" s="125"/>
+      <c r="I52" s="125"/>
+      <c r="J52" s="125"/>
+      <c r="K52" s="125"/>
+      <c r="L52" s="125"/>
+      <c r="M52" s="125"/>
+      <c r="N52" s="125"/>
       <c r="O52" s="59"/>
       <c r="P52" s="59"/>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="136"/>
-      <c r="B53" s="136"/>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="136"/>
-      <c r="F53" s="136"/>
-      <c r="G53" s="136"/>
-      <c r="H53" s="136"/>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
-      <c r="K53" s="136"/>
-      <c r="L53" s="136"/>
-      <c r="M53" s="136"/>
-      <c r="N53" s="136"/>
+      <c r="A53" s="125"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="125"/>
+      <c r="D53" s="125"/>
+      <c r="E53" s="125"/>
+      <c r="F53" s="125"/>
+      <c r="G53" s="125"/>
+      <c r="H53" s="125"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="125"/>
+      <c r="K53" s="125"/>
+      <c r="L53" s="125"/>
+      <c r="M53" s="125"/>
+      <c r="N53" s="125"/>
       <c r="O53" s="59"/>
       <c r="P53" s="59"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="136"/>
-      <c r="B54" s="136"/>
-      <c r="C54" s="136"/>
-      <c r="D54" s="136"/>
-      <c r="E54" s="136"/>
-      <c r="F54" s="136"/>
-      <c r="G54" s="136"/>
-      <c r="H54" s="136"/>
-      <c r="I54" s="136"/>
-      <c r="J54" s="136"/>
-      <c r="K54" s="136"/>
-      <c r="L54" s="136"/>
-      <c r="M54" s="136"/>
-      <c r="N54" s="136"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="125"/>
+      <c r="F54" s="125"/>
+      <c r="G54" s="125"/>
+      <c r="H54" s="125"/>
+      <c r="I54" s="125"/>
+      <c r="J54" s="125"/>
+      <c r="K54" s="125"/>
+      <c r="L54" s="125"/>
+      <c r="M54" s="125"/>
+      <c r="N54" s="125"/>
       <c r="O54" s="59"/>
       <c r="P54" s="59"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="136"/>
-      <c r="B55" s="136"/>
-      <c r="C55" s="136"/>
-      <c r="D55" s="136"/>
-      <c r="E55" s="136"/>
-      <c r="F55" s="136"/>
-      <c r="G55" s="136"/>
-      <c r="H55" s="136"/>
-      <c r="I55" s="136"/>
-      <c r="J55" s="136"/>
-      <c r="K55" s="136"/>
-      <c r="L55" s="136"/>
-      <c r="M55" s="136"/>
-      <c r="N55" s="136"/>
+      <c r="A55" s="125"/>
+      <c r="B55" s="125"/>
+      <c r="C55" s="125"/>
+      <c r="D55" s="125"/>
+      <c r="E55" s="125"/>
+      <c r="F55" s="125"/>
+      <c r="G55" s="125"/>
+      <c r="H55" s="125"/>
+      <c r="I55" s="125"/>
+      <c r="J55" s="125"/>
+      <c r="K55" s="125"/>
+      <c r="L55" s="125"/>
+      <c r="M55" s="125"/>
+      <c r="N55" s="125"/>
       <c r="O55" s="59"/>
       <c r="P55" s="59"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="136"/>
-      <c r="B56" s="136"/>
-      <c r="C56" s="136"/>
-      <c r="D56" s="136"/>
-      <c r="E56" s="136"/>
-      <c r="F56" s="136"/>
-      <c r="G56" s="136"/>
-      <c r="H56" s="136"/>
-      <c r="I56" s="136"/>
-      <c r="J56" s="136"/>
-      <c r="K56" s="136"/>
-      <c r="L56" s="136"/>
-      <c r="M56" s="136"/>
-      <c r="N56" s="136"/>
+      <c r="A56" s="125"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="125"/>
+      <c r="D56" s="125"/>
+      <c r="E56" s="125"/>
+      <c r="F56" s="125"/>
+      <c r="G56" s="125"/>
+      <c r="H56" s="125"/>
+      <c r="I56" s="125"/>
+      <c r="J56" s="125"/>
+      <c r="K56" s="125"/>
+      <c r="L56" s="125"/>
+      <c r="M56" s="125"/>
+      <c r="N56" s="125"/>
       <c r="O56" s="59"/>
       <c r="P56" s="59"/>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="136"/>
-      <c r="B57" s="136"/>
-      <c r="C57" s="136"/>
-      <c r="D57" s="136"/>
-      <c r="E57" s="136"/>
-      <c r="F57" s="136"/>
-      <c r="G57" s="136"/>
-      <c r="H57" s="136"/>
-      <c r="I57" s="136"/>
-      <c r="J57" s="136"/>
-      <c r="K57" s="136"/>
-      <c r="L57" s="136"/>
-      <c r="M57" s="136"/>
-      <c r="N57" s="136"/>
+      <c r="A57" s="125"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="125"/>
+      <c r="D57" s="125"/>
+      <c r="E57" s="125"/>
+      <c r="F57" s="125"/>
+      <c r="G57" s="125"/>
+      <c r="H57" s="125"/>
+      <c r="I57" s="125"/>
+      <c r="J57" s="125"/>
+      <c r="K57" s="125"/>
+      <c r="L57" s="125"/>
+      <c r="M57" s="125"/>
+      <c r="N57" s="125"/>
       <c r="O57" s="59"/>
       <c r="P57" s="59"/>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="136"/>
-      <c r="B58" s="136"/>
-      <c r="C58" s="136"/>
-      <c r="D58" s="136"/>
-      <c r="E58" s="136"/>
-      <c r="F58" s="136"/>
-      <c r="G58" s="136"/>
-      <c r="H58" s="136"/>
-      <c r="I58" s="136"/>
-      <c r="J58" s="136"/>
-      <c r="K58" s="136"/>
-      <c r="L58" s="136"/>
-      <c r="M58" s="136"/>
-      <c r="N58" s="136"/>
+      <c r="A58" s="125"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="125"/>
+      <c r="D58" s="125"/>
+      <c r="E58" s="125"/>
+      <c r="F58" s="125"/>
+      <c r="G58" s="125"/>
+      <c r="H58" s="125"/>
+      <c r="I58" s="125"/>
+      <c r="J58" s="125"/>
+      <c r="K58" s="125"/>
+      <c r="L58" s="125"/>
+      <c r="M58" s="125"/>
+      <c r="N58" s="125"/>
       <c r="O58" s="59"/>
       <c r="P58" s="59"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="136"/>
-      <c r="B59" s="136"/>
-      <c r="C59" s="136"/>
-      <c r="D59" s="136"/>
-      <c r="E59" s="136"/>
-      <c r="F59" s="136"/>
-      <c r="G59" s="136"/>
-      <c r="H59" s="136"/>
-      <c r="I59" s="136"/>
-      <c r="J59" s="136"/>
-      <c r="K59" s="136"/>
-      <c r="L59" s="136"/>
-      <c r="M59" s="136"/>
-      <c r="N59" s="136"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="125"/>
+      <c r="C59" s="125"/>
+      <c r="D59" s="125"/>
+      <c r="E59" s="125"/>
+      <c r="F59" s="125"/>
+      <c r="G59" s="125"/>
+      <c r="H59" s="125"/>
+      <c r="I59" s="125"/>
+      <c r="J59" s="125"/>
+      <c r="K59" s="125"/>
+      <c r="L59" s="125"/>
+      <c r="M59" s="125"/>
+      <c r="N59" s="125"/>
       <c r="O59" s="59"/>
       <c r="P59" s="59"/>
     </row>
@@ -47214,28 +47486,14 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A46:N46"/>
-    <mergeCell ref="A47:N47"/>
-    <mergeCell ref="A48:N48"/>
-    <mergeCell ref="A49:N49"/>
-    <mergeCell ref="A42:N42"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="A43:N43"/>
-    <mergeCell ref="A44:N44"/>
-    <mergeCell ref="A45:N45"/>
-    <mergeCell ref="A50:N50"/>
-    <mergeCell ref="A51:N51"/>
-    <mergeCell ref="A52:N52"/>
-    <mergeCell ref="A53:N53"/>
-    <mergeCell ref="A54:N54"/>
-    <mergeCell ref="A55:N55"/>
-    <mergeCell ref="A56:N56"/>
-    <mergeCell ref="A57:N57"/>
-    <mergeCell ref="A58:N58"/>
-    <mergeCell ref="A59:N59"/>
-    <mergeCell ref="A41:M41"/>
-    <mergeCell ref="A38:N38"/>
-    <mergeCell ref="A39:N39"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B31:O31"/>
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="B33:O33"/>
+    <mergeCell ref="B28:O28"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="B29:O29"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="O1:O3"/>
     <mergeCell ref="I1:I3"/>
@@ -47249,14 +47507,28 @@
     <mergeCell ref="D1:E3"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="B30:O30"/>
-    <mergeCell ref="B31:O31"/>
-    <mergeCell ref="B32:O32"/>
-    <mergeCell ref="B33:O33"/>
-    <mergeCell ref="B28:O28"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="A56:N56"/>
+    <mergeCell ref="A57:N57"/>
+    <mergeCell ref="A58:N58"/>
+    <mergeCell ref="A59:N59"/>
+    <mergeCell ref="A41:M41"/>
+    <mergeCell ref="A51:N51"/>
+    <mergeCell ref="A52:N52"/>
+    <mergeCell ref="A53:N53"/>
+    <mergeCell ref="A54:N54"/>
+    <mergeCell ref="A55:N55"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="A43:N43"/>
+    <mergeCell ref="A44:N44"/>
+    <mergeCell ref="A45:N45"/>
+    <mergeCell ref="A50:N50"/>
+    <mergeCell ref="A38:N38"/>
+    <mergeCell ref="A39:N39"/>
+    <mergeCell ref="A46:N46"/>
+    <mergeCell ref="A47:N47"/>
+    <mergeCell ref="A48:N48"/>
+    <mergeCell ref="A49:N49"/>
+    <mergeCell ref="A42:N42"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -47265,549 +47537,1216 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE09EFEF-EC0B-4984-B180-595A6EF1BBAD}">
-  <dimension ref="B1:F31"/>
+  <dimension ref="B2:K47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="51"/>
-    <col min="2" max="2" width="15.7109375" style="51" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" style="51" customWidth="1"/>
-    <col min="4" max="16384" width="20.7109375" style="51"/>
+    <col min="2" max="4" width="20.7109375" style="51" customWidth="1"/>
+    <col min="5" max="16384" width="20.7109375" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B1" s="147" t="s">
+    <row r="2" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B2" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-    </row>
-    <row r="2" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B2" s="148" t="s">
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="161"/>
+    </row>
+    <row r="3" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B3" s="162" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-    </row>
-    <row r="3" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-    </row>
-    <row r="4" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B4" s="149" t="s">
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="163"/>
+    </row>
+    <row r="4" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B4" s="162" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="163"/>
+    </row>
+    <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B5" s="164"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="157"/>
+      <c r="J5" s="157"/>
+      <c r="K5" s="163"/>
+    </row>
+    <row r="6" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B6" s="165" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="149"/>
-      <c r="D4" s="149"/>
-      <c r="E4" s="149"/>
-      <c r="F4" s="149"/>
-    </row>
-    <row r="5" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B5" s="150"/>
-      <c r="C5" s="150"/>
-      <c r="D5" s="150"/>
-      <c r="E5" s="150"/>
-      <c r="F5" s="150"/>
-    </row>
-    <row r="6" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B6" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="120" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="120" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="120" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="122" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="120"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="122"/>
-    </row>
-    <row r="8" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="120"/>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122"/>
-    </row>
-    <row r="9" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="53">
-        <v>1</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="54">
-        <f>'Capacidade de Corrente'!I5</f>
-        <v>1200</v>
-      </c>
-      <c r="E10" s="54">
-        <f>'Capacidade de Corrente'!J5</f>
+      <c r="C6" s="154"/>
+      <c r="D6" s="151" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="151"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="157"/>
+      <c r="K6" s="163"/>
+    </row>
+    <row r="7" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B7" s="166" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="150"/>
+      <c r="D7" s="156" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="147" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="163"/>
+    </row>
+    <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B8" s="166" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="150"/>
+      <c r="D8" s="156" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="163"/>
+    </row>
+    <row r="9" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B9" s="167"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="148"/>
+      <c r="J9" s="148"/>
+      <c r="K9" s="170"/>
+    </row>
+    <row r="10" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="149"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="149"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="149"/>
+    </row>
+    <row r="11" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="152" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="152"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="152"/>
+      <c r="G11" s="152"/>
+      <c r="H11" s="152"/>
+      <c r="I11" s="152"/>
+      <c r="J11" s="152"/>
+      <c r="K11" s="152"/>
+    </row>
+    <row r="12" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="155" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="155" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="155" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="155" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="155" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="155" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="155" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="155" t="s">
+        <v>144</v>
+      </c>
+      <c r="J12" s="155" t="s">
+        <v>145</v>
+      </c>
+      <c r="K12" s="155" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="153"/>
+      <c r="C13" s="153"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="153"/>
+      <c r="F13" s="153"/>
+      <c r="G13" s="153"/>
+      <c r="H13" s="153"/>
+      <c r="I13" s="153"/>
+      <c r="J13" s="153"/>
+      <c r="K13" s="153"/>
+    </row>
+    <row r="14" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B14" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="54">
+        <v>400</v>
+      </c>
+      <c r="D14" s="171">
         <v>127</v>
       </c>
-      <c r="F10" s="146">
-        <f>'Capacidade de Corrente'!K5</f>
-        <v>9.4488188976377945</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B11" s="53">
-        <v>2</v>
-      </c>
-      <c r="C11" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="54">
-        <f>'Capacidade de Corrente'!I6</f>
-        <v>1700</v>
-      </c>
-      <c r="E11" s="54">
-        <f>'Capacidade de Corrente'!J6</f>
+      <c r="E14" s="158">
+        <f>C14/D14</f>
+        <v>3.1496062992125986</v>
+      </c>
+      <c r="F14" s="158">
+        <v>14.629899999999999</v>
+      </c>
+      <c r="G14" s="158">
+        <f>F14/1000</f>
+        <v>1.46299E-2</v>
+      </c>
+      <c r="H14" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I14" s="158">
+        <f>H14*E14*G14*100/D14</f>
+        <v>0.51883581127162259</v>
+      </c>
+      <c r="J14" s="158">
+        <f>I14</f>
+        <v>0.51883581127162259</v>
+      </c>
+      <c r="K14" s="176">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B15" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="54">
+        <v>300</v>
+      </c>
+      <c r="D15" s="171">
         <v>127</v>
       </c>
-      <c r="F11" s="146">
-        <f>'Capacidade de Corrente'!K6</f>
-        <v>13.385826771653543</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B12" s="53">
-        <v>3</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="54">
-        <f>'Capacidade de Corrente'!I7</f>
-        <v>2100</v>
-      </c>
-      <c r="E12" s="54">
-        <f>'Capacidade de Corrente'!J7</f>
+      <c r="E15" s="158">
+        <f t="shared" ref="E15:E17" si="0">C15/D15</f>
+        <v>2.3622047244094486</v>
+      </c>
+      <c r="F15" s="158">
+        <v>4.0477999999999996</v>
+      </c>
+      <c r="G15" s="158">
+        <f t="shared" ref="G15:G25" si="1">F15/1000</f>
+        <v>4.0477999999999998E-3</v>
+      </c>
+      <c r="H15" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I15" s="158">
+        <f t="shared" ref="I15:I25" si="2">H15*E15*G15*100/D15</f>
+        <v>0.10766359972719945</v>
+      </c>
+      <c r="J15" s="158">
+        <f>I14+I15</f>
+        <v>0.626499410998822</v>
+      </c>
+      <c r="K15" s="177"/>
+    </row>
+    <row r="16" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B16" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="54">
+        <v>200</v>
+      </c>
+      <c r="D16" s="171">
         <v>127</v>
       </c>
-      <c r="F12" s="146">
-        <f>'Capacidade de Corrente'!K7</f>
-        <v>16.535433070866141</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B13" s="53">
-        <v>4</v>
-      </c>
-      <c r="C13" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="54">
-        <f>'Capacidade de Corrente'!I8</f>
-        <v>1900</v>
-      </c>
-      <c r="E13" s="54">
-        <f>'Capacidade de Corrente'!J8</f>
+      <c r="E16" s="158">
+        <f t="shared" si="0"/>
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="F16" s="158">
+        <v>4.4528999999999996</v>
+      </c>
+      <c r="G16" s="158">
+        <f t="shared" si="1"/>
+        <v>4.4528999999999992E-3</v>
+      </c>
+      <c r="H16" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I16" s="158">
+        <f t="shared" si="2"/>
+        <v>7.8958980717961438E-2</v>
+      </c>
+      <c r="J16" s="158">
+        <f>SUM(I14:I16)</f>
+        <v>0.70545839171678348</v>
+      </c>
+      <c r="K16" s="177"/>
+    </row>
+    <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B17" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="54">
+        <v>100</v>
+      </c>
+      <c r="D17" s="171">
         <v>127</v>
       </c>
-      <c r="F13" s="146">
-        <f>'Capacidade de Corrente'!K8</f>
-        <v>14.960629921259843</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="53">
-        <v>5</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="54">
-        <f>'Capacidade de Corrente'!I9</f>
-        <v>1900</v>
-      </c>
-      <c r="E14" s="54">
-        <f>'Capacidade de Corrente'!J9</f>
+      <c r="E17" s="158">
+        <f t="shared" si="0"/>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F17" s="158">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="G17" s="158">
+        <f t="shared" si="1"/>
+        <v>4.1229999999999999E-3</v>
+      </c>
+      <c r="H17" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I17" s="158">
+        <f t="shared" si="2"/>
+        <v>3.6554591109182216E-2</v>
+      </c>
+      <c r="J17" s="158">
+        <f>SUM(I14:I17)</f>
+        <v>0.74201298282596573</v>
+      </c>
+      <c r="K17" s="178"/>
+    </row>
+    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B18" s="172"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="173"/>
+      <c r="E18" s="173"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="173"/>
+      <c r="H18" s="173"/>
+      <c r="I18" s="173"/>
+      <c r="J18" s="173"/>
+      <c r="K18" s="174"/>
+    </row>
+    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B19" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="54">
+        <v>200</v>
+      </c>
+      <c r="D19" s="171">
         <v>127</v>
       </c>
-      <c r="F14" s="146">
-        <f>'Capacidade de Corrente'!K9</f>
-        <v>14.960629921259843</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B15" s="53">
-        <v>6</v>
-      </c>
-      <c r="C15" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="54">
-        <f>'Capacidade de Corrente'!I10</f>
-        <v>2500</v>
-      </c>
-      <c r="E15" s="54">
-        <f>'Capacidade de Corrente'!J10</f>
+      <c r="E19" s="158">
+        <f>C19/D19</f>
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="F19" s="158">
+        <v>9.98</v>
+      </c>
+      <c r="G19" s="158">
+        <f t="shared" si="1"/>
+        <v>9.980000000000001E-3</v>
+      </c>
+      <c r="H19" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I19" s="158">
+        <f t="shared" si="2"/>
+        <v>0.1769657139314279</v>
+      </c>
+      <c r="J19" s="158">
+        <f>I19</f>
+        <v>0.1769657139314279</v>
+      </c>
+      <c r="K19" s="176">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B20" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="54">
+        <v>100</v>
+      </c>
+      <c r="D20" s="171">
         <v>127</v>
       </c>
-      <c r="F15" s="146">
-        <f>'Capacidade de Corrente'!K10</f>
-        <v>19.685039370078741</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B16" s="53">
-        <v>7</v>
-      </c>
-      <c r="C16" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="54">
-        <f>'Capacidade de Corrente'!I11</f>
-        <v>2000</v>
-      </c>
-      <c r="E16" s="54">
-        <f>'Capacidade de Corrente'!J11</f>
+      <c r="E20" s="158">
+        <f>C20/D20</f>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F20" s="158">
+        <v>3.3422999999999998</v>
+      </c>
+      <c r="G20" s="158">
+        <f t="shared" si="1"/>
+        <v>3.3422999999999999E-3</v>
+      </c>
+      <c r="H20" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I20" s="158">
+        <f t="shared" si="2"/>
+        <v>2.9632891065782135E-2</v>
+      </c>
+      <c r="J20" s="158">
+        <f>I19+I20</f>
+        <v>0.20659860499721003</v>
+      </c>
+      <c r="K20" s="178"/>
+    </row>
+    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B21" s="172"/>
+      <c r="C21" s="173"/>
+      <c r="D21" s="173"/>
+      <c r="E21" s="173"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173"/>
+      <c r="J21" s="173"/>
+      <c r="K21" s="174"/>
+    </row>
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B22" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="54">
+        <v>600</v>
+      </c>
+      <c r="D22" s="171">
         <v>127</v>
       </c>
-      <c r="F16" s="146">
-        <f>'Capacidade de Corrente'!K11</f>
-        <v>15.748031496062993</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B17" s="53">
-        <v>8</v>
-      </c>
-      <c r="C17" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="54">
-        <f>'Capacidade de Corrente'!I12</f>
-        <v>2000</v>
-      </c>
-      <c r="E17" s="54">
-        <f>'Capacidade de Corrente'!J12</f>
+      <c r="E22" s="158">
+        <f t="shared" ref="E22:E25" si="3">C22/D22</f>
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="F22" s="158">
+        <v>8.1341999999999999</v>
+      </c>
+      <c r="G22" s="158">
+        <f t="shared" si="1"/>
+        <v>8.1341999999999994E-3</v>
+      </c>
+      <c r="H22" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I22" s="158">
+        <f t="shared" si="2"/>
+        <v>0.43270776861553717</v>
+      </c>
+      <c r="J22" s="158">
+        <f>I22</f>
+        <v>0.43270776861553717</v>
+      </c>
+      <c r="K22" s="176">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B23" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="54">
+        <v>100</v>
+      </c>
+      <c r="D23" s="171">
         <v>127</v>
       </c>
-      <c r="F17" s="146">
-        <f>'Capacidade de Corrente'!K12</f>
-        <v>15.748031496062993</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B18" s="53">
-        <v>9</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="54">
-        <f>'Capacidade de Corrente'!I13</f>
-        <v>2000</v>
-      </c>
-      <c r="E18" s="54">
-        <f>'Capacidade de Corrente'!J13</f>
+      <c r="E23" s="158">
+        <f t="shared" si="3"/>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F23" s="158">
+        <v>4.5681000000000003</v>
+      </c>
+      <c r="G23" s="158">
+        <f t="shared" si="1"/>
+        <v>4.5681000000000003E-3</v>
+      </c>
+      <c r="H23" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I23" s="158">
+        <f t="shared" si="2"/>
+        <v>4.0500855601711211E-2</v>
+      </c>
+      <c r="J23" s="158">
+        <f>I22+I23</f>
+        <v>0.47320862421724841</v>
+      </c>
+      <c r="K23" s="177"/>
+    </row>
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B24" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="54">
+        <v>400</v>
+      </c>
+      <c r="D24" s="171">
         <v>127</v>
       </c>
-      <c r="F18" s="146">
-        <f>'Capacidade de Corrente'!K13</f>
-        <v>15.748031496062993</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B19" s="53">
-        <v>10</v>
-      </c>
-      <c r="C19" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="54">
-        <f>'Capacidade de Corrente'!I14</f>
-        <v>5400</v>
-      </c>
-      <c r="E19" s="54">
-        <f>'Capacidade de Corrente'!J14</f>
-        <v>220</v>
-      </c>
-      <c r="F19" s="146">
-        <f>'Capacidade de Corrente'!K14</f>
-        <v>24.545454545454547</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B20" s="53">
-        <v>11</v>
-      </c>
-      <c r="C20" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="54">
-        <f>'Capacidade de Corrente'!I15</f>
-        <v>5400</v>
-      </c>
-      <c r="E20" s="54">
-        <f>'Capacidade de Corrente'!J15</f>
-        <v>220</v>
-      </c>
-      <c r="F20" s="146">
-        <f>'Capacidade de Corrente'!K15</f>
-        <v>24.545454545454547</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B21" s="53">
-        <v>12</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="54">
-        <f>'Capacidade de Corrente'!I16</f>
-        <v>2625</v>
-      </c>
-      <c r="E21" s="54">
-        <f>'Capacidade de Corrente'!J16</f>
-        <v>220</v>
-      </c>
-      <c r="F21" s="146">
-        <f>'Capacidade de Corrente'!K16</f>
-        <v>11.931818181818182</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B22" s="53">
-        <v>13</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="54">
-        <f>'Capacidade de Corrente'!I17</f>
-        <v>1650</v>
-      </c>
-      <c r="E22" s="54">
-        <f>'Capacidade de Corrente'!J17</f>
-        <v>220</v>
-      </c>
-      <c r="F22" s="146">
-        <f>'Capacidade de Corrente'!K17</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B23" s="53">
-        <v>14</v>
-      </c>
-      <c r="C23" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="54">
-        <f>'Capacidade de Corrente'!I18</f>
-        <v>1650</v>
-      </c>
-      <c r="E23" s="54">
-        <f>'Capacidade de Corrente'!J18</f>
-        <v>220</v>
-      </c>
-      <c r="F23" s="146">
-        <f>'Capacidade de Corrente'!K18</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B24" s="53">
-        <v>15</v>
-      </c>
-      <c r="C24" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="54">
-        <f>'Capacidade de Corrente'!I19</f>
+      <c r="E24" s="158">
+        <f t="shared" si="3"/>
+        <v>3.1496062992125986</v>
+      </c>
+      <c r="F24" s="158">
+        <v>4.7576999999999998</v>
+      </c>
+      <c r="G24" s="158">
+        <f t="shared" si="1"/>
+        <v>4.7577000000000001E-3</v>
+      </c>
+      <c r="H24" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I24" s="158">
+        <f t="shared" si="2"/>
+        <v>0.16872741025482052</v>
+      </c>
+      <c r="J24" s="158">
+        <f>I22+I23+I24</f>
+        <v>0.64193603447206893</v>
+      </c>
+      <c r="K24" s="177"/>
+    </row>
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B25" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="54">
+        <v>200</v>
+      </c>
+      <c r="D25" s="171">
+        <v>127</v>
+      </c>
+      <c r="E25" s="158">
+        <f t="shared" si="3"/>
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="F25" s="158">
+        <v>11.351800000000001</v>
+      </c>
+      <c r="G25" s="158">
+        <f t="shared" si="1"/>
+        <v>1.13518E-2</v>
+      </c>
+      <c r="H25" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I25" s="158">
+        <f t="shared" si="2"/>
+        <v>0.20129052018104041</v>
+      </c>
+      <c r="J25" s="158">
+        <f>I22+I23+I24+I25</f>
+        <v>0.84322655465310936</v>
+      </c>
+      <c r="K25" s="178"/>
+    </row>
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B28" s="152" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="152"/>
+      <c r="D28" s="152"/>
+      <c r="E28" s="152"/>
+      <c r="F28" s="152"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="152"/>
+      <c r="I28" s="152"/>
+      <c r="J28" s="152"/>
+      <c r="K28" s="152"/>
+    </row>
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B29" s="155" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="155" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="155" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="155" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="155" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="155" t="s">
+        <v>143</v>
+      </c>
+      <c r="H29" s="155" t="s">
+        <v>164</v>
+      </c>
+      <c r="I29" s="155" t="s">
+        <v>144</v>
+      </c>
+      <c r="J29" s="155" t="s">
+        <v>145</v>
+      </c>
+      <c r="K29" s="155" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B30" s="153"/>
+      <c r="C30" s="153"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="153"/>
+      <c r="F30" s="153"/>
+      <c r="G30" s="153"/>
+      <c r="H30" s="153"/>
+      <c r="I30" s="153"/>
+      <c r="J30" s="153"/>
+      <c r="K30" s="153"/>
+    </row>
+    <row r="31" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B31" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="54">
+        <v>600</v>
+      </c>
+      <c r="D31" s="171">
+        <v>127</v>
+      </c>
+      <c r="E31" s="158">
+        <f>C31/D31</f>
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="F31" s="158">
+        <v>1.7907</v>
+      </c>
+      <c r="G31" s="158">
+        <f>F31/1000</f>
+        <v>1.7906999999999999E-3</v>
+      </c>
+      <c r="H31" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I31" s="158">
+        <f>H31*E31*G31*100/D31</f>
+        <v>9.5258267716535422E-2</v>
+      </c>
+      <c r="J31" s="158">
+        <f>I31</f>
+        <v>9.5258267716535422E-2</v>
+      </c>
+      <c r="K31" s="176">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B32" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="54">
         <v>400</v>
       </c>
-      <c r="E24" s="54">
-        <f>'Capacidade de Corrente'!J19</f>
+      <c r="D32" s="171">
         <v>127</v>
       </c>
-      <c r="F24" s="146">
-        <f>'Capacidade de Corrente'!K19</f>
+      <c r="E32" s="158">
+        <f t="shared" ref="E32:E34" si="4">C32/D32</f>
         <v>3.1496062992125986</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B25" s="53">
-        <v>16</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="54">
-        <f>'Capacidade de Corrente'!I20</f>
-        <v>1760</v>
-      </c>
-      <c r="E25" s="54">
-        <f>'Capacidade de Corrente'!J20</f>
-        <v>220</v>
-      </c>
-      <c r="F25" s="146">
-        <f>'Capacidade de Corrente'!K20</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B26" s="53">
-        <v>17</v>
-      </c>
-      <c r="C26" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="54">
-        <f>'Capacidade de Corrente'!I21</f>
+      <c r="F32" s="158">
+        <v>3.5156999999999998</v>
+      </c>
+      <c r="G32" s="158">
+        <f t="shared" ref="G32:G47" si="5">F32/1000</f>
+        <v>3.5156999999999996E-3</v>
+      </c>
+      <c r="H32" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I32" s="158">
+        <f t="shared" ref="I32:I34" si="6">H32*E32*G32*100/D32</f>
+        <v>0.12468103416206831</v>
+      </c>
+      <c r="J32" s="158">
+        <f>I32+I31</f>
+        <v>0.21993930187860372</v>
+      </c>
+      <c r="K32" s="177"/>
+    </row>
+    <row r="33" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B33" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="54">
+        <v>200</v>
+      </c>
+      <c r="D33" s="171">
+        <v>127</v>
+      </c>
+      <c r="E33" s="158">
+        <f t="shared" si="4"/>
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="F33" s="158">
+        <v>3.3047</v>
+      </c>
+      <c r="G33" s="158">
+        <f t="shared" si="5"/>
+        <v>3.3046999999999998E-3</v>
+      </c>
+      <c r="H33" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I33" s="158">
+        <f t="shared" si="6"/>
+        <v>5.8599057598115199E-2</v>
+      </c>
+      <c r="J33" s="158">
+        <f>I31+I32+I33</f>
+        <v>0.2785383594767189</v>
+      </c>
+      <c r="K33" s="177"/>
+    </row>
+    <row r="34" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B34" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" s="54">
+        <v>100</v>
+      </c>
+      <c r="D34" s="171">
+        <v>127</v>
+      </c>
+      <c r="E34" s="158">
+        <f t="shared" si="4"/>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F34" s="158">
+        <v>2.2797000000000001</v>
+      </c>
+      <c r="G34" s="158">
+        <f t="shared" si="5"/>
+        <v>2.2797E-3</v>
+      </c>
+      <c r="H34" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I34" s="158">
+        <f t="shared" si="6"/>
+        <v>2.0211860623721253E-2</v>
+      </c>
+      <c r="J34" s="158">
+        <f>I31+I32+I33+I34</f>
+        <v>0.29875022010044017</v>
+      </c>
+      <c r="K34" s="178"/>
+    </row>
+    <row r="35" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B35" s="172"/>
+      <c r="C35" s="173"/>
+      <c r="D35" s="173"/>
+      <c r="E35" s="173"/>
+      <c r="F35" s="173"/>
+      <c r="G35" s="173"/>
+      <c r="H35" s="173"/>
+      <c r="I35" s="173"/>
+      <c r="J35" s="173"/>
+      <c r="K35" s="174"/>
+    </row>
+    <row r="36" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B36" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="54">
+        <v>600</v>
+      </c>
+      <c r="D36" s="171">
+        <v>127</v>
+      </c>
+      <c r="E36" s="158">
+        <f>C36/D36</f>
+        <v>4.7244094488188972</v>
+      </c>
+      <c r="F36" s="158">
+        <v>2.3816999999999999</v>
+      </c>
+      <c r="G36" s="158">
+        <f t="shared" si="5"/>
+        <v>2.3817E-3</v>
+      </c>
+      <c r="H36" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I36" s="158">
+        <f t="shared" ref="I36:I37" si="7">H36*E36*G36*100/D36</f>
+        <v>0.12669716659433319</v>
+      </c>
+      <c r="J36" s="158">
+        <f>I36</f>
+        <v>0.12669716659433319</v>
+      </c>
+      <c r="K36" s="176">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B37" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="54">
+        <v>500</v>
+      </c>
+      <c r="D37" s="171">
+        <v>127</v>
+      </c>
+      <c r="E37" s="158">
+        <f>C37/D37</f>
+        <v>3.9370078740157481</v>
+      </c>
+      <c r="F37" s="158">
+        <v>2.3018999999999998</v>
+      </c>
+      <c r="G37" s="158">
+        <f t="shared" si="5"/>
+        <v>2.3019E-3</v>
+      </c>
+      <c r="H37" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I37" s="158">
+        <f t="shared" si="7"/>
+        <v>0.10204343108686219</v>
+      </c>
+      <c r="J37" s="158">
+        <f>I36+I37</f>
+        <v>0.22874059768119537</v>
+      </c>
+      <c r="K37" s="177"/>
+    </row>
+    <row r="38" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B38" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="54">
+        <v>400</v>
+      </c>
+      <c r="D38" s="171">
+        <v>127</v>
+      </c>
+      <c r="E38" s="158">
+        <f t="shared" ref="E38:E41" si="8">C38/D38</f>
+        <v>3.1496062992125986</v>
+      </c>
+      <c r="F38" s="158">
+        <v>2.0811999999999999</v>
+      </c>
+      <c r="G38" s="158">
+        <f t="shared" si="5"/>
+        <v>2.0812000000000001E-3</v>
+      </c>
+      <c r="H38" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I38" s="158">
+        <f t="shared" ref="I38:I46" si="9">H38*E38*G38*100/D38</f>
+        <v>7.3807824415648843E-2</v>
+      </c>
+      <c r="J38" s="158">
+        <f>SUM(I36:I38)</f>
+        <v>0.30254842209684418</v>
+      </c>
+      <c r="K38" s="177"/>
+    </row>
+    <row r="39" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B39" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="54">
         <v>300</v>
       </c>
-      <c r="E26" s="54">
-        <f>'Capacidade de Corrente'!J21</f>
-        <v>220</v>
-      </c>
-      <c r="F26" s="146">
-        <f>'Capacidade de Corrente'!K21</f>
-        <v>1.3636363636363635</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B27" s="53">
-        <v>18</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="54">
-        <f>'Capacidade de Corrente'!I22</f>
-        <v>600</v>
-      </c>
-      <c r="E27" s="54">
-        <f>'Capacidade de Corrente'!J22</f>
+      <c r="D39" s="171">
         <v>127</v>
       </c>
-      <c r="F27" s="146">
-        <f>'Capacidade de Corrente'!K22</f>
-        <v>4.7244094488188972</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B28" s="53">
-        <v>19</v>
-      </c>
-      <c r="C28" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="54">
-        <f>'Capacidade de Corrente'!I23</f>
-        <v>600</v>
-      </c>
-      <c r="E28" s="54">
-        <f>'Capacidade de Corrente'!J23</f>
+      <c r="E39" s="158">
+        <f t="shared" si="8"/>
+        <v>2.3622047244094486</v>
+      </c>
+      <c r="F39" s="158">
+        <v>1.9261999999999999</v>
+      </c>
+      <c r="G39" s="158">
+        <f t="shared" si="5"/>
+        <v>1.9261999999999999E-3</v>
+      </c>
+      <c r="H39" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I39" s="158">
+        <f t="shared" si="9"/>
+        <v>5.1233170066340129E-2</v>
+      </c>
+      <c r="J39" s="158">
+        <f>SUM(I36:I39)</f>
+        <v>0.35378159216318433</v>
+      </c>
+      <c r="K39" s="177"/>
+    </row>
+    <row r="40" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B40" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="54">
+        <v>100</v>
+      </c>
+      <c r="D40" s="171">
         <v>127</v>
       </c>
-      <c r="F28" s="146">
-        <f>'Capacidade de Corrente'!K23</f>
-        <v>4.7244094488188972</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B29" s="53">
-        <v>20</v>
-      </c>
-      <c r="C29" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="54">
-        <f>'Capacidade de Corrente'!I24</f>
-        <v>600</v>
-      </c>
-      <c r="E29" s="54">
-        <f>'Capacidade de Corrente'!J24</f>
+      <c r="E40" s="158">
+        <f t="shared" si="8"/>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F40" s="158">
+        <v>2.5341</v>
+      </c>
+      <c r="G40" s="158">
+        <f t="shared" si="5"/>
+        <v>2.5341000000000001E-3</v>
+      </c>
+      <c r="H40" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I40" s="158">
+        <f t="shared" si="9"/>
+        <v>2.2467375534751075E-2</v>
+      </c>
+      <c r="J40" s="158">
+        <f>SUM(I36:I40)</f>
+        <v>0.37624896769793542</v>
+      </c>
+      <c r="K40" s="177"/>
+    </row>
+    <row r="41" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B41" s="54" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="54">
+        <v>100</v>
+      </c>
+      <c r="D41" s="171">
         <v>127</v>
       </c>
-      <c r="F29" s="146">
-        <f>'Capacidade de Corrente'!K24</f>
-        <v>4.7244094488188972</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B30" s="53">
-        <v>21</v>
-      </c>
-      <c r="C30" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="54">
-        <f>'Capacidade de Corrente'!I25</f>
-        <v>600</v>
-      </c>
-      <c r="E30" s="54">
-        <f>'Capacidade de Corrente'!J25</f>
+      <c r="E41" s="158">
+        <f t="shared" si="8"/>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F41" s="158">
+        <v>3.4512999999999998</v>
+      </c>
+      <c r="G41" s="158">
+        <f t="shared" si="5"/>
+        <v>3.4513E-3</v>
+      </c>
+      <c r="H41" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I41" s="158">
+        <f t="shared" si="9"/>
+        <v>3.0599286998574001E-2</v>
+      </c>
+      <c r="J41" s="158">
+        <f>SUM(I36:I41)</f>
+        <v>0.40684825469650943</v>
+      </c>
+      <c r="K41" s="178"/>
+    </row>
+    <row r="42" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B42" s="172"/>
+      <c r="C42" s="173"/>
+      <c r="D42" s="173"/>
+      <c r="E42" s="173"/>
+      <c r="F42" s="173"/>
+      <c r="G42" s="173"/>
+      <c r="H42" s="173"/>
+      <c r="I42" s="173"/>
+      <c r="J42" s="173"/>
+      <c r="K42" s="174"/>
+    </row>
+    <row r="43" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B43" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="54">
+        <v>500</v>
+      </c>
+      <c r="D43" s="171">
         <v>127</v>
       </c>
-      <c r="F30" s="146">
-        <f>'Capacidade de Corrente'!K25</f>
-        <v>4.7244094488188972</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B31" s="65">
-        <v>22</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="54">
-        <f>'Capacidade de Corrente'!I26</f>
-        <v>38885</v>
-      </c>
-      <c r="E31" s="54"/>
-      <c r="F31" s="146"/>
+      <c r="E43" s="158">
+        <f>C43/D43</f>
+        <v>3.9370078740157481</v>
+      </c>
+      <c r="F43" s="158">
+        <v>1.8081</v>
+      </c>
+      <c r="G43" s="158">
+        <f t="shared" si="5"/>
+        <v>1.8081E-3</v>
+      </c>
+      <c r="H43" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I43" s="158">
+        <f t="shared" si="9"/>
+        <v>8.015323330646662E-2</v>
+      </c>
+      <c r="J43" s="158">
+        <f>I43</f>
+        <v>8.015323330646662E-2</v>
+      </c>
+      <c r="K43" s="175">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B44" s="54" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="54">
+        <v>100</v>
+      </c>
+      <c r="D44" s="171">
+        <v>127</v>
+      </c>
+      <c r="E44" s="158">
+        <f>C44/D44</f>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F44" s="158">
+        <v>1.9812000000000001</v>
+      </c>
+      <c r="G44" s="158">
+        <f t="shared" si="5"/>
+        <v>1.9812000000000002E-3</v>
+      </c>
+      <c r="H44" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I44" s="158">
+        <f t="shared" si="9"/>
+        <v>1.7565354330708664E-2</v>
+      </c>
+      <c r="J44" s="158">
+        <f>SUM(I43:I44)</f>
+        <v>9.771858763717528E-2</v>
+      </c>
+      <c r="K44" s="175"/>
+    </row>
+    <row r="45" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B45" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="54">
+        <v>300</v>
+      </c>
+      <c r="D45" s="171">
+        <v>127</v>
+      </c>
+      <c r="E45" s="158">
+        <f t="shared" ref="E45:E47" si="10">C45/D45</f>
+        <v>2.3622047244094486</v>
+      </c>
+      <c r="F45" s="158">
+        <v>1.5363</v>
+      </c>
+      <c r="G45" s="158">
+        <f t="shared" si="5"/>
+        <v>1.5363E-3</v>
+      </c>
+      <c r="H45" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I45" s="158">
+        <f t="shared" ref="I45:I47" si="11">H45*E45*G45*100/D45</f>
+        <v>4.0862589125178254E-2</v>
+      </c>
+      <c r="J45" s="158">
+        <f>SUM(I43:I45)</f>
+        <v>0.13858117676235354</v>
+      </c>
+      <c r="K45" s="175"/>
+    </row>
+    <row r="46" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B46" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="54">
+        <v>200</v>
+      </c>
+      <c r="D46" s="171">
+        <v>127</v>
+      </c>
+      <c r="E46" s="158">
+        <f t="shared" si="10"/>
+        <v>1.5748031496062993</v>
+      </c>
+      <c r="F46" s="158">
+        <v>1.2608999999999999</v>
+      </c>
+      <c r="G46" s="158">
+        <f t="shared" si="5"/>
+        <v>1.2608999999999999E-3</v>
+      </c>
+      <c r="H46" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I46" s="158">
+        <f t="shared" si="9"/>
+        <v>2.2358323516647034E-2</v>
+      </c>
+      <c r="J46" s="158">
+        <f>SUM(I43:I46)</f>
+        <v>0.16093950027900059</v>
+      </c>
+      <c r="K46" s="175"/>
+    </row>
+    <row r="47" spans="2:11" ht="20.100000000000001" customHeight="1">
+      <c r="B47" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="54">
+        <v>100</v>
+      </c>
+      <c r="D47" s="171">
+        <v>127</v>
+      </c>
+      <c r="E47" s="158">
+        <f t="shared" si="10"/>
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="F47" s="158">
+        <v>1.5118</v>
+      </c>
+      <c r="G47" s="158">
+        <f t="shared" si="5"/>
+        <v>1.5118E-3</v>
+      </c>
+      <c r="H47" s="54">
+        <v>14.3</v>
+      </c>
+      <c r="I47" s="158">
+        <f t="shared" si="11"/>
+        <v>1.3403645607291216E-2</v>
+      </c>
+      <c r="J47" s="158">
+        <f>SUM(I43:I47)</f>
+        <v>0.17434314588629179</v>
+      </c>
+      <c r="K47" s="175"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
+  <mergeCells count="42">
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="K36:K41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="K43:K47"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K22:K25"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G7:J9"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="B10:H10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>